<commit_message>
feat: support all previous weeks
</commit_message>
<xml_diff>
--- a/docs/weekly_nerf_meta_data.xlsx
+++ b/docs/weekly_nerf_meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelinzhao/cache/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8195D18-03C0-7C48-875F-E85D0FEF4FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C60FB59-60DA-B44B-8FE0-6B92E0534BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="625">
   <si>
     <t>week</t>
   </si>
@@ -175,9 +175,6 @@
     <t>Deforming Radiance Fields with Cages</t>
   </si>
   <si>
-    <t>ECCV2022 (Oral)</t>
-  </si>
-  <si>
     <t>NeuMesh: Learning Disentangled Neural Mesh-based Implicit Field for Geometry and Texture Editing</t>
   </si>
   <si>
@@ -497,6 +494,1419 @@
   </si>
   <si>
     <t>pose-slam</t>
+  </si>
+  <si>
+    <t>Previous weeks</t>
+  </si>
+  <si>
+    <t>NeRF: Representing Scenes as Neural Radiance Fields for View Synthesis</t>
+  </si>
+  <si>
+    <t>Neural Sparse Voxel Fields</t>
+  </si>
+  <si>
+    <t>ECCV2020</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2003.08934</t>
+  </si>
+  <si>
+    <t>http://tancik.com/nerf</t>
+  </si>
+  <si>
+    <t>NeRF：将场景表示为用于视图合成的神经辐射场</t>
+  </si>
+  <si>
+    <t>我们提出了一种方法，该方法通过使用稀疏输入视图集优化底层连续体积场景函数，实现了合成复杂场景的新视图的最新结果。我们的算法使用全连接（非卷积）深度网络表示场景，其输入是单个连续 5D 坐标（空间位置（x,y,z）和观察方向（θ,φ）），其输出是该空间位置的体积密度和与视图相关的发射辐射。我们通过沿相机光线查询 5D 坐标来合成视图，并使用经典的体渲染技术将输出颜色和密度投影到图像中。因为体积渲染是自然可微的，所以优化我们的表示所需的唯一输入是一组具有已知相机姿势的图像。我们描述了如何有效地优化神经辐射场以渲染具有复杂几何形状和外观的场景的逼真的新颖视图，并展示了优于先前在神经渲染和视图合成方面的工作的结果。查看合成结果最好以视频形式观看，因此我们敦促读者观看我们的补充视频以进行令人信服的比较。</t>
+  </si>
+  <si>
+    <t>We introduce Neural Sparse Voxel Fields (NSVF), a new neural scene representation for fast and high-quality free-viewpoint rendering. NSVF defines a set of voxel-bounded implicit fields organized in a sparse voxel octree to model local properties in each cell. We progressively learn the underlying voxel structures with a diffentiable ray-marching operation from only a set of posed RGB images. With the sparse voxel octree structure, rendering novel views can be accelerated by skipping the voxels containing no relevant scene content. Our method is over 10 times faster than the state-of-the-art (namely, NeRF (Mildenhall et al., 2020)) at inference time while achieving higher quality results. Furthermore, by utilizing an explicit sparse voxel representation, our method can easily be applied to scene editing and scene composition. We also demonstrate several challenging tasks, including multi-scene learning, free-viewpoint rendering of a moving human, and large-scale scene rendering.</t>
+  </si>
+  <si>
+    <t>https://lingjie0206.github.io/papers/NSVF/</t>
+  </si>
+  <si>
+    <t>https://github.com/facebookresearch/NSVF</t>
+  </si>
+  <si>
+    <t>我们介绍了神经稀疏体素场 (NSVF)，这是一种用于快速和高质量自由视点渲染的新神经场景表示。 NSVF 定义了一组以稀疏体素八叉树组织的体素有界隐式字段，以对每个单元中的局部属性进行建模。 我们仅从一组姿势的 RGB 图像中通过可区分的光线行进操作逐步学习底层体素结构。 使用稀疏体素八叉树结构，可以通过跳过不包含相关场景内容的体素来加速渲染新颖的视图。 我们的方法在推理时比最先进的方法（即 NeRF (Mildenhall et al., 2020)）快 10 倍以上，同时获得更高质量的结果。 此外，通过利用显式稀疏体素表示，我们的方法可以很容易地应用于场景编辑和场景合成。 我们还展示了几个具有挑战性的任务，包括多场景学习、移动人体的自由视点渲染和大规模场景渲染。</t>
+  </si>
+  <si>
+    <t>神经稀疏体素场</t>
+  </si>
+  <si>
+    <t>AutoInt: Automatic Integration for Fast Neural Volume Rendering</t>
+  </si>
+  <si>
+    <t>CVPR2021</t>
+  </si>
+  <si>
+    <t>Numerical integration is a foundational technique in scientific computing and is at the core of many computer vision applications. Among these applications, implicit neural volume rendering has recently been proposed as a new paradigm for view synthesis, achieving photorealistic image quality. However, a fundamental obstacle to making these methods practical is the extreme computational and memory requirements caused by the required volume integrations along the rendered rays during training and inference. Millions of rays, each requiring hundreds of forward passes through a neural network are needed to approximate those integrations with Monte Carlo sampling. Here, we propose automatic integration, a new framework for learning efficient, closed-form solutions to integrals using implicit neural representation networks. For training, we instantiate the computational graph corresponding to the derivative of the implicit neural representation. The graph is fitted to the signal to integrate. After optimization, we reassemble the graph to obtain a network that represents the antiderivative. By the fundamental theorem of calculus, this enables the calculation of any definite integral in two evaluations of the network. Using this approach, we demonstrate a greater than 10× improvement in computation requirements, enabling fast neural volume rendering.</t>
+  </si>
+  <si>
+    <t>数值积分是科学计算的基础技术，是许多计算机视觉应用的核心。在这些应用中，隐式神经体绘制最近被提出作为视图合成的新范式，实现逼真的图像质量。然而，使这些方法实用的一个基本障碍是在训练和推理期间沿渲染光线所需的体积积分导致的极端计算和内存要求。需要数百万条光线，每条光线都需要数百次通过神经网络的前向传播，才能通过蒙特卡罗采样来近似这些集成。在这里，我们提出了自动积分，这是一种使用隐式神经表示网络来学习有效的、封闭形式的积分解决方案的新框架。对于训练，我们实例化对应于隐式神经表示的导数的计算图。该图适合要积分的信号。优化后，我们重新组装图以获得代表反导数的网络。根据微积分的基本定理，这可以在网络的两次评估中计算任何定积分。使用这种方法，我们展示了超过 10 倍的计算要求改进，从而实现了快速的神经体绘制。</t>
+  </si>
+  <si>
+    <t>AutoInt：快速神经体积渲染的自动集成</t>
+  </si>
+  <si>
+    <t>http://www.computationalimaging.org/publications/automatic-integration/</t>
+  </si>
+  <si>
+    <t>https://github.com/computational-imaging/automatic-integration</t>
+  </si>
+  <si>
+    <t>DeRF: Decomposed Radiance Fields</t>
+  </si>
+  <si>
+    <t>With the advent of Neural Radiance Fields (NeRF), neural networks can now render novel views of a 3D scene with quality that fools the human eye. Yet, generating these images is very computationally intensive, limiting their applicability in practical scenarios. In this paper, we propose a technique based on spatial decomposition capable of mitigating this issue. Our key observation is that there are diminishing returns in employing larger (deeper and/or wider) networks. Hence, we propose to spatially decompose a scene and dedicate smaller networks for each decomposed part. When working together, these networks can render the whole scene. This allows us near-constant inference time regardless of the number of decomposed parts. Moreover, we show that a Voronoi spatial decomposition is preferable for this purpose, as it is provably compatible with the Painter's Algorithm for efficient and GPU-friendly rendering. Our experiments show that for real-world scenes, our method provides up to 3x more efficient inference than NeRF (with the same rendering quality), or an improvement of up to 1.0~dB in PSNR (for the same inference cost).</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2011.12490</t>
+  </si>
+  <si>
+    <t>DONeRF: Towards Real-Time Rendering of Compact Neural Radiance Fields using Depth Oracle Networks</t>
+  </si>
+  <si>
+    <t>CGF2021</t>
+  </si>
+  <si>
+    <t>The recent research explosion around Neural Radiance Fields (NeRFs) shows that there is immense potential for implicitly storing scene and lighting information in neural networks, e.g., for novel view generation. However, one major limitation preventing the widespread use of NeRFs is the prohibitive computational cost of excessive network evaluations along each view ray, requiring dozens of petaFLOPS when aiming for real-time rendering on current devices. We show that the number of samples required for each view ray can be significantly reduced when local samples are placed around surfaces in the scene. To this end, we propose a depth oracle network, which predicts ray sample locations for each view ray with a single network evaluation. We show that using a classification network around logarithmically discretized and spherically warped depth values is essential to encode surface locations rather than directly estimating depth. The combination of these techniques leads to DONeRF, a dual network design with a depth oracle network as a first step and a locally sampled shading network for ray accumulation. With our design, we reduce the inference costs by up to 48x compared to NeRF. Using an off-the-shelf inference API in combination with simple compute kernels, we are the first to render raymarching-based neural representations at interactive frame rates (15 frames per second at 800x800) on a single GPU. At the same time, since we focus on the important parts of the scene around surfaces, we achieve equal or better quality compared to NeRF.</t>
+  </si>
+  <si>
+    <t>https://depthoraclenerf.github.io/</t>
+  </si>
+  <si>
+    <t>https://github.com/facebookresearch/DONERF</t>
+  </si>
+  <si>
+    <t>FastNeRF: High-Fidelity Neural Rendering at 200FPS</t>
+  </si>
+  <si>
+    <t>Recent work on Neural Radiance Fields (NeRF) showed how neural networks can be used to encode complex 3D environments that can be rendered photorealistically from novel viewpoints. Rendering these images is very computationally demanding and recent improvements are still a long way from enabling interactive rates, even on high-end hardware. Motivated by scenarios on mobile and mixed reality devices, we propose FastNeRF, the first NeRF-based system capable of rendering high fidelity photorealistic images at 200Hz on a high-end consumer GPU. The core of our method is a graphics-inspired factorization that allows for (i) compactly caching a deep radiance map at each position in space, (ii) efficiently querying that map using ray directions to estimate the pixel values in the rendered image. Extensive experiments show that the proposed method is 3000 times faster than the original NeRF algorithm and at least an order of magnitude faster than existing work on accelerating NeRF, while maintaining visual quality and extensibility.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.10380</t>
+  </si>
+  <si>
+    <t>ICCV2021</t>
+  </si>
+  <si>
+    <t>KiloNeRF: Speeding up Neural Radiance Fields with Thousands of Tiny MLPs </t>
+  </si>
+  <si>
+    <t>NeRF synthesizes novel views of a scene with unprecedented quality by fitting a neural radiance field to RGB images. However, NeRF requires querying a deep Multi-Layer Perceptron (MLP) millions of times, leading to slow rendering times, even on modern GPUs. In this paper, we demonstrate that real-time rendering is possible by utilizing thousands of tiny MLPs instead of one single large MLP. In our setting, each individual MLP only needs to represent parts of the scene, thus smaller and faster-to-evaluate MLPs can be used. By combining this divide-and-conquer strategy with further optimizations, rendering is accelerated by three orders of magnitude compared to the original NeRF model without incurring high storage costs. Further, using teacher-student distillation for training, we show that this speed-up can be achieved without sacrificing visual quality.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.13744</t>
+  </si>
+  <si>
+    <t>https://github.com/creiser/kilonerf/</t>
+  </si>
+  <si>
+    <t>PlenOctrees for Real-time Rendering of Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>ICCV2021(oral)</t>
+  </si>
+  <si>
+    <t>Real-time performance is achieved by pre-tabulating the NeRF into an octree-based radiance field that we call PlenOctrees. In order to preserve view-dependent effects such as specularities, we propose to encode appearances via closed-form spherical basis functions. Specifically, we show that it is possible to train NeRFs to predict a spherical harmonic representation of radiance, removing the viewing direction as input to the neural network. Furthermore, we show that our PlenOctrees can be directly optimized to further minimize the reconstruction loss, which leads to equal or better quality than competing methods. We further show that this octree optimization step can be used to accelerate the training time, as we no longer need to wait for the NeRF training to converge fully. Our real-time neural rendering approach may potentially enable new applications such as 6-DOF industrial and product visualizations, as well as next generation AR/VR systems.</t>
+  </si>
+  <si>
+    <t>https://alexyu.net/plenoctrees/</t>
+  </si>
+  <si>
+    <t>https://github.com/sxyu/volrend</t>
+  </si>
+  <si>
+    <t>Mixture of Volumetric Primitives for Efficient Neural Rendering</t>
+  </si>
+  <si>
+    <t>SIGGRAPH2021</t>
+  </si>
+  <si>
+    <t>Real-time rendering and animation of humans is a core function in games, movies, and telepresence applications. Existing methods have a number of drawbacks we aim to address with our work. Triangle meshes have difficulty modeling thin structures like hair, volumetric representations like Neural Volumes are too low-resolution given a reasonable memory budget, and high-resolution implicit representations like Neural Radiance Fields are too slow for use in real-time applications. We present Mixture of Volumetric Primitives (MVP), a representation for rendering dynamic 3D content that combines the completeness of volumetric representations with the efficiency of primitive-based rendering, e.g., point-based or mesh-based methods. Our approach achieves this by leveraging spatially shared computation with a deconvolutional architecture and by minimizing computation in empty regions of space with volumetric primitives that can move to cover only occupied regions. Our parameterization supports the integration of correspondence and tracking constraints, while being robust to areas where classical tracking fails, such as around thin or translucent structures and areas with large topological variability. MVP is a hybrid that generalizes both volumetric and primitive-based representations. Through a series of extensive experiments we demonstrate that it inherits the strengths of each, while avoiding many of their limitations. We also compare our approach to several state-of-the-art methods and demonstrate that MVP produces superior results in terms of quality and runtime performance.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.01954</t>
+  </si>
+  <si>
+    <t>Light Field Networks: Neural Scene Representations with Single-Evaluation Rendering</t>
+  </si>
+  <si>
+    <t>Inferring representations of 3D scenes from 2D observations is a fundamental problem of computer graphics, computer vision, and artificial intelligence. Emerging 3D-structured neural scene representations are a promising approach to 3D scene understanding. In this work, we propose a novel neural scene representation, Light Field Networks or LFNs, which represent both geometry and appearance of the underlying 3D scene in a 360-degree, four-dimensional light field parameterized via a neural implicit representation. Rendering a ray from an LFN requires only a *single* network evaluation, as opposed to hundreds of evaluations per ray for ray-marching or volumetric based renderers in 3D-structured neural scene representations. In the setting of simple scenes, we leverage meta-learning to learn a prior over LFNs that enables multi-view consistent light field reconstruction from as little as a single image observation. This results in dramatic reductions in time and memory complexity, and enables real-time rendering. The cost of storing a 360-degree light field via an LFN is two orders of magnitude lower than conventional methods such as the Lumigraph. Utilizing the analytical differentiability of neural implicit representations and a novel parameterization of light space, we further demonstrate the extraction of sparse depth maps from LFNs.</t>
+  </si>
+  <si>
+    <t>https://www.vincentsitzmann.com/lfns/</t>
+  </si>
+  <si>
+    <t>https://github.com/vsitzmann/light-field-networks</t>
+  </si>
+  <si>
+    <t>Depth-supervised NeRF: Fewer Views and Faster Training for Free</t>
+  </si>
+  <si>
+    <t>https://github.com/dunbar12138/DSNeRF</t>
+  </si>
+  <si>
+    <t>CVPR2022</t>
+  </si>
+  <si>
+    <t>A commonly observed failure mode of Neural Radiance Field (NeRF) is fitting incorrect geometries when given an insufficient number of input views. One potential reason is that standard volumetric rendering does not enforce the constraint that most of a scene's geometry consist of empty space and opaque surfaces. We formalize the above assumption through DS-NeRF (Depth-supervised Neural Radiance Fields), a loss for learning radiance fields that takes advantage of readily-available depth supervision. We leverage the fact that current NeRF pipelines require images with known camera poses that are typically estimated by running structure-from-motion (SFM). Crucially, SFM also produces sparse 3D points that can be used as "free" depth supervision during training: we add a loss to encourage the distribution of a ray's terminating depth matches a given 3D keypoint, incorporating depth uncertainty. DS-NeRF can render better images given fewer training views while training 2-3x faster. Further, we show that our loss is compatible with other recently proposed NeRF methods, demonstrating that depth is a cheap and easily digestible supervisory signal. And finally, we find that DS-NeRF can support other types of depth supervision such as scanned depth sensors and RGB-D reconstruction outputs.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2107.02791</t>
+  </si>
+  <si>
+    <t>Direct Voxel Grid Optimization: Super-fast Convergence for Radiance Fields Reconstruction</t>
+  </si>
+  <si>
+    <t>CVPR2022(oral)</t>
+  </si>
+  <si>
+    <t>We present a super-fast convergence approach to reconstructing the per-scene radiance field from a set of images that capture the scene with known poses. This task, which is often applied to novel view synthesis, is recently revolutionized by Neural Radiance Field (NeRF) for its state-of-the-art quality and flexibility. However, NeRF and its variants require a lengthy training time ranging from hours to days for a single scene. In contrast, our approach achieves NeRF-comparable quality and converges rapidly from scratch in less than 15 minutes with a single GPU. We adopt a representation consisting of a density voxel grid for scene geometry and a feature voxel grid with a shallow network for complex view-dependent appearance. Modeling with explicit and discretized volume representations is not new, but we propose two simple yet non-trivial techniques that contribute to fast convergence speed and high-quality output. First, we introduce the post-activation interpolation on voxel density, which is capable of producing sharp surfaces in lower grid resolution. Second, direct voxel density optimization is prone to suboptimal geometry solutions, so we robustify the optimization process by imposing several priors. Finally, evaluation on five inward-facing benchmarks shows that our method matches, if not surpasses, NeRF's quality, yet it only takes about 15 minutes to train from scratch for a new scene.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2111.11215</t>
+  </si>
+  <si>
+    <t>https://github.com/sunset1995/DirectVoxGO</t>
+  </si>
+  <si>
+    <t>NeRF in the Wild: Neural Radiance Fields for Unconstrained Photo Collections</t>
+  </si>
+  <si>
+    <t>We present a learning-based method for synthesizing novel views of complex scenes using only unstructured collections of in-the-wild photographs. We build on Neural Radiance Fields (NeRF), which uses the weights of a multilayer perceptron to model the density and color of a scene as a function of 3D coordinates. While NeRF works well on images of static subjects captured under controlled settings, it is incapable of modeling many ubiquitous, real-world phenomena in uncontrolled images, such as variable illumination or transient occluders. We introduce a series of extensions to NeRF to address these issues, thereby enabling accurate reconstructions from unstructured image collections taken from the internet. We apply our system, dubbed NeRF-W, to internet photo collections of famous landmarks, and demonstrate temporally consistent novel view renderings that are significantly closer to photorealism than the prior state of the art.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2008.02268</t>
+  </si>
+  <si>
+    <t>Ha-NeRF: Hallucinated Neural Radiance Fields in the Wild</t>
+  </si>
+  <si>
+    <t>Neural Radiance Fields (NeRF) has recently gained popularity for its impressive novel view synthesis ability. This paper studies the problem of hallucinated NeRF: i.e., recovering a realistic NeRF at a different time of day from a group of tourism images. Existing solutions adopt NeRF with a controllable appearance embedding to render novel views under various conditions, but they cannot render view-consistent images with an unseen appearance. To solve this problem, we present an end-to-end framework for constructing a hallucinated NeRF, dubbed as Ha-NeRF. Specifically, we propose an appearance hallucination module to handle time-varying appearances and transfer them to novel views. Considering the complex occlusions of tourism images, we introduce an anti-occlusion module to decompose the static subjects for visibility accurately. Experimental results on synthetic data and real tourism photo collections demonstrate that our method can hallucinate the desired appearances and render occlusion-free images from different views.</t>
+  </si>
+  <si>
+    <t>https://rover-xingyu.github.io/Ha-NeRF/</t>
+  </si>
+  <si>
+    <t>https://github.com/rover-xingyu/Ha-NeRF</t>
+  </si>
+  <si>
+    <t>Nerfies: Deformable Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>We present the first method capable of photorealistically reconstructing deformable scenes using photos/videos captured casually from mobile phones. Our approach augments neural radiance fields (NeRF) by optimizing an additional continuous volumetric deformation field that warps each observed point into a canonical 5D NeRF. We observe that these NeRF-like deformation fields are prone to local minima, and propose a coarse-to-fine optimization method for coordinate-based models that allows for more robust optimization. By adapting principles from geometry processing and physical simulation to NeRF-like models, we propose an elastic regularization of the deformation field that further improves robustness. We show that our method can turn casually captured selfie photos/videos into deformable NeRF models that allow for photorealistic renderings of the subject from arbitrary viewpoints, which we dub "nerfies." We evaluate our method by collecting time-synchronized data using a rig with two mobile phones, yielding train/validation images of the same pose at different viewpoints. We show that our method faithfully reconstructs non-rigidly deforming scenes and reproduces unseen views with high fidelity.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2011.12948</t>
+  </si>
+  <si>
+    <t>D-NeRF: Neural Radiance Fields for Dynamic Scenes</t>
+  </si>
+  <si>
+    <t>Neural rendering techniques combining machine learning with geometric reasoning have arisen as one of the most promising approaches for synthesizing novel views of a scene from a sparse set of images. Among these, stands out the Neural radiance fields (NeRF), which trains a deep network to map 5D input coordinates (representing spatial location and viewing direction) into a volume density and view-dependent emitted radiance. However, despite achieving an unprecedented level of photorealism on the generated images, NeRF is only applicable to static scenes, where the same spatial location can be queried from different images. In this paper we introduce D-NeRF, a method that extends neural radiance fields to a dynamic domain, allowing to reconstruct and render novel images of objects under rigid and non-rigid motions from a \emph{single} camera moving around the scene. For this purpose we consider time as an additional input to the system, and split the learning process in two main stages: one that encodes the scene into a canonical space and another that maps this canonical representation into the deformed scene at a particular time. Both mappings are simultaneously learned using fully-connected networks. Once the networks are trained, D-NeRF can render novel images, controlling both the camera view and the time variable, and thus, the object movement. We demonstrate the effectiveness of our approach on scenes with objects under rigid, articulated and non-rigid motions. Code, model weights and the dynamic scenes dataset will be released.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2011.13961</t>
+  </si>
+  <si>
+    <t>https://github.com/albertpumarola/D-NeRF</t>
+  </si>
+  <si>
+    <t>Dynamic Neural Radiance Fields for Monocular 4D Facial Avatar Reconstruction</t>
+  </si>
+  <si>
+    <t>We present dynamic neural radiance fields for modeling the appearance and dynamics of a human face. Digitally modeling and reconstructing a talking human is a key building-block for a variety of applications. Especially, for telepresence applications in AR or VR, a faithful reproduction of the appearance including novel viewpoint or head-poses is required. In contrast to state-of-the-art approaches that model the geometry and material properties explicitly, or are purely image-based, we introduce an implicit representation of the head based on scene representation networks. To handle the dynamics of the face, we combine our scene representation network with a low-dimensional morphable model which provides explicit control over pose and expressions. We use volumetric rendering to generate images from this hybrid representation and demonstrate that such a dynamic neural scene representation can be learned from monocular input data only, without the need of a specialized capture setup. In our experiments, we show that this learned volumetric representation allows for photo-realistic image generation that surpasses the quality of state-of-the-art video-based reenactment methods.</t>
+  </si>
+  <si>
+    <t>https://gafniguy.github.io/4D-Facial-Avatars/</t>
+  </si>
+  <si>
+    <t>https://github.com/gafniguy/4D-Facial-Avatars</t>
+  </si>
+  <si>
+    <t>Non-Rigid Neural Radiance Fields: Reconstruction and Novel View Synthesis of a Deforming Scene from Monocular Video,</t>
+  </si>
+  <si>
+    <t>We present Non-Rigid Neural Radiance Fields (NR-NeRF), a reconstruction and novel view synthesis approach for general non-rigid dynamic scenes. Our approach takes RGB images of a dynamic scene as input (e.g., from a monocular video recording), and creates a high-quality space-time geometry and appearance representation. We show that a single handheld consumer-grade camera is sufficient to synthesize sophisticated renderings of a dynamic scene from novel virtual camera views, e.g. a `bullet-time' video effect. NR-NeRF disentangles the dynamic scene into a canonical volume and its deformation. Scene deformation is implemented as ray bending, where straight rays are deformed non-rigidly. We also propose a novel rigidity network to better constrain rigid regions of the scene, leading to more stable results. The ray bending and rigidity network are trained without explicit supervision. Our formulation enables dense correspondence estimation across views and time, and compelling video editing applications such as motion exaggeration. Our code will be open sourced.</t>
+  </si>
+  <si>
+    <t>https://vcai.mpi-inf.mpg.de/projects/nonrigid_nerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/facebookresearch/nonrigid_nerf</t>
+  </si>
+  <si>
+    <t>PVA: Pixel-aligned Volumetric Avatars</t>
+  </si>
+  <si>
+    <t>Acquisition and rendering of photorealistic human heads is a highly challenging research problem of particular importance for virtual telepresence. Currently, the highest quality is achieved by volumetric approaches trained in a person-specific manner on multi-view data. These models better represent fine structure, such as hair, compared to simpler mesh-based models. Volumetric models typically employ a global code to represent facial expressions, such that they can be driven by a small set of animation parameters. While such architectures achieve impressive rendering quality, they can not easily be extended to the multi-identity setting. In this paper, we devise a novel approach for predicting volumetric avatars of the human head given just a small number of inputs. We enable generalization across identities by a novel parameterization that combines neural radiance fields with local, pixel-aligned features extracted directly from the inputs, thus side-stepping the need for very deep or complex networks. Our approach is trained in an end-to-end manner solely based on a photometric rerendering loss without requiring explicit 3D supervision.We demonstrate that our approach outperforms the existing state of the art in terms of quality and is able to generate faithful facial expressions in a multi-identity setting.</t>
+  </si>
+  <si>
+    <t>https://volumetric-avatars.github.io/</t>
+  </si>
+  <si>
+    <t>Neural Articulated Radiance Field</t>
+  </si>
+  <si>
+    <t>We present Neural Articulated Radiance Field (NARF), a novel deformable 3D representation for articulated objects learned from images. While recent advances in 3D implicit representation have made it possible to learn models of complex objects, learning pose-controllable representations of articulated objects remains a challenge, as current methods require 3D shape supervision and are unable to render appearance. In formulating an implicit representation of 3D articulated objects, our method considers only the rigid transformation of the most relevant object part in solving for the radiance field at each 3D location. In this way, the proposed method represents pose-dependent changes without significantly increasing the computational complexity. NARF is fully differentiable and can be trained from images with pose annotations. Moreover, through the use of an autoencoder, it can learn appearance variations over multiple instances of an object class. Experiments show that the proposed method is efficient and can generalize well to novel poses.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2104.03110</t>
+  </si>
+  <si>
+    <t>https://github.com/nogu-atsu/NARF#code</t>
+  </si>
+  <si>
+    <t>CLA-NeRF: Category-Level Articulated Neural Radiance Field</t>
+  </si>
+  <si>
+    <t>ICRA2022</t>
+  </si>
+  <si>
+    <t>We propose CLA-NeRF -- a Category-Level Articulated Neural Radiance Field that can perform view synthesis, part segmentation, and articulated pose estimation. CLA-NeRF is trained at the object category level using no CAD models and no depth, but a set of RGB images with ground truth camera poses and part segments. During inference, it only takes a few RGB views (i.e., few-shot) of an unseen 3D object instance within the known category to infer the object part segmentation and the neural radiance field. Given an articulated pose as input, CLA-NeRF can perform articulation-aware volume rendering to generate the corresponding RGB image at any camera pose. Moreover, the articulated pose of an object can be estimated via inverse rendering. In our experiments, we evaluate the framework across five categories on both synthetic and real-world data. In all cases, our method shows realistic deformation results and accurate articulated pose estimation. We believe that both few-shot articulated object rendering and articulated pose estimation open doors for robots to perceive and interact with unseen articulated objects.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2202.00181</t>
+  </si>
+  <si>
+    <t>Animatable Neural Radiance Fields for Human Body Modeling</t>
+  </si>
+  <si>
+    <t>This paper addresses the challenge of reconstructing an animatable human model from a multi-view video. Some recent works have proposed to decompose a non-rigidly deforming scene into a canonical neural radiance field and a set of deformation fields that map observation-space points to the canonical space, thereby enabling them to learn the dynamic scene from images. However, they represent the deformation field as translational vector field or SE(3) field, which makes the optimization highly under-constrained. Moreover, these representations cannot be explicitly controlled by input motions. Instead, we introduce neural blend weight fields to produce the deformation fields. Based on the skeleton-driven deformation, blend weight fields are used with 3D human skeletons to generate observation-to-canonical and canonical-to-observation correspondences. Since 3D human skeletons are more observable, they can regularize the learning of deformation fields. Moreover, the learned blend weight fields can be combined with input skeletal motions to generate new deformation fields to animate the human model. Experiments show that our approach significantly outperforms recent human synthesis methods. The code will be available at https://zju3dv.github.io/animatable_nerf/.</t>
+  </si>
+  <si>
+    <t>https://zju3dv.github.io/animatable_nerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/zju3dv/animatable_nerf</t>
+  </si>
+  <si>
+    <t>Neural Actor: Neural Free-view Synthesis of Human Actors with Pose Control</t>
+  </si>
+  <si>
+    <t>SIGSIGGRAPH Asia 2021</t>
+  </si>
+  <si>
+    <t>We propose Neural Actor (NA), a new method for high-quality synthesis of humans from arbitrary viewpoints and under arbitrary controllable poses. Our method is built upon recent neural scene representation and rendering works which learn representations of geometry and appearance from only 2D images. While existing works demonstrated compelling rendering of static scenes and playback of dynamic scenes, photo-realistic reconstruction and rendering of humans with neural implicit methods, in particular under user-controlled novel poses, is still difficult. To address this problem, we utilize a coarse body model as the proxy to unwarp the surrounding 3D space into a canonical pose. A neural radiance field learns pose-dependent geometric deformations and pose- and view-dependent appearance effects in the canonical space from multi-view video input. To synthesize novel views of high fidelity dynamic geometry and appearance, we leverage 2D texture maps defined on the body model as latent variables for predicting residual deformations and the dynamic appearance. Experiments demonstrate that our method achieves better quality than the state-of-the-arts on playback as well as novel pose synthesis, and can even generalize well to new poses that starkly differ from the training poses. Furthermore, our method also supports body shape control of the synthesized results.</t>
+  </si>
+  <si>
+    <t>https://vcai.mpi-inf.mpg.de/projects/NeuralActor/</t>
+  </si>
+  <si>
+    <t>https://people.mpi-inf.mpg.de/~lliu/projects/NeuralActor/</t>
+  </si>
+  <si>
+    <t>Neural Scene Flow Fields for Space-Time View Synthesis of Dynamic Scenes</t>
+  </si>
+  <si>
+    <t>http://www.cs.cornell.edu/~zl548/NSFF/</t>
+  </si>
+  <si>
+    <t>https://github.com/zhengqili/Neural-Scene-Flow-Fields</t>
+  </si>
+  <si>
+    <t>video</t>
+  </si>
+  <si>
+    <t>We present a method that achieves state-of-the-art results for synthesizing novel views of complex scenes by optimizing an underlying continuous volumetric scene function using a sparse set of input views. Our algorithm represents a scene using a fully-connected (non-convolutional) deep network, whose input is a single continuous 5D coordinate (spatial location (x,y,z) and viewing direction (θ,ϕ)) and whose output is the volume density and view-dependent emitted radiance at that spatial location. We synthesize views by querying 5D coordinates along camera rays and use classic volume rendering techniques to project the output colors and densities into an image. Because volume rendering is naturally differentiable, the only input required to optimize our representation is a set of images with known camera poses. We describe how to effectively optimize neural radiance fields to render photorealistic novel views of scenes with complicated geometry and appearance, and demonstrate results that outperform prior work on neural rendering and view synthesis. View synthesis results are best viewed as videos, so we urge readers to view our supplementary video for convincing comparisons.</t>
+  </si>
+  <si>
+    <t>We present a method to perform novel view and time synthesis of dynamic scenes, requiring only a monocular video with known camera poses as input. To do this, we introduce Neural Scene Flow Fields, a new representation that models the dynamic scene as a time-variant continuous function of appearance, geometry, and 3D scene motion. Our representation is optimized through a neural network to fit the observed input views. We show that our representation can be used for complex dynamic scenes, including thin structures, view-dependent effects, and natural degrees of motion. We conduct a number of experiments that demonstrate our approach significantly outperforms recent monocular view synthesis methods, and show qualitative results of space-time view synthesis on a variety of real-world videos.</t>
+  </si>
+  <si>
+    <t>human</t>
+  </si>
+  <si>
+    <t>Neural Body: Implicit Neural Representations with Structured Latent Codes for Novel View Synthesis of Dynamic Humans</t>
+  </si>
+  <si>
+    <t>This paper addresses the challenge of novel view synthesis for a human performer from a very sparse set of camera views. Some recent works have shown that learning implicit neural representations of 3D scenes achieves remarkable view synthesis quality given dense input views. However, the representation learning will be ill-posed if the views are highly sparse. To solve this ill-posed problem, our key idea is to integrate observations over video frames. To this end, we propose Neural Body, a new human body representation which assumes that the learned neural representations at different frames share the same set of latent codes anchored to a deformable mesh, so that the observations across frames can be naturally integrated. The deformable mesh also provides geometric guidance for the network to learn 3D representations more efficiently. To evaluate our approach, we create a multi-view dataset named ZJU-MoCap that captures performers with complex motions. Experiments on ZJU-MoCap show that our approach outperforms prior works by a large margin in terms of novel view synthesis quality. We also demonstrate the capability of our approach to reconstruct a moving person from a monocular video on the People-Snapshot dataset.</t>
+  </si>
+  <si>
+    <t>https://zju3dv.github.io/neuralbody/</t>
+  </si>
+  <si>
+    <t>https://github.com/zju3dv/neuralbody</t>
+  </si>
+  <si>
+    <t>Neural 3D Video Synthesis from Multi-view Video</t>
+  </si>
+  <si>
+    <t>We propose a novel approach for 3D video synthesis that is able to represent multi-view video recordings of a dynamic real-world scene in a compact, yet expressive representation that enables high-quality view synthesis and motion interpolation. Our approach takes the high quality and compactness of static neural radiance fields in a new direction: to a model-free, dynamic setting. At the core of our approach is a novel time-conditioned neural radiance fields that represents scene dynamics using a set of compact latent codes. To exploit the fact that changes between adjacent frames of a video are typically small and locally consistent, we propose two novel strategies for efficient training of our neural network: 1) An efficient hierarchical training scheme, and 2) an importance sampling strategy that selects the next rays for training based on the temporal variation of the input videos. In combination, these two strategies significantly boost the training speed, lead to fast convergence of the training process, and enable high quality results. Our learned representation is highly compact and able to represent a 10 second 30 FPS multi-view video recording by 18 cameras with a model size of just 28MB. We demonstrate that our method can render high-fidelity wide-angle novel views at over 1K resolution, even for highly complex and dynamic scenes. We perform an extensive qualitative and quantitative evaluation that shows that our approach outperforms the current state of the art. Project website: https://neural-3d-video.github.io.</t>
+  </si>
+  <si>
+    <t>https://neural-3d-video.github.io/</t>
+  </si>
+  <si>
+    <t>Dynamic View Synthesis from Dynamic Monocular Video</t>
+  </si>
+  <si>
+    <t>We present an algorithm for generating novel views at arbitrary viewpoints and any input time step given a monocular video of a dynamic scene. Our work builds upon recent advances in neural implicit representation and uses continuous and differentiable functions for modeling the time-varying structure and the appearance of the scene. We jointly train a time-invariant static NeRF and a time-varying dynamic NeRF, and learn how to blend the results in an unsupervised manner. However, learning this implicit function from a single video is highly ill-posed (with infinitely many solutions that match the input video). To resolve the ambiguity, we introduce regularization losses to encourage a more physically plausible solution. We show extensive quantitative and qualitative results of dynamic view synthesis from casually captured videos.</t>
+  </si>
+  <si>
+    <t>https://free-view-video.github.io/</t>
+  </si>
+  <si>
+    <t>https://github.com/gaochen315/DynamicNeRF</t>
+  </si>
+  <si>
+    <t>GRAF: Generative Radiance Fields for 3D-Aware Image Synthesis</t>
+  </si>
+  <si>
+    <t>https://github.com/autonomousvision/graf</t>
+  </si>
+  <si>
+    <t>While 2D generative adversarial networks have enabled high-resolution image synthesis, they largely lack an understanding of the 3D world and the image formation process. Thus, they do not provide precise control over camera viewpoint or object pose. To address this problem, several recent approaches leverage intermediate voxel-based representations in combination with differentiable rendering. However, existing methods either produce low image resolution or fall short in disentangling camera and scene properties, eg, the object identity may vary with the viewpoint. In this paper, we propose a generative model for radiance fields which have recently proven successful for novel view synthesis of a single scene. In contrast to voxel-based representations, radiance fields are not confined to a coarse discretization of the 3D space, yet allow for disentangling camera and scene properties while degrading gracefully in the presence of reconstruction ambiguity. By introducing a multi-scale patch-based discriminator, we demonstrate synthesis of high-resolution images while training our model from unposed 2D images alone. We systematically analyze our approach on several challenging synthetic and real-world datasets. Our experiments reveal that radiance fields are a powerful representation for generative image synthesis, leading to 3D consistent models that render with high fidelity.</t>
+  </si>
+  <si>
+    <t>GRF: Learning a General Radiance Field for 3D Scene Representation and Rendering</t>
+  </si>
+  <si>
+    <t>We present a simple yet powerful neural network that implicitly represents and renders 3D objects and scenes only from 2D observations. The network models 3D geometries as a general radiance field, which takes a set of 2D images with camera poses and intrinsics as input, constructs an internal representation for each point of the 3D space, and then renders the corresponding appearance and geometry of that point viewed from an arbitrary position. The key to our approach is to learn local features for each pixel in 2D images and to then project these features to 3D points, thus yielding general and rich point representations. We additionally integrate an attention mechanism to aggregate pixel features from multiple 2D views, such that visual occlusions are implicitly taken into account. Extensive experiments demonstrate that our method can generate high-quality and realistic novel views for novel objects, unseen categories and challenging real-world scenes.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2010.04595</t>
+  </si>
+  <si>
+    <t>https://github.com/alextrevithick/GRF</t>
+  </si>
+  <si>
+    <t>pixelNeRF: Neural Radiance Fields from One or Few Images</t>
+  </si>
+  <si>
+    <t>We propose pixelNeRF, a learning framework that predicts a continuous neural scene representation conditioned on one or few input images. The existing approach for constructing neural radiance fields involves optimizing the representation to every scene independently, requiring many calibrated views and significant compute time. We take a step towards resolving these shortcomings by introducing an architecture that conditions a NeRF on image inputs in a fully convolutional manner. This allows the network to be trained across multiple scenes to learn a scene prior, enabling it to perform novel view synthesis in a feed-forward manner from a sparse set of views (as few as one). Leveraging the volume rendering approach of NeRF, our model can be trained directly from images with no explicit 3D supervision. We conduct extensive experiments on ShapeNet benchmarks for single image novel view synthesis tasks with held-out objects as well as entire unseen categories. We further demonstrate the flexibility of pixelNeRF by demonstrating it on multi-object ShapeNet scenes and real scenes from the DTU dataset. In all cases, pixelNeRF outperforms current state-of-the-art baselines for novel view synthesis and single image 3D reconstruction. For the video and code, please visit the project website: this https URL</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2012.02190</t>
+  </si>
+  <si>
+    <t>https://github.com/sxyu/pixel-nerf</t>
+  </si>
+  <si>
+    <t>Learned Initializations for Optimizing Coordinate-Based Neural Representations</t>
+  </si>
+  <si>
+    <t>Coordinate-based neural representations have shown significant promise as an alternative to discrete, array-based representations for complex low dimensional signals. However, optimizing a coordinate-based network from randomly initialized weights for each new signal is inefficient. We propose applying standard meta-learning algorithms to learn the initial weight parameters for these fully-connected networks based on the underlying class of signals being represented (e.g., images of faces or 3D models of chairs). Despite requiring only a minor change in implementation, using these learned initial weights enables faster convergence during optimization and can serve as a strong prior over the signal class being modeled, resulting in better generalization when only partial observations of a given signal are available. We explore these benefits across a variety of tasks, including representing 2D images, reconstructing CT scans, and recovering 3D shapes and scenes from 2D image observations.</t>
+  </si>
+  <si>
+    <t>https://github.com/tancik/learnit</t>
+  </si>
+  <si>
+    <t>https://www.matthewtancik.com/learnit</t>
+  </si>
+  <si>
+    <t>pi-GAN: Periodic Implicit Generative Adversarial Networks for 3D-Aware Image Synthesis</t>
+  </si>
+  <si>
+    <t>CVPR2021(oral)</t>
+  </si>
+  <si>
+    <t>ECCV2022(oral)</t>
+  </si>
+  <si>
+    <t>We have witnessed rapid progress on 3D-aware image synthesis, leveraging recent advances in generative visual models and neural rendering. Existing approaches however fall short in two ways: first, they may lack an underlying 3D representation or rely on view-inconsistent rendering, hence synthesizing images that are not multi-view consistent; second, they often depend upon representation network architectures that are not expressive enough, and their results thus lack in image quality. We propose a novel generative model, named Periodic Implicit Generative Adversarial Networks (π-GAN or pi-GAN), for high-quality 3D-aware image synthesis. π-GAN leverages neural representations with periodic activation functions and volumetric rendering to represent scenes as view-consistent 3D representations with fine detail. The proposed approach obtains state-of-the-art results for 3D-aware image synthesis with multiple real and synthetic datasets.</t>
+  </si>
+  <si>
+    <t>https://marcoamonteiro.github.io/pi-GAN-website/</t>
+  </si>
+  <si>
+    <t>https://github.com/marcoamonteiro/pi-GAN</t>
+  </si>
+  <si>
+    <t>Portrait Neural Radiance Fields from a Single Image</t>
+  </si>
+  <si>
+    <t>We present a method for estimating Neural Radiance Fields (NeRF) from a single headshot portrait. While NeRF has demonstrated high-quality view synthesis, it requires multiple images of static scenes and thus impractical for casual captures and moving subjects. In this work, we propose to pretrain the weights of a multilayer perceptron (MLP), which implicitly models the volumetric density and colors, with a meta-learning framework using a light stage portrait dataset. To improve the generalization to unseen faces, we train the MLP in the canonical coordinate space approximated by 3D face morphable models. We quantitatively evaluate the method using controlled captures and demonstrate the generalization to real portrait images, showing favorable results against state-of-the-arts.</t>
+  </si>
+  <si>
+    <t>https://portrait-nerf.github.io/</t>
+  </si>
+  <si>
+    <t>ShaRF: Shape-conditioned Radiance Fields from a Single View</t>
+  </si>
+  <si>
+    <t>ICML2021</t>
+  </si>
+  <si>
+    <t>We present a method for estimating neural scenes representations of objects given only a single image. The core of our method is the estimation of a geometric scaffold for the object and its use as a guide for the reconstruction of the underlying radiance field. Our formulation is based on a generative process that first maps a latent code to a voxelized shape, and then renders it to an image, with the object appearance being controlled by a second latent code. During inference, we optimize both the latent codes and the networks to fit a test image of a new object. The explicit disentanglement of shape and appearance allows our model to be fine-tuned given a single image. We can then render new views in a geometrically consistent manner and they represent faithfully the input object. Additionally, our method is able to generalize to images outside of the training domain (more realistic renderings and even real photographs). Finally, the inferred geometric scaffold is itself an accurate estimate of the object's 3D shape. We demonstrate in several experiments the effectiveness of our approach in both synthetic and real images.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2102.08860</t>
+  </si>
+  <si>
+    <t>https://github.com/tensorflow/graphics/tree/master/tensorflow_graphics/projects/radiance_fields</t>
+  </si>
+  <si>
+    <t>IBRNet: Learning Multi-View Image-Based Rendering</t>
+  </si>
+  <si>
+    <t>We present a method that synthesizes novel views of complex scenes by interpolating a sparse set of nearby views. The core of our method is a network architecture that includes a multilayer perceptron and a ray transformer that estimates radiance and volume density at continuous 5D locations (3D spatial locations and 2D viewing directions), drawing appearance information on the fly from multiple source views. By drawing on source views at render time, our method hearkens back to classic work on image-based rendering (IBR), and allows us to render high-resolution imagery. Unlike neural scene representation work that optimizes per-scene functions for rendering, we learn a generic view interpolation function that generalizes to novel scenes. We render images using classic volume rendering, which is fully differentiable and allows us to train using only multi-view posed images as supervision. Experiments show that our method outperforms recent novel view synthesis methods that also seek to generalize to novel scenes. Further, if fine-tuned on each scene, our method is competitive with state-of-the-art single-scene neural rendering methods. Project page: this https URL</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2102.13090</t>
+  </si>
+  <si>
+    <t>https://github.com/googleinterns/IBRNet</t>
+  </si>
+  <si>
+    <t>CAMPARI: Camera-Aware Decomposed Generative Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>Tremendous progress in deep generative models has led to photorealistic image synthesis. While achieving compelling results, most approaches operate in the two-dimensional image domain, ignoring the three-dimensional nature of our world. Several recent works therefore propose generative models which are 3D-aware, i.e., scenes are modeled in 3D and then rendered differentiably to the image plane. This leads to impressive 3D consistency, but incorporating such a bias comes at a price: the camera needs to be modeled as well. Current approaches assume fixed intrinsics and a predefined prior over camera pose ranges. As a result, parameter tuning is typically required for real-world data, and results degrade if the data distribution is not matched. Our key hypothesis is that learning a camera generator jointly with the image generator leads to a more principled approach to 3D-aware image synthesis. Further, we propose to decompose the scene into a background and foreground model, leading to more efficient and disentangled scene representations. While training from raw, unposed image collections, we learn a 3D- and camera-aware generative model which faithfully recovers not only the image but also the camera data distribution. At test time, our model generates images with explicit control over the camera as well as the shape and appearance of the scene.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/pdf/2103.17269.pdf</t>
+  </si>
+  <si>
+    <t>NeRF-VAE: A Geometry Aware 3D Scene Generative Model</t>
+  </si>
+  <si>
+    <t>We propose NeRF-VAE, a 3D scene generative model that incorporates geometric structure via NeRF and differentiable volume rendering. In contrast to NeRF, our model takes into account shared structure across scenes, and is able to infer the structure of a novel scene -- without the need to re-train -- using amortized inference. NeRF-VAE's explicit 3D rendering process further contrasts previous generative models with convolution-based rendering which lacks geometric structure. Our model is a VAE that learns a distribution over radiance fields by conditioning them on a latent scene representation. We show that, once trained, NeRF-VAE is able to infer and render geometrically-consistent scenes from previously unseen 3D environments using very few input images. We further demonstrate that NeRF-VAE generalizes well to out-of-distribution cameras, while convolutional models do not. Finally, we introduce and study an attention-based conditioning mechanism of NeRF-VAE's decoder, which improves model performance.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2104.00587</t>
+  </si>
+  <si>
+    <t>Unconstrained Scene Generation with Locally Conditioned Radiance Fields</t>
+  </si>
+  <si>
+    <t>https://apple.github.io/ml-gsn/</t>
+  </si>
+  <si>
+    <t>https://github.com/apple/ml-gsn</t>
+  </si>
+  <si>
+    <t>MVSNeRF: Fast Generalizable Radiance Field Reconstruction from Multi-View Stereo</t>
+  </si>
+  <si>
+    <t>We present MVSNeRF, a novel neural rendering approach that can efficiently reconstruct neural radiance fields for view synthesis. Unlike prior works on neural radiance fields that consider per-scene optimization on densely captured images, we propose a generic deep neural network that can reconstruct radiance fields from only three nearby input views via fast network inference. Our approach leverages plane-swept cost volumes (widely used in multi-view stereo) for geometry-aware scene reasoning, and combines this with physically based volume rendering for neural radiance field reconstruction. We train our network on real objects in the DTU dataset, and test it on three different datasets to evaluate its effectiveness and generalizability. Our approach can generalize across scenes (even indoor scenes, completely different from our training scenes of objects) and generate realistic view synthesis results using only three input images, significantly outperforming concurrent works on generalizable radiance field reconstruction. Moreover, if dense images are captured, our estimated radiance field representation can be easily fine-tuned; this leads to fast per-scene reconstruction with higher rendering quality and substantially less optimization time than NeRF.</t>
+  </si>
+  <si>
+    <t>https://apchenstu.github.io/mvsnerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/apchenstu/mvsnerf</t>
+  </si>
+  <si>
+    <t>Stereo Radiance Fields (SRF): Learning View Synthesis from Sparse Views of Novel Scenes</t>
+  </si>
+  <si>
+    <t>Recent neural view synthesis methods have achieved impressive quality and realism, surpassing classical pipelines which rely on multi-view reconstruction. State-of-the-Art methods, such as NeRF, are designed to learn a single scene with a neural network and require dense multi-view inputs. Testing on a new scene requires re-training from scratch, which takes 2-3 days. In this work, we introduce Stereo Radiance Fields (SRF), a neural view synthesis approach that is trained end-to-end, generalizes to new scenes, and requires only sparse views at test time. The core idea is a neural architecture inspired by classical multi-view stereo methods, which estimates surface points by finding similar image regions in stereo images. In SRF, we predict color and density for each 3D point given an encoding of its stereo correspondence in the input images. The encoding is implicitly learned by an ensemble of pair-wise similarities -- emulating classical stereo. Experiments show that SRF learns structure instead of overfitting on a scene. We train on multiple scenes of the DTU dataset and generalize to new ones without re-training, requiring only 10 sparse and spread-out views as input. We show that 10-15 minutes of fine-tuning further improve the results, achieving significantly sharper, more detailed results than scene-specific models. The code, model, and videos are available at this https URL.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2104.06935</t>
+  </si>
+  <si>
+    <t>https://virtualhumans.mpi-inf.mpg.de/srf/</t>
+  </si>
+  <si>
+    <t>Neural Rays for Occlusion-aware Image-based Rendering</t>
+  </si>
+  <si>
+    <t>We present a new neural representation, called Neural Ray (NeuRay), for the novel view synthesis task. Recent works construct radiance fields from image features of input views to render novel view images, which enables the generalization to new scenes. However, due to occlusions, a 3D point may be invisible to some input views. On such a 3D point, these generalization methods will include inconsistent image features from invisible views, which interfere with the radiance field construction. To solve this problem, we predict the visibility of 3D points to input views within our NeuRay representation. This visibility enables the radiance field construction to focus on visible image features, which significantly improves its rendering quality. Meanwhile, a novel consistency loss is proposed to refine the visibility in NeuRay when finetuning on a specific scene. Experiments demonstrate that our approach achieves state-of-the-art performance on the novel view synthesis task when generalizing to unseen scenes and outperforms per-scene optimization methods after finetuning.</t>
+  </si>
+  <si>
+    <t>https://liuyuan-pal.github.io/NeuRay/</t>
+  </si>
+  <si>
+    <t>https://github.com/liuyuan-pal/NeuRay</t>
+  </si>
+  <si>
+    <t>Putting NeRF on a Diet: Semantically Consistent Few-Shot View Synthesis</t>
+  </si>
+  <si>
+    <t>https://www.ajayj.com/dietnerf</t>
+  </si>
+  <si>
+    <t>https://github.com/ajayjain/DietNeRF</t>
+  </si>
+  <si>
+    <t>Towards Continuous Depth MPI with NeRF for Novel View Synthesis</t>
+  </si>
+  <si>
+    <t>In this paper, we propose MINE to perform novel view synthesis and depth estimation via dense 3D reconstruction from a single image. Our approach is a continuous depth generalization of the Multiplane Images (MPI) by introducing the NEural radiance fields (NeRF). Given a single image as input, MINE predicts a 4-channel image (RGB and volume density) at arbitrary depth values to jointly reconstruct the camera frustum and fill in occluded contents. The reconstructed and inpainted frustum can then be easily rendered into novel RGB or depth views using differentiable rendering. Extensive experiments on RealEstate10K, KITTI and Flowers Light Fields show that our MINE outperforms state-of-the-art by a large margin in novel view synthesis. We also achieve competitive results in depth estimation on iBims-1 and NYU-v2 without annotated depth supervision. Our source code is available at this https URL</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.14910</t>
+  </si>
+  <si>
+    <t>https://github.com/vincentfung13/MINE</t>
+  </si>
+  <si>
+    <t>TöRF: Time-of-Flight Radiance Fields for Dynamic Scene View Synthesis</t>
+  </si>
+  <si>
+    <t>Neural networks can represent and accurately reconstruct radiance fields for static 3D scenes (e.g., NeRF). Several works extend these to dynamic scenes captured with monocular video, with promising performance. However, the monocular setting is known to be an under-constrained problem, and so methods rely on data-driven priors for reconstructing dynamic content. We replace these priors with measurements from a time-of-flight (ToF) camera, and introduce a neural representation based on an image formation model for continuous-wave ToF cameras. Instead of working with processed depth maps, we model the raw ToF sensor measurements to improve reconstruction quality and avoid issues with low reflectance regions, multi-path interference, and a sensor's limited unambiguous depth range. We show that this approach improves robustness of dynamic scene reconstruction to erroneous calibration and large motions, and discuss the benefits and limitations of integrating RGB+ToF sensors that are now available on modern smartphones.</t>
+  </si>
+  <si>
+    <t>https://imaging.cs.cmu.edu/torf/</t>
+  </si>
+  <si>
+    <t>https://github.com/breuckelen/torf</t>
+  </si>
+  <si>
+    <t>CodeNeRF: Disentangled Neural Radiance Fields for Object Categories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeNeRF is an implicit 3D neural representation that learns the variation of object shapes and textures across a category and can be trained, from a set of posed images, to synthesize novel views of unseen objects. Unlike the original NeRF, which is scene specific, CodeNeRF learns to disentangle shape and texture by learning separate embeddings. At test time, given a single unposed image of an unseen object, CodeNeRF jointly estimates camera viewpoint, and shape and appearance codes via optimization. Unseen objects can be reconstructed from a single image, and then rendered from new viewpoints or their shape and texture edited by varying the latent codes. We conduct experiments on the SRN benchmark, which show that CodeNeRF generalises well to unseen objects and achieves on-par performance with methods that require known camera pose at test time. Our results on real-world images demonstrate that CodeNeRF can bridge the sim-to-real gap. </t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https%3A%2F%2Fgithub.com%2Fwbjang%2Fcode-nerf&amp;sa=D&amp;sntz=1&amp;usg=AOvVaw2eD5ZoRbk2aWFuwUSHlh5_</t>
+  </si>
+  <si>
+    <t>https://www.google.com/url?q=https%3A%2F%2Farxiv.org%2Fpdf%2F2109.01750.pdf&amp;sa=D&amp;sntz=1&amp;usg=AOvVaw1Fnir0e4aRa22Nt0HoXDWh</t>
+  </si>
+  <si>
+    <t>StyleNeRF: A Style-based 3D-Aware Generator for High-resolution Image Synthesis</t>
+  </si>
+  <si>
+    <t>ICLR2022</t>
+  </si>
+  <si>
+    <t>We propose StyleNeRF, a 3D-aware generative model for photo-realistic high-resolution image synthesis with high multi-view consistency, which can be trained on unstructured 2D images. Existing approaches either cannot synthesize high-resolution images with fine details or yield noticeable 3D-inconsistent artifacts. In addition, many of them lack control over style attributes and explicit 3D camera poses. StyleNeRF integrates the neural radiance field (NeRF) into a style-based generator to tackle the aforementioned challenges, i.e., improving rendering efficiency and 3D consistency for high-resolution image generation. We perform volume rendering only to produce a low-resolution feature map and progressively apply upsampling in 2D to address the first issue. To mitigate the inconsistencies caused by 2D upsampling, we propose multiple designs, including a better upsampler and a new regularization loss. With these designs, StyleNeRF can synthesize high-resolution images at interactive rates while preserving 3D consistency at high quality. StyleNeRF also enables control of camera poses and different levels of styles, which can generalize to unseen views. It also supports challenging tasks, including zoom-in and-out, style mixing, inversion, and semantic editing.</t>
+  </si>
+  <si>
+    <t>https://jiataogu.me/style_nerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/facebookresearch/StyleNeRF</t>
+  </si>
+  <si>
+    <t>NeRF in the Dark: High Dynamic Range View Synthesis from Noisy Raw Images</t>
+  </si>
+  <si>
+    <t>Neural Radiance Fields (NeRF) is a technique for high quality novel view synthesis from a collection of posed input images. Like most view synthesis methods, NeRF uses tonemapped low dynamic range (LDR) as input; these images have been processed by a lossy camera pipeline that smooths detail, clips highlights, and distorts the simple noise distribution of raw sensor data. We modify NeRF to instead train directly on linear raw images, preserving the scene's full dynamic range. By rendering raw output images from the resulting NeRF, we can perform novel high dynamic range (HDR) view synthesis tasks. In addition to changing the camera viewpoint, we can manipulate focus, exposure, and tonemapping after the fact. Although a single raw image appears significantly more noisy than a postprocessed one, we show that NeRF is highly robust to the zero-mean distribution of raw noise. When optimized over many noisy raw inputs (25-200), NeRF produces a scene representation so accurate that its rendered novel views outperform dedicated single and multi-image deep raw denoisers run on the same wide baseline input images. As a result, our method, which we call RawNeRF, can reconstruct scenes from extremely noisy images captured in near-darkness.</t>
+  </si>
+  <si>
+    <t>https://bmild.github.io/rawnerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/google-research/multinerf</t>
+  </si>
+  <si>
+    <t>iNeRF: Inverting Neural Radiance Fields for Pose Estimation</t>
+  </si>
+  <si>
+    <t>IROS2021</t>
+  </si>
+  <si>
+    <t>We present iNeRF, a framework that performs pose estimation by “inverting” a trained Neural Radiance Field(NeRF). NeRFs have been shown to be remarkably effective for the task of view synthesis — synthesizing photorealisticnovel views of real-world scenes or objects. In this work, we investigate whether we can apply analysis-by-synthesis with NeRF for 6DoF pose estimation – given an image, find the translation and rotation of a camera relative to a 3Dmodel. Starting from an initial pose estimate, we use gradient descent to minimize the residual between pixels rendered from an already-trained NeRF and pixels in an observed image. In our experiments, we first study 1) how to sample rays during pose refinement for iNeRF to collect informative gradients and 2) how different batch sizes ofrays affect iNeRF on a synthetic dataset. We then show that for complex real-world scenes from the LLFF dataset, iNeRF can improve NeRF by estimating the camera poses of novel images and using these images as additional trainingdata for NeRF. Finally, we show iNeRF can be combinedwith feature-based pose initialization. The approach outperforms all other RGB-based methods relying on syntheticdata on LineMOD.</t>
+  </si>
+  <si>
+    <t>http://yenchenlin.me/inerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/yenchenlin/iNeRF-public</t>
+  </si>
+  <si>
+    <t>A-NeRF: Surface-free Human 3D Pose Refinement via Neural Rendering</t>
+  </si>
+  <si>
+    <t>NeurIPS2020</t>
+  </si>
+  <si>
+    <t>NeurIPS2021(spotlight)</t>
+  </si>
+  <si>
+    <t>https://avg.is.mpg.de/publications/schwarz2020NeurIPS</t>
+  </si>
+  <si>
+    <t>NeurIPS2021</t>
+  </si>
+  <si>
+    <t>While deep learning reshaped the classical motion capture pipeline with feed-forward networks, generative models are required to recover fine alignment via iterative refinement. Unfortunately, the existing models are usually hand-crafted or learned in controlled conditions, only applicable to limited domains. We propose a method to learn a generative neural body model from unlabelled monocular videos by extending Neural Radiance Fields (NeRFs). We equip them with a skeleton to apply to time-varying and articulated motion. A key insight is that implicit models require the inverse of the forward kinematics used in explicit surface models. Our reparameterization defines spatial latent variables relative to the pose of body parts and thereby overcomes ill-posed inverse operations with an overparameterization. This enables learning volumetric body shape and appearance from scratch while jointly refining the articulated pose; all without ground truth labels for appearance, pose, or 3D shape on the input videos. When used for novel-view-synthesis and motion capture, our neural model improves accuracy on diverse datasets. Project website: this https URL .</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2102.06199</t>
+  </si>
+  <si>
+    <t>https://github.com/LemonATsu/A-NeRF</t>
+  </si>
+  <si>
+    <t>https://nerfmm.active.vision/</t>
+  </si>
+  <si>
+    <t>NeRF--: Neural Radiance Fields Without Known Camera Parameters</t>
+  </si>
+  <si>
+    <t>https://github.com/ActiveVisionLab/nerfmm</t>
+  </si>
+  <si>
+    <t>Implicit Mapping and Positioning in Real-Time</t>
+  </si>
+  <si>
+    <t>We show for the first time that a multilayer perceptron (MLP) can serve as the only scene representation in a real-time SLAM system for a handheld RGB-D camera. Our network is trained in live operation without prior data, building a dense, scene-specific implicit 3D model of occupancy and colour which is also immediately used for tracking.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.12352</t>
+  </si>
+  <si>
+    <t>NICE-SLAM  Neural Implicit Scalable Encoding for SLAM</t>
+  </si>
+  <si>
+    <t>Neural implicit representations have recently shown encouraging results in various domains, including promising progress in simultaneous localization and mapping (SLAM). Nevertheless, existing methods produce over-smoothed scene reconstructions and have difficulty scaling up to large scenes. These limitations are mainly due to their simple fully-connected network architecture that does not incorporate local information in the observations. In this paper, we present NICE-SLAM, a dense SLAM system that incorporates multi-level local information by introducing a hierarchical scene representation. Optimizing this representation with pre-trained geometric priors enables detailed reconstruction on large indoor scenes. Compared to recent neural implicit SLAM systems, our approach is more scalable, efficient, and robust. Experiments on five challenging datasets demonstrate competitive results of NICE-SLAM in both mapping and tracking quality.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2112.12130</t>
+  </si>
+  <si>
+    <t>https://github.com/cvg/nice-slam</t>
+  </si>
+  <si>
+    <t>GNeRF: GAN-based Neural Radiance Field without Posed Camera</t>
+  </si>
+  <si>
+    <t>We introduce GNeRF, a framework to marry Generative Adversarial Networks (GAN) with Neural Radiance Field (NeRF) reconstruction for the complex scenarios with unknown and even randomly initialized camera poses. Recent NeRF-based advances have gained popularity for remarkable realistic novel view synthesis. However, most of them heavily rely on accurate camera poses estimation, while few recent methods can only optimize the unknown camera poses in roughly forward-facing scenes with relatively short camera trajectories and require rough camera poses initialization. Differently, our GNeRF only utilizes randomly initialized poses for complex outside-in scenarios. We propose a novel two-phases end-to-end framework. The first phase takes the use of GANs into the new realm for optimizing coarse camera poses and radiance fields jointly, while the second phase refines them with additional photometric loss. We overcome local minima using a hybrid and iterative optimization scheme. Extensive experiments on a variety of synthetic and natural scenes demonstrate the effectiveness of GNeRF. More impressively, our approach outperforms the baselines favorably in those scenes with repeated patterns or even low textures that are regarded as extremely challenging before.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2103.15606</t>
+  </si>
+  <si>
+    <t>BARF: Bundle-Adjusting Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>Neural Radiance Fields (NeRF) have recently gained a surge of interest within the computer vision community for its power to synthesize photorealistic novel views of real-world scenes. One limitation of NeRF, however, is its requirement of accurate camera poses to learn the scene representations. In this paper, we propose Bundle-Adjusting Neural Radiance Fields (BARF) for training NeRF from imperfect (or even unknown) camera poses — the joint problem of learning neural 3D representations and registering camera frames. We establish a theoretical connection to classical image alignment and show that coarse-to-fine registration is also applicable to NeRF. Furthermore, we show that naively applying positional encoding in NeRF has a negative impact on registration with a synthesis-based objective. Experiments on synthetic and real-world data show that BARF can effectively optimize the neural scene representations and resolve large camera pose misalignment at the same time. This enables view synthesis and localization of video sequences from unknown camera poses, opening up new avenues for visual localization systems (e.g. SLAM) and potential applications for dense 3D mapping and reconstruction.</t>
+  </si>
+  <si>
+    <t>https://chenhsuanlin.bitbucket.io/bundle-adjusting-NeRF/</t>
+  </si>
+  <si>
+    <t>https://github.com/chenhsuanlin/bundle-adjusting-NeRF</t>
+  </si>
+  <si>
+    <t>Self-Calibrating Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>In this work, we propose a camera self-calibration algorithm for generic cameras with arbitrary non-linear distortions. We jointly learn the geometry of the scene and the accurate camera parameters without any calibration objects. Our camera model consists a pinhole model, radial distortion, and a generic noise model that can learn arbitrary non-linear camera distortions. While traditional self-calibration algorithms mostly rely on geometric constraints, we additionally incorporate photometric consistency. This requires learning the geometry of the scene and we use Neural Radiance Fields (NeRF). We also propose a new geometric loss function, viz., projected ray distance loss, to incorporate geometric consistency for complex non-linear camera models. We validate our approach on standard real image datasets and demonstrate our model can learn the camera intrinsics and extrinsics (pose) from scratch without COLMAP initialization. Also, we show that learning accurate camera models in differentiable manner allows us to improves PSNR over NeRF. We experimentally demonstrate that our proposed method is applicable to variants of NeRF. In addition, we use a set of images captured with a fish-eye lens to demonstrate that learning camera model jointly improves the performance significantly over the COLMAP initialization.</t>
+  </si>
+  <si>
+    <t>https://postech-cvlab.github.io/SCNeRF/</t>
+  </si>
+  <si>
+    <t>https://github.com/POSTECH-CVLab/SCNeRF</t>
+  </si>
+  <si>
+    <t>NeRD: Neural Reflectance Decomposition from Image Collections</t>
+  </si>
+  <si>
+    <t>Decomposing a scene into its shape, reflectance, and illumination is a challenging but important problem in computer vision and graphics. This problem is inherently more challenging when the illumination is not a single light source under laboratory conditions but is instead an unconstrained environmental illumination. Though recent work has shown that implicit representations can be used to model the radiance field of an object, most of these techniques only enable view synthesis and not relighting. Additionally, evaluating these radiance fields is resource and time-intensive. We propose a neural reflectance decomposition (NeRD) technique that uses physically-based rendering to decompose the scene into spatially varying BRDF material properties. In contrast to existing techniques, our input images can be captured under different illumination conditions. In addition, we also propose techniques to convert the learned reflectance volume into a relightable textured mesh enabling fast real-time rendering with novel illuminations. We demonstrate the potential of the proposed approach with experiments on both synthetic and real datasets, where we are able to obtain high-quality relightable 3D assets from image collections.</t>
+  </si>
+  <si>
+    <t>https://markboss.me/publication/2021-nerd/#:~:text=NeRD%20is%20a%20novel%20method,can%20turn%20around%20the%20object.</t>
+  </si>
+  <si>
+    <t>https://github.com/cgtuebingen/NeRD-Neural-Reflectance-Decomposition</t>
+  </si>
+  <si>
+    <t>NeRV: Neural Reflectance and Visibility Fields for Relighting and View Synthesis</t>
+  </si>
+  <si>
+    <t>We present a method that takes as input a set of images of a scene illuminated by unconstrained known lighting, and produces as output a 3D representation that can be rendered from novel viewpoints under arbitrary lighting conditions. Our method represents the scene as a continuous volumetric function parameterized as MLPs whose inputs are a 3D location and whose outputs are the following scene properties at that input location: volume density, surface normal, material parameters, distance to the first surface intersection in any direction, and visibility of the external environment in any direction. Together, these allow us to render novel views of the object under arbitrary lighting, including indirect illumination effects. The predicted visibility and surface intersection fields are critical to our model's ability to simulate direct and indirect illumination during training, because the brute-force techniques used by prior work are intractable for lighting conditions outside of controlled setups with a single light. Our method outperforms alternative approaches for recovering relightable 3D scene representations, and performs well in complex lighting settings that have posed a significant challenge to prior work.</t>
+  </si>
+  <si>
+    <t>https://pratulsrinivasan.github.io/nerv/</t>
+  </si>
+  <si>
+    <t>NeX: Real-time View Synthesis with Neural Basis Expansion</t>
+  </si>
+  <si>
+    <t>We present NeX, a new approach to novel view synthesis based on enhancements of multiplane image (MPI) that can reproduce NeXt-level view-dependent effects---in real time. Unlike traditional MPI that uses a set of simple RGBα planes, our technique models view-dependent effects by instead parameterizing each pixel as a linear combination of basis functions learned from a neural network. Moreover, we propose a hybrid implicit-explicit modeling strategy that improves upon fine detail and produces state-of-the-art results. Our method is evaluated on benchmark forward-facing datasets as well as our newly-introduced dataset designed to test the limit of view-dependent modeling with significantly more challenging effects such as the rainbow reflections on a CD. Our method achieves the best overall scores across all major metrics on these datasets with more than 1000× faster rendering time than the state of the art.</t>
+  </si>
+  <si>
+    <t>https://nex-mpi.github.io/</t>
+  </si>
+  <si>
+    <t>https://github.com/nex-mpi/nex-code/</t>
+  </si>
+  <si>
+    <t>https://xiuming.info/projects/nerfactor/</t>
+  </si>
+  <si>
+    <t>NeRFactor: Neural Factorization of Shape and Reflectance Under an Unknown Illumination</t>
+  </si>
+  <si>
+    <t>TOG 2021 (Proc. SIGGRAPH Asia)</t>
+  </si>
+  <si>
+    <t>We address the problem of recovering the shape and spatially-varying reflectance of an object from multi-view images (and their camera poses) of an object illuminated by one unknown lighting condition. This enables the rendering of novel views of the object under arbitrary environment lighting and editing of the object's material properties. The key to our approach, which we call Neural Radiance Factorization (NeRFactor), is to distill the volumetric geometry of a Neural Radiance Field (NeRF) [Mildenhall et al. 2020] representation of the object into a surface representation and then jointly refine the geometry while solving for the spatially-varying reflectance and environment lighting. Specifically, NeRFactor recovers 3D neural fields of surface normals, light visibility, albedo, and Bidirectional Reflectance Distribution Functions (BRDFs) without any supervision, using only a re-rendering loss, simple smoothness priors, and a data-driven BRDF prior learned from real-world BRDF measurements. By explicitly modeling light visibility, NeRFactor is able to separate shadows from albedo and synthesize realistic soft or hard shadows under arbitrary lighting conditions. NeRFactor is able to recover convincing 3D models for free-viewpoint relighting in this challenging and underconstrained capture setup for both synthetic and real scenes. Qualitative and quantitative experiments show that NeRFactor outperforms classic and deep learning-based state of the art across various tasks. Our videos, code, and data are available at people.csail.mit.edu/xiuming/projects/nerfactor/.</t>
+  </si>
+  <si>
+    <t>NeRF++: Analyzing and Improving Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>Neural Radiance Fields (NeRF) achieve impressive view synthesis results for a variety of capture settings, including 360 capture of bounded scenes and forward-facing capture of bounded and unbounded scenes. NeRF fits multi-layer perceptrons (MLPs) representing view-invariant opacity and view-dependent color volumes to a set of training images, and samples novel views based on volume rendering techniques. In this technical report, we first remark on radiance fields and their potential ambiguities, namely the shape-radiance ambiguity, and analyze NeRF's success in avoiding such ambiguities. Second, we address a parametrization issue involved in applying NeRF to 360 captures of objects within large-scale, unbounded 3D scenes. Our method improves view synthesis fidelity in this challenging scenario. Code is available at this https URL.</t>
+  </si>
+  <si>
+    <t>https://github.com/Kai-46/nerfplusplus;</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2010.07492</t>
+  </si>
+  <si>
+    <t>GIRAFFE: Representing Scenes as Compositional Generative Neural Feature Fields</t>
+  </si>
+  <si>
+    <t>Deep generative models allow for photorealistic image synthesis at high resolutions. But for many applications, this is not enough: content creation also needs to be controllable. While several recent works investigate how to disentangle underlying factors of variation in the data, most of them operate in 2D and hence ignore that our world is three-dimensional. Further, only few works consider the compositional nature of scenes. Our key hypothesis is that incorporating a compositional 3D scene representation into the generative model leads to more controllable image synthesis. Representing scenes as compositional generative neural feature fields allows us to disentangle one or multiple objects from the background as well as individual objects' shapes and appearances while learning from unstructured and unposed image collections without any additional supervision. Combining this scene representation with a neural rendering pipeline yields a fast and realistic image synthesis model. As evidenced by our experiments, our model is able to disentangle individual objects and allows for translating and rotating them in the scene as well as changing the camera pose.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2011.12100</t>
+  </si>
+  <si>
+    <t>https://github.com/autonomousvision/giraffe</t>
+  </si>
+  <si>
+    <t>Object-Centric Neural Scene Rendering</t>
+  </si>
+  <si>
+    <t>We present a method for composing photorealistic scenes from captured images of objects. Our work builds upon neural radiance fields (NeRFs), which implicitly model the volumetric density and directionally-emitted radiance of a scene. While NeRFs synthesize realistic pictures, they only model static scenes and are closely tied to specific imaging conditions. This property makes NeRFs hard to generalize to new scenarios, including new lighting or new arrangements of objects. Instead of learning a scene radiance field as a NeRF does, we propose to learn object-centric neural scattering functions (OSFs), a representation that models per-object light transport implicitly using a lighting- and view-dependent neural network. This enables rendering scenes even when objects or lights move, without retraining. Combined with a volumetric path tracing procedure, our framework is capable of rendering both intra- and inter-object light transport effects including occlusions, specularities, shadows, and indirect illumination. We evaluate our approach on scene composition and show that it generalizes to novel illumination conditions, producing photorealistic, physically accurate renderings of multi-object scenes.</t>
+  </si>
+  <si>
+    <t>https://shellguo.com/osf/</t>
+  </si>
+  <si>
+    <t>Learning Compositional Radiance Fields of Dynamic Human Heads</t>
+  </si>
+  <si>
+    <t>Photorealistic rendering of dynamic humans is an important ability for telepresence systems, virtual shopping, synthetic data generation, and more. Recently, neural rendering methods, which combine techniques from computer graphics and machine learning, have created high-fidelity models of humans and objects. Some of these methods do not produce results with high-enough fidelity for driveable human models (Neural Volumes) whereas others have extremely long rendering times (NeRF). We propose a novel compositional 3D representation that combines the best of previous methods to produce both higher-resolution and faster results. Our representation bridges the gap between discrete and continuous volumetric representations by combining a coarse 3D-structure-aware grid of animation codes with a continuous learned scene function that maps every position and its corresponding local animation code to its view-dependent emitted radiance and local volume density. Differentiable volume rendering is employed to compute photo-realistic novel views of the human head and upper body as well as to train our novel representation end-to-end using only 2D supervision. In addition, we show that the learned dynamic radiance field can be used to synthesize novel unseen expressions based on a global animation code. Our approach achieves state-of-the-art results for synthesizing novel views of dynamic human heads and the upper body.</t>
+  </si>
+  <si>
+    <t>https://ziyanw1.github.io/hybrid_nerf/</t>
+  </si>
+  <si>
+    <t>Neural Scene Graphs for Dynamic Scenes</t>
+  </si>
+  <si>
+    <t>Recent implicit neural rendering methods have demonstrated that it is possible to learn accurate view synthesis for complex scenes by predicting their volumetric density and color supervised solely by a set of RGB images. However, existing methods are restricted to learning efficient representations of static scenes that encode all scene objects into a single neural network, and lack the ability to represent dynamic scenes and decompositions into individual scene objects. In this work, we present the first neural rendering method that decomposes dynamic scenes into scene graphs. We propose a learned scene graph representation, which encodes object transformation and radiance, to efficiently render novel arrangements and views of the scene. To this end, we learn implicitly encoded scenes, combined with a jointly learned latent representation to describe objects with a single implicit function. We assess the proposed method on synthetic and real automotive data, validating that our approach learns dynamic scenes -- only by observing a video of this scene -- and allows for rendering novel photo-realistic views of novel scene compositions with unseen sets of objects at unseen poses.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2011.10379</t>
+  </si>
+  <si>
+    <t>https://github.com/princeton-computational-imaging/neural-scene-graphs</t>
+  </si>
+  <si>
+    <t>Unsupervised Discovery of Object Radiance Fields</t>
+  </si>
+  <si>
+    <t>We study the problem of inferring an object-centric scene representation from a single image, aiming to derive a representation that explains the image formation process, captures the scene's 3D nature, and is learned without supervision. Most existing methods on scene decomposition lack one or more of these characteristics, due to the fundamental challenge in integrating the complex 3D-to-2D image formation process into powerful inference schemes like deep networks. In this paper, we propose unsupervised discovery of Object Radiance Fields (uORF), integrating recent progresses in neural 3D scene representations and rendering with deep inference networks for unsupervised 3D scene decomposition. Trained on multi-view RGB images without annotations, uORF learns to decompose complex scenes with diverse, textured background from a single image. We show that uORF performs well on unsupervised 3D scene segmentation, novel view synthesis, and scene editing on three datasets.</t>
+  </si>
+  <si>
+    <t>Learning Object-Compositional Neural Radiance Field for Editable Scene Rendering</t>
+  </si>
+  <si>
+    <t>Implicit neural rendering techniques have shown promising results for novel view synthesis. However, existing methods usually encode the entire scene as a whole, which is generally not aware of the object identity and limits the ability to the high-level editing tasks such as moving or adding furniture. In this paper, we present a novel neural scene rendering system, which learns an object-compositional neural radiance field and produces realistic rendering with editing capability for a clustered and real-world scene. Specifically, we design a novel two-pathway architecture, in which the scene branch encodes the scene geometry and appearance, and the object branch encodes each standalone object conditioned on learnable object activation codes. To survive the training in heavily cluttered scenes, we propose a scene-guided training strategy to solve the 3D space ambiguity in the occluded regions and learn sharp boundaries for each object. Extensive experiments demonstrate that our system not only achieves competitive performance for static scene novel-view synthesis, but also produces realistic rendering for object-level editing.</t>
+  </si>
+  <si>
+    <t>https://zju3dv.github.io/object_nerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/zju3dv/object_nerf</t>
+  </si>
+  <si>
+    <t>https://shuaifengzhi.com/Semantic-NeRF/</t>
+  </si>
+  <si>
+    <t>https://github.com/Harry-Zhi/semantic_nerf/</t>
+  </si>
+  <si>
+    <t>Semantic labelling is highly correlated with geometry and radiance reconstruction, as scene entities with similar shape and appearance are more likely to come from similar classes. Recent implicit neural reconstruction techniques are appealing as they do not require prior training data, but the same fully self-supervised approach is not possible for semantics because labels are human-defined properties.</t>
+  </si>
+  <si>
+    <t>In-Place Scene Labelling and Understanding with Implicit Scene Representation</t>
+  </si>
+  <si>
+    <t>Editing Conditional Radiance Fields</t>
+  </si>
+  <si>
+    <t>A neural radiance field (NeRF) is a scene model supporting high-quality view synthesis, optimized per scene. In this paper, we explore enabling user editing of a category-level NeRF - also known as a conditional radiance field - trained on a shape category. Specifically, we introduce a method for propagating coarse 2D user scribbles to the 3D space, to modify the color or shape of a local region. First, we propose a conditional radiance field that incorporates new modular network components, including a shape branch that is shared across object instances. Observing multiple instances of the same category, our model learns underlying part semantics without any supervision, thereby allowing the propagation of coarse 2D user scribbles to the entire 3D region (e.g., chair seat). Next, we propose a hybrid network update strategy that targets specific network components, which balances efficiency and accuracy. During user interaction, we formulate an optimization problem that both satisfies the user's constraints and preserves the original object structure. We demonstrate our approach on various editing tasks over three shape datasets and show that it outperforms prior neural editing approaches. Finally, we edit the appearance and shape of a real photograph and show that the edit propagates to extrapolated novel views.</t>
+  </si>
+  <si>
+    <t>http://editnerf.csail.mit.edu/</t>
+  </si>
+  <si>
+    <t>https://github.com/stevliu/editnerf</t>
+  </si>
+  <si>
+    <t>Editable Free-Viewpoint Video using a Layered Neural Representation</t>
+  </si>
+  <si>
+    <t>Generating free-viewpoint videos is critical for immersive VR/AR experience but recent neural advances still lack the editing ability to manipulate the visual perception for large dynamic scenes. To fill this gap, in this paper we propose the first approach for editable photo-realistic free-viewpoint video generation for large-scale dynamic scenes using only sparse 16 cameras. The core of our approach is a new layered neural representation, where each dynamic entity including the environment itself is formulated into a space-time coherent neural layered radiance representation called ST-NeRF. Such layered representation supports fully perception and realistic manipulation of the dynamic scene whilst still supporting a free viewing experience in a wide range. In our ST-NeRF, the dynamic entity/layer is represented as continuous functions, which achieves the disentanglement of location, deformation as well as the appearance of the dynamic entity in a continuous and self-supervised manner. We propose a scene parsing 4D label map tracking to disentangle the spatial information explicitly, and a continuous deform module to disentangle the temporal motion implicitly. An object-aware volume rendering scheme is further introduced for the re-assembling of all the neural layers. We adopt a novel layered loss and motion-aware ray sampling strategy to enable efficient training for a large dynamic scene with multiple performers, Our framework further enables a variety of editing functions, i.e., manipulating the scale and location, duplicating or retiming individual neural layers to create numerous visual effects while preserving high realism. Extensive experiments demonstrate the effectiveness of our approach to achieve high-quality, photo-realistic, and editable free-viewpoint video generation for dynamic scenes.</t>
+  </si>
+  <si>
+    <t>https://jiakai-zhang.github.io/st-nerf/</t>
+  </si>
+  <si>
+    <t>https://jiakai-zhang.github.io/st-nerf/#code</t>
+  </si>
+  <si>
+    <t>FiG-NeRF: Figure Ground Neural Radiance Fields for 3D Object Category Modelling</t>
+  </si>
+  <si>
+    <t>3DV2021</t>
+  </si>
+  <si>
+    <t>We investigate the use of Neural Radiance Fields (NeRF) to learn high quality 3D object category models from collections of input images. In contrast to previous work, we are able to do this whilst simultaneously separating foreground objects from their varying backgrounds. We achieve this via a 2-component NeRF model, FiG-NeRF, that prefers explanation of the scene as a geometrically constant background and a deformable foreground that represents the object category. We show that this method can learn accurate 3D object category models using only photometric supervision and casually captured images of the objects. Additionally, our 2-part decomposition allows the model to perform accurate and crisp amodal segmentation. We quantitatively evaluate our method with view synthesis and image fidelity metrics, using synthetic, lab-captured, and in-the-wild data. Our results demonstrate convincing 3D object category modelling that exceed the performance of existing methods.</t>
+  </si>
+  <si>
+    <t>https://fig-nerf.github.io/</t>
+  </si>
+  <si>
+    <t>NeRF-Tex: Neural Reflectance Field Textures</t>
+  </si>
+  <si>
+    <t>EGSR2021</t>
+  </si>
+  <si>
+    <t>We investigate the use of neural fields for modeling diverse mesoscale structures, such as fur, fabric, and grass. Instead of using classical graphics primitives to model the structure, we propose to employ a versatile volumetric primitive represented by a neural reflectance field (NeRF-Tex), which jointly models the geometry of the material and its response to lighting. The NeRF-Tex primitive can be instantiated over a base mesh to “texture” it with the desired meso and microscale appearance. We condition the reflectance field on user-defined parameters that control the appearance. A single NeRF texture thus captures an entire space of reflectance fields rather than one specific structure. This increases the gamut of appearances that can be modeled and provides a solution for combating repetitive texturing artifacts. We also demonstrate that NeRF textures naturally facilitate continuous level-of-detail rendering. Our approach unites the versatility and modeling power of neural networks with the artistic control needed for precise modeling of virtual scenes. While all our training data is currently synthetic, our work provides a recipe that can be further extended to extract complex, hard-to-model appearances from real images.</t>
+  </si>
+  <si>
+    <t>https://developer.nvidia.com/blog/nvidia-research-nerf-tex-neural-reflectance-field-textures/</t>
+  </si>
+  <si>
+    <t>https://github.com/hbaatz/nerf-tex</t>
+  </si>
+  <si>
+    <t>Mip-NeRF: A Multiscale Representation for Anti-Aliasing Neural Radiance Fields</t>
+  </si>
+  <si>
+    <t>The rendering procedure used by neural radiance fields (NeRF) samples a scene with a single ray per pixel and may therefore produce renderings that are excessively blurred or aliased when training or testing images observe scene content at different resolutions. The straightforward solution of supersampling by rendering with multiple rays per pixel is impractical for NeRF, because rendering each ray requires querying a multilayer perceptron hundreds of times. Our solution, which we call "mip-NeRF" (à la "mipmap"), extends NeRF to represent the scene at a continuously-valued scale. By efficiently rendering anti-aliased conical frustums instead of rays, mip-NeRF reduces objectionable aliasing artifacts and significantly improves NeRF's ability to represent fine details, while also being 7% faster than NeRF and half the size. Compared to NeRF, mip-NeRF reduces average error rates by 17% on the dataset presented with NeRF and by 60% on a challenging multiscale variant of that dataset that we present. mip-NeRF is also able to match the accuracy of a brute-force supersampled NeRF on our multiscale dataset while being 22x faster.</t>
+  </si>
+  <si>
+    <t>https://jonbarron.info/mipnerf/</t>
+  </si>
+  <si>
+    <t>https://github.com/google/mipnerf</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2104.10078</t>
+  </si>
+  <si>
+    <t>UNISURF: Unifying Neural Implicit Surfaces and Radiance Fields for Multi-View Reconstruction</t>
+  </si>
+  <si>
+    <t>Neural implicit 3D representations have emerged as a powerful paradigm for reconstructing surfaces from multi-view images and synthesizing novel views. Unfortunately, existing methods such as DVR or IDR require accurate per-pixel object masks as supervision. At the same time, neural radiance fields have revolutionized novel view synthesis. However, NeRF's estimated volume density does not admit accurate surface reconstruction. Our key insight is that implicit surface models and radiance fields can be formulated in a unified way, enabling both surface and volume rendering using the same model. This unified perspective enables novel, more efficient sampling procedures and the ability to reconstruct accurate surfaces without input masks. We compare our method on the DTU, BlendedMVS, and a synthetic indoor dataset. Our experiments demonstrate that we outperform NeRF in terms of reconstruction quality while performing on par with IDR without requiring masks.</t>
+  </si>
+  <si>
+    <t>https://github.com/autonomousvision/unisurf</t>
+  </si>
+  <si>
+    <t>NeuS: Learning Neural Implicit Surfaces by Volume Rendering for Multi-view Reconstruction</t>
+  </si>
+  <si>
+    <t>We present a novel neural surface reconstruction method, called NeuS, for reconstructing objects and scenes with high fidelity from 2D image inputs. Existing neural surface reconstruction approaches, such as DVR and IDR, require foreground mask as supervision, easily get trapped in local minima, and therefore struggle with the reconstruction of objects with severe self-occlusion or thin structures. Meanwhile, recent neural methods for novel view synthesis, such as NeRF and its variants, use volume rendering to produce a neural scene representation with robustness of optimization, even for highly complex objects. However, extracting high-quality surfaces from this learned implicit representation is difficult because there are not sufficient surface constraints in the representation. In NeuS, we propose to represent a surface as the zero-level set of a signed distance function (SDF) and develop a new volume rendering method to train a neural SDF representation. We observe that the conventional volume rendering method causes inherent geometric errors (i.e. bias) for surface reconstruction, and therefore propose a new formulation that is free of bias in the first order of approximation, thus leading to more accurate surface reconstruction even without the mask supervision. Experiments on the DTU dataset and the BlendedMVS dataset show that NeuS outperforms the state-of-the-arts in high-quality surface reconstruction, especially for objects and scenes with complex structures and self-occlusion.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2106.10689</t>
+  </si>
+  <si>
+    <t>https://github.com/Totoro97/NeuS</t>
+  </si>
+  <si>
+    <t>Volume Rendering of Neural Implicit Surfaces</t>
+  </si>
+  <si>
+    <t>Neural volume rendering became increasingly popular recently due to its success in synthesizing novel views of a scene from a sparse set of input images. So far, the geometry learned by neural volume rendering techniques was modeled using a generic density function. Furthermore, the geometry itself was extracted using an arbitrary level set of the density function leading to a noisy, often low fidelity reconstruction. The goal of this paper is to improve geometry representation and reconstruction in neural volume rendering. We achieve that by modeling the volume density as a function of the geometry. This is in contrast to previous work modeling the geometry as a function of the volume density. In more detail, we define the volume density function as Laplace's cumulative distribution function (CDF) applied to a signed distance function (SDF) representation. This simple density representation has three benefits: (i) it provides a useful inductive bias to the geometry learned in the neural volume rendering process; (ii) it facilitates a bound on the opacity approximation error, leading to an accurate sampling of the viewing ray. Accurate sampling is important to provide a precise coupling of geometry and radiance; and (iii) it allows efficient unsupervised disentanglement of shape and appearance in volume rendering. Applying this new density representation to challenging scene multiview datasets produced high quality geometry reconstructions, outperforming relevant baselines. Furthermore, switching shape and appearance between scenes is possible due to the disentanglement of the two.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2106.12052</t>
+  </si>
+  <si>
+    <t>NerfingMVS: Guided Optimization of Neural Radiance Fields for Indoor Multi-view Stereo</t>
+  </si>
+  <si>
+    <t>In this work, we present a new multi-view depth estimation method that utilizes both conventional SfM reconstruction and learning-based priors over the recently proposed neural radiance fields (NeRF). Unlike existing neural network based optimization method that relies on estimated correspondences, our method directly optimizes over implicit volumes, eliminating the challenging step of matching pixels in indoor scenes. The key to our approach is to utilize the learning-based priors to guide the optimization process of NeRF. Our system firstly adapts a monocular depth network over the target scene by finetuning on its sparse SfM reconstruction. Then, we show that the shape-radiance ambiguity of NeRF still exists in indoor environments and propose to address the issue by employing the adapted depth priors to monitor the sampling process of volume rendering. Finally, a per-pixel confidence map acquired by error computation on the rendered image can be used to further improve the depth quality. Experiments show that our proposed framework significantly outperforms state-of-the-art methods on indoor scenes, with surprising findings presented on the effectiveness of correspondence-based optimization and NeRF-based optimization over the adapted depth priors. In addition, we show that the guided optimization scheme does not sacrifice the original synthesis capability of neural radiance fields, improving the rendering quality on both seen and novel views.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2109.01129</t>
+  </si>
+  <si>
+    <t>https://github.com/weiyithu/NerfingMVS</t>
+  </si>
+  <si>
+    <t>3D Neural Scene Representations for Visuomotor Control</t>
+  </si>
+  <si>
+    <t>CoRL2021(oral)</t>
+  </si>
+  <si>
+    <t>Humans have a strong intuitive understanding of the 3D environment around us. The mental model of the physics in our brain applies to objects of different materials and enables us to perform a wide range of manipulation tasks that are far beyond the reach of current robots. In this work, we desire to learn models for dynamic 3D scenes purely from 2D visual observations. Our model combines Neural Radiance Fields (NeRF) and time contrastive learning with an autoencoding framework, which learns viewpoint-invariant 3D-aware scene representations. We show that a dynamics model, constructed over the learned representation space, enables visuomotor control for challenging manipulation tasks involving both rigid bodies and fluids, where the target is specified in a viewpoint different from what the robot operates on. When coupled with an auto-decoding framework, it can even support goal specification from camera viewpoints that are outside the training distribution. We further demonstrate the richness of the learned 3D dynamics model by performing future prediction and novel view synthesis. Finally, we provide detailed ablation studies regarding different system designs and qualitative analysis of the learned representations.</t>
+  </si>
+  <si>
+    <t>https://3d-representation-learning.github.io/nerf-dy/</t>
+  </si>
+  <si>
+    <t>Vision-Only Robot Navigation in a Neural Radiance World</t>
+  </si>
+  <si>
+    <t>Neural Radiance Fields (NeRFs) have recently emerged as a powerful paradigm for the representation of natural, complex 3D scenes. NeRFs represent continuous volumetric density and RGB values in a neural network, and generate photo-realistic images from unseen camera viewpoints through ray tracing. We propose an algorithm for navigating a robot through a 3D environment represented as a NeRF using only an on-board RGB camera for localization. We assume the NeRF for the scene has been pre-trained offline, and the robot's objective is to navigate through unoccupied space in the NeRF to reach a goal pose. We introduce a trajectory optimization algorithm that avoids collisions with high-density regions in the NeRF based on a discrete time version of differential flatness that is amenable to constraining the robot's full pose and control inputs. We also introduce an optimization based filtering method to estimate 6DoF pose and velocities for the robot in the NeRF given only an onboard RGB camera. We combine the trajectory planner with the pose filter in an online replanning loop to give a vision-based robot navigation pipeline. We present simulation results with a quadrotor robot navigating through a jungle gym environment, the inside of a church, and Stonehenge using only an RGB camera. We also demonstrate an omnidirectional ground robot navigating through the church, requiring it to reorient to fit through the narrow gap. Videos of this work can be found at this https URL .</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2110.00168</t>
+  </si>
+  <si>
+    <t>We follow an adversarial learning framework, where the generator models scenes via their radiance field, and the discriminator attempts to distinguish between images rendered from those radiance fields and images of real scenes. Conceptually, our model decomposes the radiance field of a scene into many small local radiance fields that result from conditioning on a 2D grid of latent codes W. W can be interpreted as a latent floorplan representing the scene.</t>
+  </si>
+  <si>
+    <t>We present DietNeRF, a 3D neural scene representation estimated from a few images. Neural Radiance Fields (NeRF) learn a continuous volumetric representation of a scene through multi-view consistency, and can be rendered from novel viewpoints by ray casting. While NeRF has an impressive ability to reconstruct geometry and fine details given many images, up to 100 for challenging 360° scenes, it often finds a degenerate solution to its image reconstruction objective when only a few input views are available. To improve few-shot quality, we propose DietNeRF. We introduce an auxiliary semantic consistency loss that encourages realistic renderings at novel poses. DietNeRF is trained on individual scenes to (1) correctly render given input views from the same pose, and (2) match high-level semantic attributes across different, random poses. Our semantic loss allows us to supervise DietNeRF from arbitrary poses. We extract these semantics using a pre-trained visual encoder such as CLIP, a Vision Transformer trained on hundreds of millions of diverse single-view, 2D photographs mined from the web with natural language supervision. In experiments, DietNeRF improves the perceptual quality of few-shot view synthesis when learned from scratch, can render novel views with as few as one observed image when pre-trained on a multi-view dataset, and produces plausible completions of completely unobserved regions.</t>
+  </si>
+  <si>
+    <t>Considering the problem of novel view synthesis (NVS) from only a set of 2D images, we simplify the training process of Neural Radiance Field (NeRF) on forward-facing scenes by removing the requirement of known or pre-computed camera parameters, including both intrinsics and 6DoF poses. To this end, we propose NeRF−−, with three contributions: First, we show that the camera parameters can be jointly optimised as learnable parameters with NeRF training, through a photometric reconstruction; Second, to benchmark the camera parameter estimation and the quality of novel view renderings, we introduce a new dataset of path-traced synthetic scenes, termed as Blender Forward-Facing Dataset (BLEFF); Third, we conduct extensive analyses to understand the training behaviours under various camera motions, and show that in most scenarios, the joint optimisation pipeline can recover accurate camera parameters and achieve comparable novel view synthesis quality as those trained with COLMAP pre-computed camera parameters.</t>
+  </si>
+  <si>
+    <t>DeRF：分解的辐射场</t>
+  </si>
+  <si>
+    <t>DONeRF：使用 Depth Oracle Networks 实现紧凑神经辐射场的实时渲染</t>
+  </si>
+  <si>
+    <t>FastNeRF：200FPS 的高保真神经渲染</t>
+  </si>
+  <si>
+    <t>KiloNeRF：使用数千个微型 MLP 加速神经辐射场</t>
+  </si>
+  <si>
+    <t>用于实时渲染神经辐射场的 PlenOctrees</t>
+  </si>
+  <si>
+    <t>用于高效神经渲染的体积基元混合</t>
+  </si>
+  <si>
+    <t>光场网络：具有单次评估渲染的神经场景表示</t>
+  </si>
+  <si>
+    <t>深度监督的 NeRF：更少的视图和更快的免费训练</t>
+  </si>
+  <si>
+    <t>直接体素网格优化：辐射场重建的超快速收敛</t>
+  </si>
+  <si>
+    <t>野外的 NeRF：无约束照片集的神经辐射场</t>
+  </si>
+  <si>
+    <t>Ha-NeRF：野外的幻觉神经辐射场</t>
+  </si>
+  <si>
+    <t>Nerfies：可变形的神经辐射场</t>
+  </si>
+  <si>
+    <t>D-NeRF：动态场景的神经辐射场</t>
+  </si>
+  <si>
+    <t>用于单目 4D 面部头像重建的动态神经辐射场</t>
+  </si>
+  <si>
+    <t>非刚性神经辐射场：单目视频变形场景的重建和新视图合成，</t>
+  </si>
+  <si>
+    <t>PVA：像素对齐的体积化身</t>
+  </si>
+  <si>
+    <t>神经关节辐射场</t>
+  </si>
+  <si>
+    <t>CLA-NeRF：类别级关节神经辐射场</t>
+  </si>
+  <si>
+    <t>用于人体建模的动画神经辐射场</t>
+  </si>
+  <si>
+    <t>神经演员：具有姿势控制的人类演员的神经自由视图合成</t>
+  </si>
+  <si>
+    <t>用于动态场景时空视图合成的神经场景流场</t>
+  </si>
+  <si>
+    <t>神经体：具有结构化潜在代码的隐式神经表示，用于动态人类的新视图合成</t>
+  </si>
+  <si>
+    <t>来自多视图视频的神经 3D 视频合成</t>
+  </si>
+  <si>
+    <t>动态单目视频的动态视图合成</t>
+  </si>
+  <si>
+    <t>GRAF：用于 3D 感知图像合成的生成辐射场</t>
+  </si>
+  <si>
+    <t>GRF：学习用于 3D 场景表示和渲染的一般辐射场</t>
+  </si>
+  <si>
+    <t>pixelNeRF：来自一个或几个图像的神经辐射场</t>
+  </si>
+  <si>
+    <t>用于优化基于坐标的神经表示的学习初始化</t>
+  </si>
+  <si>
+    <t>pi-GAN：用于 3D 感知图像合成的周期性隐式生成对抗网络</t>
+  </si>
+  <si>
+    <t>单张图像的人像神经辐射场</t>
+  </si>
+  <si>
+    <t>ShaRF：单一视图的形状条件辐射场</t>
+  </si>
+  <si>
+    <t>IBRNet：学习基于图像的多视图渲染</t>
+  </si>
+  <si>
+    <t>CAMPARI：相机感知分解生成神经辐射场</t>
+  </si>
+  <si>
+    <t>NeRF-VAE：几何感知 3D 场景生成模型</t>
+  </si>
+  <si>
+    <t>具有局部条件辐射场的无约束场景生成</t>
+  </si>
+  <si>
+    <t>MVSNeRF：从多视图立体快速概括辐射场重建</t>
+  </si>
+  <si>
+    <t>立体辐射场 (SRF)：从新场景的稀疏视图中学习视图合成</t>
+  </si>
+  <si>
+    <t>用于遮挡感知的基于图像的渲染的神经射线</t>
+  </si>
+  <si>
+    <t>节食 NeRF：语义一致的 Few-Shot 视图合成</t>
+  </si>
+  <si>
+    <t>使用 NeRF 实现新视图合成的连续深度 MPI</t>
+  </si>
+  <si>
+    <t>TöRF：动态场景视图合成的飞行时间辐射场</t>
+  </si>
+  <si>
+    <t>CodeNeRF：对象类别的解开神经辐射场</t>
+  </si>
+  <si>
+    <t>StyleNeRF：用于高分辨率图像合成的基于样式的 3D 感知生成器</t>
+  </si>
+  <si>
+    <t>黑暗中的 NeRF：来自嘈杂原始图像的高动态范围视图合成</t>
+  </si>
+  <si>
+    <t>iNeRF：用于姿势估计的反转神经辐射场</t>
+  </si>
+  <si>
+    <t>A-NeRF：通过神经渲染进行无表面人体 3D 姿势细化</t>
+  </si>
+  <si>
+    <t>NeRF--：没有已知相机参数的神经辐射场</t>
+  </si>
+  <si>
+    <t>实时隐式映射和定位</t>
+  </si>
+  <si>
+    <t>用于 SLAM 的 NICE-SLAM 神经隐​​式可扩展编码</t>
+  </si>
+  <si>
+    <t>GNeRF：基于 GAN 的无姿势相机的神经辐射场</t>
+  </si>
+  <si>
+    <t>BARF：捆绑调整神经辐射场</t>
+  </si>
+  <si>
+    <t>自校准神经辐射场</t>
+  </si>
+  <si>
+    <t>NeRD：来自图像集合的神经反射分解</t>
+  </si>
+  <si>
+    <t>NeRV：用于重新照明和视图合成的神经反射率和可见性场</t>
+  </si>
+  <si>
+    <t>NeX：具有神经基础扩展的实时视图合成</t>
+  </si>
+  <si>
+    <t>NeRFactor：未知光照下形状和反射率的神经分解</t>
+  </si>
+  <si>
+    <t>NeRF++：分析和改进神经辐射场</t>
+  </si>
+  <si>
+    <t>GIRAFFE：将场景表示为合成生成神经特征场</t>
+  </si>
+  <si>
+    <t>以对象为中心的神经场景渲染</t>
+  </si>
+  <si>
+    <t>学习动态人头的组成辐射场</t>
+  </si>
+  <si>
+    <t>动态场景的神经场景图</t>
+  </si>
+  <si>
+    <t>物体辐射场的无监督发现</t>
+  </si>
+  <si>
+    <t>学习用于可编辑场景渲染的对象组合神经辐射场</t>
+  </si>
+  <si>
+    <t>使用隐式场景表示进行就地场景标记和理解</t>
+  </si>
+  <si>
+    <t>编辑条件辐射场</t>
+  </si>
+  <si>
+    <t>使用分层神经表示的可编辑自由视点视频</t>
+  </si>
+  <si>
+    <t>Fig-NeRF：用于 3D 对象类别建模的图地面神经辐射场</t>
+  </si>
+  <si>
+    <t>NeRF-Tex：神经反射场纹理</t>
+  </si>
+  <si>
+    <t>Mip-NeRF：抗锯齿神经辐射场的多尺度表示</t>
+  </si>
+  <si>
+    <t>UNISURF：统一神经隐式表面和辐射场以进行多视图重建</t>
+  </si>
+  <si>
+    <t>NeuS：通过体渲染学习神经隐式表面以进行多视图重建</t>
+  </si>
+  <si>
+    <t>神经隐式表面的体积渲染</t>
+  </si>
+  <si>
+    <t>NerfingMVS：室内多视角立体神经辐射场的引导优化</t>
+  </si>
+  <si>
+    <t>用于视觉运动控制的 3D 神经场景表示</t>
+  </si>
+  <si>
+    <t>神经辐射世界中的仅视觉机器人导航</t>
+  </si>
+  <si>
+    <t>随着神经辐射场 (NeRF) 的出现，神经网络现在可以渲染 3D 场景的新颖视图，其质量足以愚弄人眼。然而，生成这些图像的计算量非常大，限制了它们在实际场景中的适用性。在本文中，我们提出了一种基于空间分解的技术，能够缓解这个问题。我们的主要观察结果是，使用更大（更深和/或更宽）的网络会带来收益递减。因此，我们建议对场景进行空间分解，并为每个分解部分分配更小的网络。当一起工作时，这些网络可以渲染整个场景。这使我们无论分解部分的数量如何，都能获得近乎恒定的推理时间。此外，我们表明，Voronoi 空间分解更适合此目的，因为它可证明与 Painter 算法兼容，可实现高效且 GPU 友好的渲染。我们的实验表明，对于现实世界的场景，我们的方法提供的推理效率比 NeRF 高出 3 倍（具有相同的渲染质量），或者 PSNR 提高了 1.0~dB（对于相同的推理成本）。</t>
+  </si>
+  <si>
+    <t>最近围绕神经辐射场 (NeRFs) 的研究爆炸表明，在神经网络中隐式存储场景和照明信息具有巨大的潜力，例如，用于生成新的视图。然而，阻止 NeRF 广泛使用的一个主要限制是沿每个视图射线进行过多网络评估的计算成本过高，当针对当前设备上的实时渲染时需要数十 petaFLOPS。我们表明，当将局部样本放置在场景中的表面周围时，可以显着减少每个视图光线所需的样本数量。为此，我们提出了一个深度预言网络，它通过单个网络评估来预测每个视图光线的光线样本位置。我们表明，使用围绕对数离散和球面扭曲深度值的分类网络对于编码表面位置而不是直接估计深度至关重要。这些技术的结合产生了 DONeRF，这是一种双网络设计，第一步是深度预言网络，以及用于光线累积的局部采样着色网络。通过我们的设计，与 NeRF 相比，我们将推理成本降低了 48 倍。使用现成的推理 API 与简单的计算内核相结合，我们率先在单个 GPU 上以交互式帧速率（每秒 15 帧，800x800）渲染基于光线追踪的神经表示。同时，由于我们专注于表面周围场景的重要部分，与 NeRF 相比，我们获得了相同或更好的质量。</t>
+  </si>
+  <si>
+    <t>最近关于神经辐射场 (NeRF) 的工作展示了如何使用神经网络对复杂的 3D 环境进行编码，这些环境可以从新颖的视角进行逼真的渲染。渲染这些图像对计算的要求非常高，最近的改进距离实现交互速率还有很长的路要走，即使在高端硬件上也是如此。受移动和混合现实设备场景的启发，我们提出了 FastNeRF，这是第一个基于 NeRF 的系统，能够在高端消费 GPU 上以 200Hz 渲染高保真逼真图像。我们方法的核心是受图形启发的分解，它允许 (i) 在空间中的每个位置紧凑地缓存深度辐射图，(ii) 使用光线方向有效地查询该图以估计渲染图像中的像素值。大量实验表明，所提出的方法比原始的 NeRF 算法快 3000 倍，并且比现有的加速 NeRF 的工作至少快一个数量级，同时保持视觉质量和可扩展性。</t>
+  </si>
+  <si>
+    <t>NeRF 通过将神经辐射场拟合到 RGB 图像，以前所未有的质量合成场景的新视图。然而，NeRF 需要数百万次查询深度多层感知器 (MLP)，导致渲染时间变慢，即使在现代 GPU 上也是如此。在本文中，我们证明了通过使用数千个微型 MLP 而不是一个大型 MLP，实时渲染是可能的。在我们的设置中，每个单独的 MLP 只需要表示场景的一部分，因此可以使用更小、更快评估的 MLP。通过将这种分而治之的策略与进一步的优化相结合，与原始 NeRF 模型相比，渲染速度提高了三个数量级，而不会产生高昂的存储成本。此外，使用师生蒸馏进行培训，我们表明可以在不牺牲视觉质量的情况下实现这种加速。</t>
+  </si>
+  <si>
+    <t>实时性能是通过将 NeRF 预先制成基于八叉树的辐射场（我们称为 PlenOctrees）来实现的。为了保留与视图相关的效果，例如镜面反射，我们建议通过封闭形式的球面基函数对外观进行编码。具体来说，我们表明可以训练 NeRFs 来预测辐射的球谐表示，将观察方向作为神经网络的输入。此外，我们表明我们的 PlenOctrees 可以直接优化以进一步最小化重建损失，这导致与竞争方法相同或更好的质量。我们进一步表明，这个八叉树优化步骤可用于加快训练时间，因为我们不再需要等待 NeRF 训练完全收敛。我们的实时神经渲染方法可能会支持新的应用，例如 6 自由度工业和产品可视化，以及下一代 AR/VR 系统。</t>
+  </si>
+  <si>
+    <t>人类的实时渲染和动画是游戏、电影和远程呈现应用中的核心功能。现有方法有许多我们的工作旨在解决的缺点。三角形网格难以建模像头发这样的细结构，像神经体积这样的体积表示在合理的内存预算下分辨率太低，而像神经辐射场这样的高分辨率隐式表示在实时应用中使用太慢。我们提出了体积基元混合（MVP），一种用于渲染动态 3D 内容的表示，它结合了体积表示的完整性和基于基元的渲染的效率，例如，基于点或基于网格的方法。我们的方法通过利用具有反卷积架构的空间共享计算以及通过使用可以移动以仅覆盖被占用区域的体积基元来最小化空间空白区域中的计算来实现这一点。我们的参数化支持对应和跟踪约束的集成，同时对经典跟踪失败的区域具有鲁棒性，例如薄或半透明结构周围以及具有大拓扑可变性的区域。 MVP 是一种混合体，它概括了基于体积和基元的表示。通过一系列广泛的实验，我们证明它继承了每种方法的优点，同时避免了它们的许多局限性。我们还将我们的方法与几种最先进的方法进行比较，并证明 MVP 在质量和运行时性能方面产生了卓越的结果。</t>
+  </si>
+  <si>
+    <t>从 2D 观察推断 3D 场景的表示是计算机图形学、计算机视觉和人工智能的基本问题。新兴的 3D 结构神经场景表示是一种有前途的 3D 场景理解方法。在这项工作中，我们提出了一种新的神经场景表示，光场网络或 LFN，它通过神经隐式表示在 360 度、四维光场中表示底层 3D 场景的几何形状和外观。渲染来自 LFN 的光线只需要*单个*网络评估，而 3D 结构化神经场景表示中的光线行进或基于体积的渲染器每条光线需要数百次评估。在简单场景的设置中，我们利用元学习来学习 LFN 的先验，从而能够从单个图像观察中进行多视图一致的光场重建。这导致时间和内存复杂性的显着降低，并实现了实时渲染。通过 LFN 存储 360 度光场的成本比 Lumigraph 等传统方法低两个数量级。利用神经隐式表示的分析可微性和光空间的新参数化，我们进一步证明了从 LFN 中提取稀疏深度图。</t>
+  </si>
+  <si>
+    <t>当输入视图数量不足时，通常观察到的神经辐射场 (NeRF) 故障模式会拟合不正确的几何形状。一个潜在的原因是标准体积渲染不会强制执行大多数场景几何体由空白空间和不透明表面组成的约束。我们通过 DS-NeRF（深度监督神经辐射场）将上述假设形式化，这是一种利用现成的深度监督学习辐射场的损失。我们利用当前的 NeRF 管道需要具有已知相机姿势的图像这一事实，这些图像通常通过运行从运动结构 (SFM) 来估计。至关重要的是，SFM 还产生稀疏 3D 点，可在训练期间用作“免费”深度监督：我们添加损失以鼓励光线的终止深度分布匹配给定的 3D 关键点，并结合深度不确定性。 DS-NeRF 可以在训练视图更少的情况下渲染更好的图像，同时训练速度提高 2-3 倍。此外，我们表明我们的损失与最近提出的其他 NeRF 方法兼容，证明深度是一种廉价且易于消化的监督信号。最后，我们发现 DS-NeRF 可以支持其他类型的深度监督，例如扫描深度传感器和 RGB-D 重建输出。</t>
+  </si>
+  <si>
+    <t>我们提出了一种超快速收敛方法，用于从一组捕获具有已知姿势的场景的图像中重建每个场景的辐射场。这项任务通常应用于新颖的视图合成，最近因其最先进的质量和灵活性而被神经辐射场 (NeRF) 彻底改变。然而，对于单个场景，NeRF 及其变体需要很长的训练时间，从数小时到数天不等。相比之下，我们的方法实现了与 NeRF 相当的质量，并在不到 15 分钟的时间内使用单个 GPU 从头开始​​快速收敛。我们采用由用于场景几何的密度体素网格和具有浅层网络的特征体素网格组成的表示，用于复杂的依赖于视图的外观。使用显式和离散化的体积表示进行建模并不新鲜，但我们提出了两种简单但非平凡的技术，有助于快速收敛和高质量输出。首先，我们介绍了体素密度的激活后插值，它能够以较低的网格分辨率产生锐利的表面。其次，直接体素密度优化容易出现次优几何解决方案，因此我们通过强加几个先验来加强优化过程。最后，对五个内向基准的评估表明，我们的方法与 NeRF 的质量相匹配，甚至超过，但从头开始训练新场景只需要大约 15 分钟。</t>
+  </si>
+  <si>
+    <t>我们提出了一种基于学习的方法，用于仅使用野外照片的非结构化集合来合成复杂场景的新视图。我们建立在神经辐射场 (NeRF) 的基础上，它使用多层感知器的权重将场景的密度和颜色建模为 3D 坐标的函数。虽然 NeRF 在受控设置下捕获的静态对象的图像上效果很好，但它无法在不受控的图像中模拟许多普遍存在的真实世界现象，例如可变照明或瞬态遮挡物。我们为 NeRF 引入了一系列扩展来解决这些问题，从而能够从互联网上获取的非结构化图像集合中进行准确的重建。我们将我们的系统（称为 NeRF-W）应用于著名地标的互联网照片集，并展示时间一致的新颖视图渲染，这些渲染比现有技术更接近真实感。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 最近因其令人印象深刻的新颖视图合成能力而广受欢迎。本文研究了幻觉 NeRF 的问题：即在一天中的不同时间从一组旅游图像中恢复一个真实的 NeRF。现有的解决方案采用具有可控外观嵌入的 NeRF 在各种条件下渲染新颖的视图，但它们无法渲染具有看不见的外观的视图一致图像。为了解决这个问题，我们提出了一个用于构建幻觉 NeRF 的端到端框架，称为 Ha-NeRF。具体来说，我们提出了一个外观幻觉模块来处理随时间变化的外观并将它们转移到新的视图中。考虑到旅游图像的复杂遮挡，我们引入了一个反遮挡模块来准确地分解静态主体以获得可见性。合成数据和真实旅游照片集的实验结果表明，我们的方法可以产生幻觉，并从不同的视图呈现无遮挡的图像。</t>
+  </si>
+  <si>
+    <t>我们提出了第一种能够使用从手机随便捕获的照片/视频来逼真地重建可变形场景的方法。我们的方法通过优化一个额外的连续体积变形场来增强神经辐射场 (NeRF)，该场将每个观察点扭曲成一个规范的 5D NeRF。我们观察到这些类似 NeRF 的变形场容易出现局部最小值，并为基于坐标的模型提出了一种从粗到细的优化方法，可以实现更稳健的优化。通过将几何处理和物理模拟的原理应用于类似 NeRF 的模型，我们提出了变形场的弹性正则化，进一步提高了鲁棒性。我们表明，我们的方法可以将随意捕获的自拍照片/视频转换为可变形的 NeRF 模型，允许从任意视角对主体进行逼真的渲染，我们称之为“nerfies”。我们通过使用带有两部手机的装备收集时间同步数据来评估我们的方法，从而在不同视点产生相同姿势的训练/验证图像。我们表明，我们的方法忠实地重建了非刚性变形的场景，并以高保真度再现了看不见的视图。</t>
+  </si>
+  <si>
+    <t>将机器学习与几何推理相结合的神经渲染技术已成为从一组稀疏图像中合成场景新视图的最有前途的方法之一。其中，神经辐射场 (NeRF) 尤为突出，它训练深度网络将 5D 输入坐标（表示空间位置和观察方向）映射为体积密度和与视图相关的发射辐射。然而，尽管在生成的图像上实现了前所未有的真实感水平，但 NeRF 仅适用于静态场景，其中可以从不同的图像中查询相同的空间位置。在本文中，我们介绍了 D-NeRF，这是一种将神经辐射场扩展到动态域的方法，允许在场景中移动的 \emph{single} 相机的刚性和非刚性运动下重建和渲染物体的新图像。为此，我们将时间视为系统的附加输入，并将学习过程分为两个主要阶段：一个将场景编码为规范空间，另一个将这个规范表示映射到特定时间的变形场景。两种映射都是使用全连接网络同时学习的。一旦网络经过训练，D-NeRF 就可以渲染新颖的图像，同时控制相机视图和时间变量，从而控制对象的移动。我们展示了我们的方法在物体处​​于刚性、关节和非刚性运动的场景中的有效性。代码、模型权重和动态场景数据集将发布。</t>
+  </si>
+  <si>
+    <t>我们提出了用于模拟人脸外观和动态的动态神经辐射场。对说话的人进行数字建模和重建是各种应用程序的关键组成部分。特别是对于 AR 或 VR 中的远程呈现应用，需要忠实再现外观，包括新颖的视点或头部姿势。与显式建模几何和材料属性或纯粹基于图像的最先进方法相比，我们引入了基于场景表示网络的头部隐式表示。为了处理面部的动态，我们将场景表示网络与低维可变形模型相结合，该模型提供对姿势和表情的显式控制。我们使用体积渲染从这种混合表示中生成图像，并证明这种动态神经场景表示只能从单目输入数据中学习，而不需要专门的捕获设置。在我们的实验中，我们表明这种学习的体积表示允许生成照片般逼真的图像，其质量超过了基于视频的最先进的重演方法的质量。</t>
+  </si>
+  <si>
+    <t>我们提出了非刚性神经辐射场 (NR-NeRF)，这是一种用于一般非刚性动态场景的重建和新颖的视图合成方法。我们的方法将动态场景的 RGB 图像作为输入（例如，来自单目视频记录），并创建高质量的时空几何和外观表示。我们表明，单个手持消费级相机足以从新颖的虚拟相机视图合成动态场景的复杂渲染，例如一个“子弹时间”的视频效果。 NR-NeRF 将动态场景分解为规范体积及其变形。场景变形被实现为光线弯曲，其中直线光线被非刚性变形。我们还提出了一种新的刚性网络来更好地约束场景的刚性区域，从而获得更稳定的结果。射线弯曲和刚性网络在没有明确监督的情况下进行训练。我们的公式可以实现跨视图和时间的密集对应估计，以及引人注目的视频编辑应用程序，例如运动夸张。我们的代码将是开源的。</t>
+  </si>
+  <si>
+    <t>逼真的人头的采集和渲染是一个极具挑战性的研究问题，对于虚拟远程呈现特别重要。目前，最高质量是通过在多视图数据上以个人特定方式训练的体积方法实现的。与更简单的基于网格的模型相比，这些模型更好地表示精细结构，例如头发。体积模型通常使用全局代码来表示面部表情，以便它们可以由一小组动画参数驱动。虽然这样的架构实现了令人印象深刻的渲染质量，但它们不能轻易地扩展到多身份设置。在本文中，我们设计了一种新颖的方法，用于在仅给定少量输入的情况下预测人头的体积化身。我们通过一种新颖的参数化实现跨身份的泛化，该参数化将神经辐射场与直接从输入中提取的局部像素对齐特征相结合，从而避免了对非常深或复杂网络的需求。我们的方法仅基于光度重新渲染损失以端到端的方式进行训练，无需明确的 3D 监督。我们证明我们的方法在质量方面优于现有的现有技术，并且能够生成忠实的面部表情多身份设置。</t>
+  </si>
+  <si>
+    <t>我们提出了神经关节辐射场 (NARF)，这是一种新颖的可变形 3D 表示，用于从图像中学习到的关节对象。虽然 3D 隐式表示的最新进展使得学习复杂对象的模型成为可能，但学习关节对象的姿势可控表示仍然是一个挑战，因为当前的方法需要 3D 形状监督并且无法呈现外观。在制定 3D 关节对象的隐式表示时，我们的方法在求解每个 3D 位置的辐射场时仅考虑最相关对象部分的刚性变换。通过这种方式，所提出的方法可以表示与姿势相关的变化，而不会显着增加计算复杂度。 NARF 是完全可微的，可以从带有姿势注释的图像中训练出来。此外，通过使用自动编码器，它可以学习对象类的多个实例的外观变化。实验表明，所提出的方法是有效的，并且可以很好地推广到新的姿势。</t>
+  </si>
+  <si>
+    <t>我们提出了 CLA-NeRF——一种类别级的关节神经辐射场，可以执行视图合成、部分分割和关节姿态估计。 CLA-NeRF 在对象类别级别进行训练，不使用 CAD 模型和深度，而是使用一组具有地面实况相机姿势和部分片段的 RGB 图像。在推理过程中，只需对已知类别中未见过的 3D 对象实例进行少量 RGB 视图（即少镜头）即可推断对象部分分割和神经辐射场。给定一个关节姿态作为输入，CLA-NeRF 可以执行关节感知体积渲染，以在任何相机姿态下生成相应的 RGB 图像。此外，可以通过逆向渲染来估计对象的关节姿势。在我们的实验中，我们对合成数据和真实数据的五个类别的框架进行了评估。在所有情况下，我们的方法都显示了真实的变形结果和准确的关节姿态估计。我们相信，少量的关节对象渲染和关节姿势估计都为机器人感知和与看不见的关节对象交互打开了大门。</t>
+  </si>
+  <si>
+    <t>本文解决了从多视图视频中重建可动画人体模型的挑战。最近的一些工作提出将非刚性变形场景分解为规范神经辐射场和一组将观察空间点映射到规范空间的变形场，从而使他们能够从图像中学习动态场景。然而，它们将变形场表示为平移矢量场或 SE(3) 场，这使得优化受到高度约束。此外，这些表示不能由输入运动明确控制。相反，我们引入了神经混合权重场来产生变形场。基于骨架驱动的变形，混合权重场与 3D 人体骨骼一起使用，以生成观察到规范和规范到观察的对应关系。由于 3D 人体骨骼更易观察，它们可以规范变形场的学习。此外，学习到的混合权重场可以与输入的骨骼运动相结合，以生成新的变形场来为人体模型设置动画。实验表明，我们的方法明显优于最近的人类合成方法。该代码将在 https://zju3dv.github.io/animatable_nerf/ 上提供。</t>
+  </si>
+  <si>
+    <t>我们提出了神经演员 (NA)，这是一种从任意视角和任意可控姿势下高质量合成人类的新方法。我们的方法建立在最近的神经场景表示和渲染工作之上，这些工作仅从 2D 图像中学习几何和外观的表示。虽然现有作品展示了令人信服的静态场景渲染和动态场景回放，但使用神经隐式方法对人类进行逼真的重建和渲染，特别是在用户控制的新姿势下，仍然很困难。为了解决这个问题，我们利用粗体模型作为代理将周围的 3D 空间展开为规范姿势。神经辐射场从多视图视频输入中学习规范空间中与姿势相关的几何变形以及与姿势和视图相关的外观效果。为了合成高保真动态几何和外观的新视图，我们利用在身体模型上定义的 2D 纹理图作为潜在变量来预测残余变形和动态外观。实验表明，我们的方法在回放和新颖的姿势合成方面取得了比现有技术更好的质量，甚至可以很好地推广到与训练姿势截然不同的新姿势。此外，我们的方法还支持合成结果的体形控制。</t>
+  </si>
+  <si>
+    <t>我们提出了一种方法来执行动态场景的新颖视图和时间合成，只需要具有已知相机姿势的单目视频作为输入。为此，我们引入了神经场景流场，这是一种将动态场景建模为外观、几何和 3D 场景运动的时变连续函数的新表示。我们的表示通过神经网络进行优化，以适应观察到的输入视图。我们表明，我们的表示可用于复杂的动态场景，包括薄结构、视图相关效果和自然运动度。我们进行了许多实验，证明我们的方法明显优于最近的单目视图合成方法，并展示了各种真实世界视频的时空视图合成的定性结果。</t>
+  </si>
+  <si>
+    <t>本文解决了人类表演者从一组非常稀疏的摄像机视图中合成新颖视图的挑战。最近的一些工作表明，在给定密集输入视图的情况下，学习 3D 场景的隐式神经表示可以实现显着的视图合成质量。但是，如果视图高度稀疏，则表示学习将是不适定的。为了解决这个不适定问题，我们的关键思想是整合对视频帧的观察。为此，我们提出了神经体，这是一种新的人体表示，它假设在不同帧上学习到的神经表示共享同一组锚定到可变形网格的潜在代码，以便可以自然地整合跨帧的观察结果。可变形网格还为网络提供几何指导，以更有效地学习 3D 表示。为了评估我们的方法，我们创建了一个名为 ZJU-MoCap 的多视图数据集，用于捕捉具有复杂动作的表演者。 ZJU-MoCap 的实验表明，我们的方法在新颖的视图合成质量方面大大优于先前的工作。我们还展示了我们的方法从 People-Snapshot 数据集上的单目视频重建移动人物的能力。</t>
+  </si>
+  <si>
+    <t>我们提出了一种新颖的 3D 视频合成方法，能够以紧凑但富有表现力的表示形式表示动态真实世界场景的多视图视频记录，从而实现高质量的视图合成和运动插值。我们的方法将静态神经辐射场的高质量和紧凑性带到了一个新的方向：无模型的动态设置。我们方法的核心是一种新颖的时间条件神经辐射场，它使用一组紧凑的潜在代码来表示场景动态。为了利用视频相邻帧之间的变化通常很小且局部一致的事实，我们提出了两种有效训练神经网络的新策略：1）有效的分层训练方案，以及 2）选择根据输入视频的时间变化进行训练的下一条光线。结合起来，这两种策略显着提高了训练速度，导致训练过程快速收敛，并获得高质量的结果。我们学习的表示非常紧凑，能够表示由 18 个摄像机录制的 10 秒 30 FPS 多视图视频，模型大小仅为 28MB。我们证明了我们的方法可以以超过 1K 的分辨率渲染高保真广角新颖视图，即使对于高度复杂和动态的场景也是如此。我们进行了广泛的定性和定量评估，表明我们的方法优于当前的技术水平。项目网站：https://neural-3d-video.github.io。</t>
+  </si>
+  <si>
+    <t>我们提出了一种算法，用于在给定动态场景的单目视频的任意视点和任何输入时间步长处生成新视图。我们的工作建立在神经隐式表示的最新进展的基础上，并使用连续和可微的函数来建模时变结构和场景的外观。我们联合训练一个时不变的静态 NeRF 和一个时变的动态 NeRF，并学习如何以无监督的方式混合结果。然而，从单个视频中学习这个隐式函数是非常不适定的（与输入视频匹配的解决方案有无限多）。为了解决歧义，我们引入了正则化损失以鼓励更合理的解决方案。我们展示了从随意捕获的视频中进行动态视图合成的广泛定量和定性结果。</t>
+  </si>
+  <si>
+    <t>虽然 2D 生成对抗网络已经实现了高分辨率图像合成，但它们在很大程度上缺乏对 3D 世界和图像形成过程的理解。因此，它们不提供对相机视点或物体姿势的精确控制。为了解决这个问题，最近的几种方法将基于中间体素的表示与可微渲染相结合。然而，现有方法要么产生低图像分辨率，要么在解开相机和场景属性方面存在不足，例如，对象身份可能随视点而变化。在本文中，我们提出了一种辐射场的生成模型，该模型最近被证明在单个场景的新颖视图合成方面是成功的。与基于体素的表示相比，辐射场并不局限于 3D 空间的粗略离散化，还允许解开相机和场景属性，同时在存在重建模糊性的情况下优雅地退化。通过引入基于多尺度补丁的鉴别器，我们展示了高分辨率图像的合成，同时仅从未定位的 2D 图像训练我们的模型。我们系统地分析了我们在几个具有挑战性的合成和现实世界数据集上的方法。我们的实验表明，辐射场是生成图像合成的强大表示，可生成以高保真度渲染的 3D 一致模型。</t>
+  </si>
+  <si>
+    <t>我们提出了一个简单而强大的神经网络，它仅从 2D 观察中隐式表示和渲染 3D 对象和场景。该网络将 3D 几何建模为一般辐射场，它以一组具有相机位姿和内在函数的 2D 图像作为输入，为 3D 空间的每个点构建内部表示，然后渲染该点的相应外观和几何观察从任意位置。我们方法的关键是学习 2D 图像中每个像素的局部特征，然后将这些特征投影到 3D 点，从而产生一般和丰富的点表示。我们还集成了一种注意力机制来聚合来自多个 2D 视图的像素特征，从而隐式考虑视觉遮挡。大量实验表明，我们的方法可以为新物体、看不见的类别和具有挑战性的现实世界场景生成高质量和逼真的新视图。</t>
+  </si>
+  <si>
+    <t>我们提出了 pixelNeRF，这是一种学习框架，可以预测以一个或几个输入图像为条件的连续神经场景表示。构建神经辐射场的现有方法涉及独立优化每个场景的表示，需要许多校准视图和大量计算时间。我们通过引入一种以完全卷积方式在图像输入上调节 NeRF 的架构，朝着解决这些缺点迈出了一步。这允许网络在多个场景中进行训练，以先学习一个场景，使其能够从一组稀疏的视图（少至一个）以前馈方式执行新颖的视图合成。利用 NeRF 的体积渲染方法，我们的模型可以直接从图像中训练，无需明确的 3D 监督。我们在 ShapeNet 基准上进行了广泛的实验，用于具有保留对象以及整个未见类别的单图像新颖视图合成任务。我们通过在多对象 ShapeNet 场景和来自 DTU 数据集的真实场景上展示 pixelNeRF 的灵活性，进一步展示了它的灵活性。在所有情况下，对于新颖的视图合成和单图像 3D 重建，pixelNeRF 都优于当前最先进的基线。有关视频和代码，请访问项目网站：此 https 网址</t>
+  </si>
+  <si>
+    <t>基于坐标的神经表示已显示出作为复杂低维信号的离散、基于数组的表示的替代方案的重要前景。然而，从每个新信号的随机初始化权重优化基于坐标的网络是低效的。我们建议应用标准的元学习算法来学习这些全连接网络的初始权重参数，这些参数基于所表示的底层信号类别（例如，面部图像或椅子的 3D 模型）。尽管只需要在实现中进行微小的更改，但使用这些学习到的初始权重可以在优化过程中实现更快的收敛，并且可以作为所建模信号类的强先验，从而在只有给定信号的部分观察可用时产生更好的泛化。我们在各种任务中探索这些好处，包括表示 2D 图像、重建 CT 扫描以及从 2D 图像观察中恢复 3D 形状和场景。</t>
+  </si>
+  <si>
+    <t>我们见证了 3D 感知图像合成的快速进展，利用了生成视觉模型和神经渲染的最新进展。然而，现有方法在两个方面存在不足：首先，它们可能缺乏底层 3D 表示或依赖于视图不一致的渲染，因此合成的图像不是多视图一致的；其次，它们通常依赖于表达能力不足的表示网络架构，因此它们的结果缺乏图像质量。我们提出了一种新颖的生成模型，称为周期性隐式生成对抗网络（π-GAN 或 pi-GAN），用于高质量的 3D 感知图像合成。 π-GAN 利用具有周期性激活函数和体积渲染的神经表示将场景表示为具有精细细节的视图一致的 3D 表示。所提出的方法获得了具有多个真实和合成数据集的 3D 感知图像合成的最新结果。</t>
+  </si>
+  <si>
+    <t>我们提出了一种从单个爆头肖像估计神经辐射场 (NeRF) 的方法。虽然 NeRF 已经展示了高质量的视图合成，但它需要静态场景的多个图像，因此对于随意捕捉和移动主体是不切实际的。在这项工作中，我们建议使用使用灯光舞台肖像数据集的元学习框架来预训练多层感知器 (MLP) 的权重，该多层感知器隐含地对体积密度和颜色进行建模。为了提高对看不见的人脸的泛化能力，我们在由 3D 人脸可变形模型近似的规范坐标空间中训练 MLP。我们使用受控捕获对方法进行定量评估，并展示了对真实肖像图像的泛化性，显示出对最先进技术的有利结果。</t>
+  </si>
+  <si>
+    <t>我们提出了一种方法，用于估计仅给定单个图像的对象的神经场景表示。我们方法的核心是估计物体的几何支架，并将其用作重建底层辐射场的指导。我们的公式基于一个生成过程，该过程首先将潜在代码映射到体素化形状，然后将其渲染为图像，对象外观由第二个潜在代码控制。在推理过程中，我们优化了潜在代码和网络以适应新对象的测试图像。形状和外观的明确解开允许我们的模型在给定单个图像的情况下进行微调。然后，我们可以以几何一致的方式渲染新视图，它们忠实地表示输入对象。此外，我们的方法能够推广到训练域之外的图像（更逼真的渲染甚至真实照片）。最后，推断的几何支架本身就是对物体 3D 形状的准确估计。我们在几个实验中证明了我们的方法在合成图像和真实图像中的有效性。</t>
+  </si>
+  <si>
+    <t>我们提出了一种通过插入一组稀疏的附近视图来合成复杂场景的新视图的方法。我们方法的核心是一个网络架构，其中包括一个多层感知器和一个光线转换器，用于估计连续 5D 位置（3D 空间位置和 2D 观察方向）的辐射和体积密度，从多个源视图动态绘制外观信息。通过在渲染时绘制源视图，我们的方法回归了基于图像的渲染 (IBR) 的经典工作，并允许我们渲染高分辨率图像。与优化每个场景函数以进行渲染的神经场景表示工作不同，我们学习了一种通用视图插值函数，该函数可以推广到新场景。我们使用经典的体渲染来渲染图像，这是完全可微的，并且允许我们仅使用多视图姿势图像作为监督进行训练。实验表明，我们的方法优于最近的新视图合成方法，这些方法也试图推广到新场景。此外，如果在每个场景上进行微调，我们的方法与最先进的单场景神经渲染方法具有竞争力。项目页面：此 https 网址</t>
+  </si>
+  <si>
+    <t>深度生成模型的巨大进步导致了逼真的图像合成。在取得令人信服的结果的同时，大多数方法都在二维图像域中运行，而忽略了我们世界的三维性质。因此，最近的几项工作提出了具有 3D 感知能力的生成模型，即场景以 3D 建模，然后可微分地渲染到图像平面。这导致了令人印象深刻的 3D 一致性，但纳入这种偏差是有代价的：相机也需要建模。当前的方法假定固定的内在函数和预先定义的相机姿势范围。因此，实际数据通常需要参数调整，如果数据分布不匹配，结果会下降。我们的关键假设是，与图像生成器一起学习相机生成器会导致更原则性的 3D 感知图像合成方法。此外，我们建议将场景分解为背景和前景模型，从而实现更有效和更清晰的场景表示。在从原始的、未定型的图像集合中进行训练时，我们学习了一个 3D 和相机感知的生成模型，它不仅忠实地恢复了图像，而且还忠实地恢复了相机数据分布。在测试时，我们的模型生成的图像可以显式控制相机以及场景的形状和外观。</t>
+  </si>
+  <si>
+    <t>我们提出了 NeRF-VAE，这是一种 3D 场景生成模型，它通过 NeRF 和可微体渲染结合了几何结构。与 NeRF 相比，我们的模型考虑了跨场景的共享结构，并且能够使用摊销推理推断新场景的结构——无需重新训练。 NeRF-VAE 的显式 3D 渲染过程进一步将先前的生成模型与缺乏几何结构的基于卷积的渲染进行对比。我们的模型是一个 VAE，它通过在潜在场景表示上调节辐射场来学习辐射场的分布。我们表明，经过训练，NeRF-VAE 能够使用很少的输入图像从以前看不见的 3D 环境中推断和渲染几何一致的场景。我们进一步证明了 NeRF-VAE 可以很好地推广到分布式相机，而卷积模型则不能。最后，我们介绍并研究了 NeRF-VAE 解码器的一种基于注意力的调节机制，该机制提高了模型性能。</t>
+  </si>
+  <si>
+    <t>我们遵循对抗性学习框架，其中生成器通过其辐射场对场景进行建模，鉴别器尝试区分从这些辐射场渲染的图像和真实场景的图像。从概念上讲，我们的模型将场景的辐射场分解为许多小的局部辐射场，这些辐射场是由二维潜在代码 W 网格上的条件产生的。W 可以解释为表示场景的潜在平面图。</t>
+  </si>
+  <si>
+    <t>我们提出了 MVSNeRF，一种新颖的神经渲染方法，可以有效地重建神经辐射场以进行视图合成。与先前的神经辐射场工作考虑对密集捕获的图像进行逐场景优化不同，我们提出了一个通用的深度神经网络，它可以通过快速网络推理仅从三个附近的输入视图重建辐射场。我们的方法利用平面扫描成本体积（广泛用于多视图立体）进行几何感知场景推理，并将其与基于物理的体积渲染相结合用于神经辐射场重建。我们在 DTU 数据集中的真实对象上训练我们的网络，并在三个不同的数据集上对其进行测试，以评估其有效性和普遍性。我们的方法可以跨场景（甚至是室内场景，与我们的对象训练场景完全不同）进行泛化，并仅使用三个输入图像生成逼真的视图合成结果，显着优于可泛化辐射场重建的并行工作。此外，如果捕捉到密集的图像，我们估计的辐射场表示可以很容易地进行微调；与 NeRF 相比，这导致具有更高渲染质量和更短优化时间的快速每场景重建。</t>
+  </si>
+  <si>
+    <t>最近的神经视图合成方法取得了令人印象深刻的质量和真实性，超越了依赖多视图重建的经典管道。最先进的方法，例如 NeRF，旨在使用神经网络学习单个场景，并且需要密集的多视图输入。在新场景上进行测试需要从头开始重新训练，这需要 2-3 天。在这项工作中，我们介绍了立体辐射场 (SRF)，这是一种端到端训练的神经视图合成方法，可以推广到新场景，并且在测试时只需要稀疏视图。核心思想是一种受经典多视图立体方法启发的神经架构，它通过在立体图像中找到相似的图像区域来估计表面点。在 SRF 中，我们预测每个 3D 点的颜色和密度，给定输入图像中立体对应的编码。编码是通过成对相似性的集合隐式学习的——模拟经典立体声。实验表明，SRF 在场景上学习结构而不是过度拟合。我们在 DTU 数据集的多个场景上进行训练，并在不重新训练的情况下推广到新场景，只需要 10 个稀疏和展开的视图作为输入。我们展示了 10-15 分钟的微调进一步改善了结果，与特定场景的模型相比，获得了更清晰、更详细的结果。代码、模型和视频可在此 https 网址上找到。</t>
+  </si>
+  <si>
+    <t>我们提出了一种新的神经表示，称为神经射线 (NeuRay)，用于新的视图合成任务。最近的工作从输入视图的图像特征构建辐射场以渲染新颖的视图图像，从而能够泛化到新场景。但是，由于遮挡，3D 点可能对某些输入视图不可见。在这样的 3D 点上，这些泛化方法将包括来自不可见视图的不一致图像特征，这会干扰辐射场的构建。为了解决这个问题，我们在 NeuRay 表示中预测 3D 点对输入视图的可见性。这种可见性使辐射场构建能够专注于可见图像特征，从而显着提高其渲染质量。同时，提出了一种新颖的一致性损失，以在对特定场景进行微调时改进 NeuRay 中的可见性。实验表明，我们的方法在推广到看不见的场景时在新颖的视图合成任务上实现了最先进的性能，并且在微调后优于每个场景的优化方法。</t>
+  </si>
+  <si>
+    <t>我们提出了 DietNeRF，一种从几张图像估计的 3D 神经场景表示。神经辐射场 (NeRF) 通过多视图一致性学习场景的连续体积表示，并且可以通过光线投射从新颖的视点进行渲染。虽然 NeRF 在给定许多图像的情况下具有令人印象深刻的重建几何和精细细节的能力，对于具有挑战性的 360° 场景最多可重建 100 个，但当只有少数输入视图可用时，它通常会为其图像重建目标找到退化的解决方案。为了提高few-shot质量，我们提出了DietNeRF。我们引入了一种辅助语义一致性损失，它鼓励以新颖的姿势进行逼真的渲染。 DietNeRF 在单个场景上进行训练，以 (1) 从相同的姿势正确渲染给定的输入视图，以及 (2) 在不同的随机姿势中匹配高级语义属性。我们的语义损失使我们能够从任意姿势监督 DietNeRF。我们使用预训练的视觉编码器提取这些语义，例如 CLIP，这是一种视觉转换器，通过自然语言监督从网络挖掘出的数亿张不同的单视图 2D 照片进行训练。在实验中，DietNeRF 在从头开始学习时提高了少镜头视图合成的感知质量，在多视图数据集上进行预训练时，可以用少至一张观察到的图像渲染新视图，并生成完全未观察到的区域的合理完成。</t>
+  </si>
+  <si>
+    <t>在本文中，我们建议 MINE 通过从单个图像进行密集 3D 重建来执行新颖的视图合成和深度估计。我们的方法是通过引入神经辐射场 (NeRF) 对多平面图像 (MPI) 进行连续深度泛化。给定单个图像作为输入，MINE 预测任意深度值的 4 通道图像（RGB 和体积密度）以联合重建相机平截头体并填充被遮挡的内容。然后可以使用可微分渲染轻松地将重建和修复的截锥体渲染为新颖的 RGB 或深度视图。在 RealEstate10K、KITTI 和 Flowers Light Fields 上进行的大量实验表明，我们的 MINE 在新颖的视图合成中大大优于最先进的技术。我们还在 iBims-1 和 NYU-v2 的深度估计方面取得了具有竞争力的结果，而无需注释深度监督。我们的源代码可在此 https 网址获得</t>
+  </si>
+  <si>
+    <t>神经网络可以表示和准确重建静态 3D 场景（例如 NeRF）的辐射场。一些作品将这些扩展到用单目视频捕获的动态场景，并具有可观的性能。然而，众所周知，单眼设置是一个约束不足的问题，因此方法依赖于数据驱动的先验来重建动态内容。我们用飞行时间 (ToF) 相机的测量值替换这些先验，并引入基于连续波 ToF 相机图像形成模型的神经表示。我们不使用处理过的深度图，而是对原始 ToF 传感器测量进行建模，以提高重建质量并避免低反射率区域、多路径干扰和传感器有限的明确深度范围等问题。我们展示了这种方法提高了动态场景重建对错误校准和大运动的鲁棒性，并讨论了集成现代智能手机上现在可用的 RGB+ToF 传感器的好处和局限性。</t>
+  </si>
+  <si>
+    <t>CodeNeRF 是一种隐式 3D 神经表示，它学习对象形状和纹理在一个类别中的变化，并且可以从一组姿势图像中进行训练，以合成看不见的对象的新视图。与特定场景的原始 NeRF 不同，CodeNeRF 通过学习单独的嵌入来学习解开形状和纹理。在测试时，给定一个看不见的物体的单个未定位图像，CodeNeRF 通过优化联合估计相机视点、形状和外观代码。看不见的物体可以从单个图像中重建，然后从新的视点渲染，或者通过改变潜在代码编辑它们的形状和纹理。我们在 SRN 基准上进行了实验，结果表明 CodeNeRF 可以很好地泛化到看不见的对象，并且在测试时需要已知相机姿态的方法达到同等性能。我们在真实世界图像上的结果表明，CodeNeRF 可以弥合模拟到真实的差距。</t>
+  </si>
+  <si>
+    <t>我们提出了 StyleNeRF，这是一种 3D 感知生成模型，用于具有高多视图一致性的逼真的高分辨率图像合成，可以在非结构化 2D 图像上进行训练。现有方法要么无法合成具有精细细节的高分辨率图像，要么产生明显的 3D 不一致伪影。此外，他们中的许多人缺乏对风格属性和明确的 3D 相机姿势的控制。 StyleNeRF 将神经辐射场 (NeRF) 集成到基于样式的生成器中，以应对上述挑战，即提高渲染效率和 3D 一致性以生成高分辨率图像。我们执行体积渲染只是为了生成一个低分辨率的特征图，并在 2D 中逐步应用上采样来解决第一个问题。为了减轻 2D 上采样引起的不一致性，我们提出了多种设计，包括更好的上采样器和新的正则化损失。通过这些设计，StyleNeRF 可以以交互速率合成高分辨率图像，同时保持高质量的 3D 一致性。 StyleNeRF 还可以控制相机姿势和不同级别的样式，可以推广到看不见的视图。它还支持具有挑战性的任务，包括放大和缩小、样式混合、反转和语义编辑。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 是一种从姿势输入图像的集合中合成高质量新颖视图的技术。与大多数视图合成方法一样，NeRF 使用色调映射低动态范围（LDR）作为输入；这些图像已由有损相机管道处理，该管道可以平滑细节、剪辑高光并扭曲原始传感器数据的简单噪声分布。我们将 NeRF 修改为直接在线性原始图像上进行训练，保留场景的完整动态范围。通过从生成的 NeRF 渲染原始输出图像，我们可以执行新颖的高动态范围 (HDR) 视图合成任务。除了改变相机视角之外，我们还可以在事后操纵焦点、曝光和色调映射。尽管单个原始图像看起来比后处理的图像噪声大得多，但我们表明 NeRF 对原始噪声的零均值分布具有高度鲁棒性。当针对许多嘈杂的原始输入 (25-200) 进行优化时，NeRF 生成的场景表示非常准确，以至于其渲染的新颖视图优于在相同宽基线输入图像上运行的专用单图像和多图像深度原始降噪器。因此，我们的方法（我们称为 RawNeRF）可以从在近黑暗中捕获的极其嘈杂的图像中重建场景。</t>
+  </si>
+  <si>
+    <t>我们提出了 iNeRF，这是一个通过“反转”经过训练的神经辐射场 (NeRF) 来执行姿态估计的框架。 NeRF 已被证明对视图合成任务非常有效——合成真实世界场景或对象的逼真的新视图。在这项工作中，我们研究是否可以使用 NeRF 进行综合分析来进行 6DoF 姿势估计——给定图像，找到相机相对于 3D 模型的平移和旋转。从初始姿态估计开始，我们使用梯度下降来最小化从已经训练的 NeRF 渲染的像素和观察图像中的像素之间的残差。在我们的实验中，我们首先研究 1）如何在 iNeRF 的姿势细化过程中对光线进行采样以收集信息梯度，以及 2）不同批次大小的光线如何影响合成数据集上的 iNeRF。然后，我们展示了对于来自 LLFF 数据集的复杂现实世界场景，iNeRF 可以通过估计新图像的相机位姿并将这些图像用作 NeRF 的额外训练数据来改进 NeRF。最后，我们展示了 iNeRF 可以与基于特征的姿势初始化相结合。该方法优于所有其他依赖 LineMOD 上的合成数据的基于 RGB 的方法。</t>
+  </si>
+  <si>
+    <t>虽然深度学习使用前馈网络重塑了经典的运动捕捉管道，但需要生成模型通过迭代细化来恢复精细对齐。不幸的是，现有模型通常是在受控条件下手工制作或学习的，仅适用于有限的领域。我们提出了一种通过扩展神经辐射场 (NeRFs) 从未标记的单目视频中学习生成神经体模型的方法。我们为它们配备了骨架，以适用于时变和关节运动。一个关键的见解是，隐式模型需要与显式曲面模型中使用的正向运动学相反。我们的重新参数化定义了相对于身体部位姿势的空间潜在变量，从而克服了过度参数化的不适定逆运算。这使得从头开始学习体积身体形状和外观，同时共同改进关节姿势；输入视频上的所有外观、姿势或 3D 形状都没有地面实况标签。当用于新视图合成和动作捕捉时，我们的神经模型提高了不同数据集的准确性。项目网站：此 https 网址。</t>
+  </si>
+  <si>
+    <t>考虑到仅来自一组 2D 图像的新视图合成 (NVS) 问题，我们通过消除已知或预先计算的相机参数的要求，简化了前向场景中神经辐射场 (NeRF) 的训练过程，包括内在函数和 6DoF 姿势。为此，我们提出了 NeRF−−，具有三个贡献：首先，我们表明相机参数可以通过光度重建作为可学习参数与 NeRF 训练联合优化；其次，为了对相机参数估计和新颖视图渲染的质量进行基准测试，我们引入了一个新的路径跟踪合成场景数据集，称为 Blender Forward-Facing Dataset (BLEFF)；第三，我们进行了广泛的分析以了解各种相机运动下的训练行为，并表明在大多数情况下，联合优化管道可以恢复准确的相机参数并实现与使用 COLMAP 预计算相机参数训练的方法相当的新视图合成质量。</t>
+  </si>
+  <si>
+    <t>我们首次展示了多层感知器 (MLP) 可以作为手持 RGB-D 相机的实时 SLAM 系统中唯一的场景表示。我们的网络在没有先验数据的情况下进行实时操作训练，构建了一个密集的、特定于场景的隐式 3D 占用率和颜色模型，该模型也可立即用于跟踪。</t>
+  </si>
+  <si>
+    <t>神经隐式表示最近在各个领域都显示出令人鼓舞的结果，包括在同时定位和映射 (SLAM) 方面取得的可喜进展。然而，现有方法会产生过度平滑的场景重建，并且难以扩展到大场景。这些限制主要是由于它们简单的全连接网络架构没有在观察中包含本地信息。在本文中，我们提出了 NICE-SLAM，这是一种密集的 SLAM 系统，它通过引入分层场景表示来结合多级局部信息。使用预先训练的几何先验优化这种表示可以在大型室内场景中进行详细的重建。与最近的神经隐式 SLAM 系统相比，我们的方法更具可扩展性、高效性和鲁棒性。在五个具有挑战性的数据集上的实验证明了 NICE-SLAM 在映射和跟踪质量方面的竞争结果。</t>
+  </si>
+  <si>
+    <t>我们介绍了 GNeRF，这是一个将生成对抗网络 (GAN) 与神经辐射场 (NeRF) 重建相结合的框架，用于具有未知甚至随机初始化相机姿势的复杂场景。最近基于 NeRF 的进展因显着的逼真的新视图合成而受到欢迎。然而，它们中的大多数严重依赖于准确的相机位姿估计，而最近的一些方法只能在相机轨迹相对较短的大致前向场景中优化未知相机位姿，并且需要粗略的相机位姿初始化。不同的是，我们的 GNeRF 仅将随机初始化的姿势用于复杂的由外而内的场景。我们提出了一种新颖的两阶段端到端框架。第一阶段将 GAN 的使用带入新领域，以联合优化粗略的相机姿势和辐射场，而第二阶段通过额外的光度损失对它们进行细化。我们使用混合迭代优化方案克服了局部最小值。对各种合成和自然场景的广泛实验证明了 GNeRF 的有效性。更令人印象深刻的是，我们的方法在那些以前被认为极具挑战性的重复模式甚至低纹理的场景中优于基线。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 最近在计算机视觉界引起了极大的兴趣，因为它具有合成真实世界场景的逼真的新颖视图的能力。然而，NeRF 的一个限制是它需要准确的相机姿势来学习场景表示。在本文中，我们提出了 Bundle-Adjusting Neural Radiance Fields (BARF)，用于从不完美（甚至未知）的相机姿势训练 NeRF——学习神经 3D 表示和注册相机帧的联合问题。我们建立了与经典图像对齐的理论联系，并表明从粗到细的配准也适用于 NeRF。此外，我们表明，在 NeRF 中天真地应用位置编码会对基于合成的目标的注册产生负面影响。合成数据和真实世界数据的实验表明，BARF 可以有效地优化神经场景表示并同时解决大的相机位姿错位问题。这使得来自未知相机位姿的视频序列的视图合成和定位成为可能，为视觉定位系统（例如 SLAM）和密集 3D 映射和重建的潜在应用开辟了新途径。</t>
+  </si>
+  <si>
+    <t>在这项工作中，我们提出了一种用于具有任意非线性失真的通用相机的相机自校准算法。我们共同学习场景的几何形状和准确的相机参数，无需任何校准对象。我们的相机模型包括针孔模型、径向失真和可以学习任意非线性相机失真的通用噪声模型。虽然传统的自校准算法主要依赖于几何约束，但我们还结合了光度一致性。这需要学习场景的几何形状，我们使用神经辐射场 (NeRF)。我们还提出了一种新的几何损失函数，即投影射线距离损失，以结合复杂非线性相机模型的几何一致性。我们在标准真实图像数据集上验证了我们的方法，并证明我们的模型可以从头开始学习相机的内在和外在（姿势），而无需 COLMAP 初始化。此外，我们表明，以可微分的方式学习准确的相机模型可以让我们在 NeRF 上提高 PSNR。我们通过实验证明我们提出的方法适用于 NeRF 的变体。此外，我们使用一组用鱼眼镜头拍摄的图像来证明学习相机模型与 COLMAP 初始化相比，共同提高了性能。</t>
+  </si>
+  <si>
+    <t>将场景分解为其形状、反射率和照明度是计算机视觉和图形学中一个具有挑战性但重要的问题。当照明不是实验室条件下的单一光源而是不受约束的环境照明时，这个问题本质上更具挑战性。尽管最近的工作表明可以使用隐式表示来模拟物体的辐射场，但这些技术中的大多数只能实现视图合成而不是重新照明。此外，评估这些辐射场是资源和时间密集型的。我们提出了一种神经反射分解 (NeRD) 技术，该技术使用基于物理的渲染将场景分解为空间变化的 BRDF 材料属性。与现有技术相比，我们的输入图像可以在不同的照明条件下捕获。此外，我们还提出了将学习到的反射体积转换为可重新照明的纹理网格的技术，从而能够使用新颖的照明进行快速实时渲染。我们通过在合成数据集和真实数据集上的实验证明了所提出方法的潜力，我们能够从图像集合中获得高质量的可重新点亮的 3D 资产。</t>
+  </si>
+  <si>
+    <t>我们提出了一种方法，该方法将由不受约束的已知照明照明的场景的一组图像作为输入，并生成可以在任意照明条件下从新视点渲染的 3D 表示作为输出。我们的方法将场景表示为参数化为 MLP 的连续体积函数，其输入是 3D 位置，其输出是该输入位置的以下场景属性：体积密度、表面法线、材料参数、到任何方向上第一个表面交点的距离，以及任何方向的外部环境的可见性。总之，这些允许我们在任意照明下渲染物体的新视图，包括间接照明效果。预测的能见度和表面相交场对于我们的模型在训练期间模拟直接和间接照明的能力至关重要，因为先前工作使用的蛮力技术对于具有单灯的受控设置之外的照明条件是难以处理的。我们的方法在恢复可重新照明的 3D 场景表示方面优于替代方法，并且在对先前工作构成重大挑战的复杂照明设置中表现良好。</t>
+  </si>
+  <si>
+    <t>我们提出了 NeX，这是一种基于多平面图像 (MPI) 增强的新型视图合成的新方法，可以实时再现 NeXt 级别的视图相关效果。与使用一组简单 RGBα 平面的传统 MPI 不同，我们的技术通过将每个像素参数化为从神经网络学习的基函数的线性组合来模拟视图相关的效果。此外，我们提出了一种混合隐式-显式建模策略，该策略改进了精细细节并产生了最先进的结果。我们的方法在基准前向数据集以及我们新引入的数据集上进行了评估，该数据集旨在测试与视图相关的建模的极限，具有明显更具挑战性的效果，例如 CD 上的彩虹反射。我们的方法在这些数据集的所有主要指标上都取得了最好的总体得分，渲染时间比现有技术快 1000 倍以上。</t>
+  </si>
+  <si>
+    <t>我们解决了从由一种未知光照条件照射的物体的多视图图像（及其相机姿势）中恢复物体的形状和空间变化反射率的问题。这使得能够在任意环境照明下渲染对象的新颖视图并编辑对象的材质属性。我们方法的关键，我们称之为神经辐射分解（NeRFactor），是提取神经辐射场（NeRF）的体积几何[Mildenhall et al。 2020] 将对象表示为表面表示，然后在解决空间变化的反射率和环境照明的同时联合细化几何。具体来说，NeRFactor 在没有任何监督的情况下恢复表面法线、光能见度、反照率和双向反射分布函数 (BRDF) 的 3D 神经场，仅使用重新渲染损失、简单的平滑先验和从真实数据中学习的数据驱动的 BRDF 先验-世界BRDF测量。通过显式建模光可见性，NeRFactor 能够从反照率中分离出阴影，并在任意光照条件下合成逼真的软阴影或硬阴影。 NeRFactor 能够恢复令人信服的 3D 模型，用于在合成场景和真实场景的这种具有挑战性且约束不足的捕获设置中进行自由视点重新照明。定性和定量实验表明，NeRFactor 在各种任务中都优于经典和基于深度学习的最新技术。我们的视频、代码和数据可在 people.csail.mit.edu/xiuming/projects/nerfactor/ 上找到。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 为各种捕捉设置实现了令人印象深刻的视图合成结果，包括有界场景的 360 度捕捉以及有界和无界场景的前向捕捉。 NeRF 将表示视图不变不透明度和视图相关颜色体积的多层感知器 (MLP) 拟合到一组训练图像，并基于体积渲染技术对新视图进行采样。在这份技术报告中，我们首先评论了辐射场及其潜在的模糊性，即形状-辐射模糊度，并分析了 NeRF 在避免这种模糊性方面的成功。其次，我们解决了将 NeRF 应用于大规模、无界 3D 场景中对象的 360 度捕获所涉及的参数化问题。我们的方法在这种具有挑战性的场景中提高了视图合成保真度。此 https 网址提供了代码。</t>
+  </si>
+  <si>
+    <t>深度生成模型允许以高分辨率进行逼真的图像合成。但对于许多应用程序来说，这还不够：内容创建还需要可控。虽然最近的几项工作研究了如何解开数据变化的潜在因素，但它们中的大多数都在 2D 中运行，因此忽略了我们的世界是 3D 的。此外，只有少数作品考虑场景的构图性质。我们的关键假设是，将合成 3D 场景表示合并到生成模型中会导致更可控的图像合成。将场景表示为合成生成神经特征场使我们能够从背景中解开一个或多个对象以及单个对象的形状和外观，同时从非结构化和未定型的图像集合中学习，而无需任何额外的监督。将这种场景表示与神经渲染管道相结合，可以生成快速且逼真的图像合成模型。正如我们的实验所证明的那样，我们的模型能够解开单个对象，并允许在场景中平移和旋转它们以及改变相机姿势。</t>
+  </si>
+  <si>
+    <t>我们提出了一种从捕获的对象图像中合成逼真场景的方法。我们的工作建立在神经辐射场 (NeRFs) 之上，它隐含地模拟了场景的体积密度和定向发射的辐射。虽然 NeRF 可以合成逼真的图片，但它们只对静态场景进行建模，并且与特定的成像条件密切相关。这个属性使得 NeRFs 难以泛化到新场景，包括新的光照或对象的新排列。我们建议学习以对象为中心的神经散射函数 (OSF)，而不是像 NeRF 那样学习场景辐射场，这是一种使用与光照和视图相关的神经网络隐式模拟每个对象的光传输的表示。即使物体或灯光移动，这也可以渲染场景，而无需重新训练。结合体积路径跟踪程序，我们的框架能够渲染对象内和对象间的光传输效果，包括遮挡、镜面反射、阴影和间接照明。我们评估了我们的场景合成方法，并表明它可以推广到新的照明条件，产生逼真的、物理上精确的多对象场景渲染。</t>
+  </si>
+  <si>
+    <t>动态人体的逼真渲染是远程呈现系统、虚拟购物、合成数据生成等的重要能力。最近，结合计算机图形学和机器学习技术的神经渲染方法已经创建了人类和物体的高保真模型。其中一些方法不会为可驱动的人体模型（神经体积）产生足够高保真度的结果，而其他方法则具有极长的渲染时间（NeRF）。我们提出了一种新颖的组合 3D 表示，它结合了以前最好的方法来产生更高分辨率和更快的结果。我们的表示通过将粗略的 3D 结构感知动画代码网格与连续学习的场景函数相结合，弥合了离散和连续体积表示之间的差距，该函数将每个位置及其相应的局部动画代码映射到其与视图相关的发射辐射和局部体积密度。可微分体渲染用于计算人头和上身的照片般逼真的新颖视图，并仅使用 2D 监督来端到端训练我们的新颖表示。此外，我们表明，学习到的动态辐射场可用于基于全局动画代码合成新的看不见的表情。我们的方法在合成动态人头和上半身的新视图方面取得了最先进的结果。</t>
+  </si>
+  <si>
+    <t>最近的隐式神经渲染方法表明，可以通过仅由一组 RGB 图像监督的预测其体积密度和颜色来学习复杂场景的准确视图合成。然而，现有方法仅限于学习将所有场景对象编码为单个神经网络的静态场景的有效表示，并且缺乏将动态场景表示和分解为单个场景对象的能力。在这项工作中，我们提出了第一个将动态场景分解为场景图的神经渲染方法。我们提出了一种学习的场景图表示，它对对象变换和辐射进行编码，以有效地渲染场景的新颖排列和视图。为此，我们学习隐式编码的场景，并结合联合学习的潜在表示来描述具有单个隐式函数的对象。我们在合成和真实汽车数据上评估所提出的方法，验证我们的方法学习动态场景 - 仅通过观察该场景的视频 - 并允许渲染具有看不见的对象集的新颖场景组合的新颖照片般逼真的视图看不见的姿势。</t>
+  </si>
+  <si>
+    <t>我们研究从单个图像推断以对象为中心的场景表示的问题，旨在推导出解释图像形成过程的表示，捕捉场景的 3D 性质，并且在没有监督的情况下学习。由于将复杂的 3D 到 2D 图像形成过程集成到强大的推理方案（如深度网络）中存在根本性挑战，大多数现有的场景分解方法都缺乏这些特征中的一个或多个。在本文中，我们提出了对象辐射场 (uORF) 的无监督发现，将神经 3D 场景表示和渲染的最新进展与深度推理网络相结合，用于无监督 3D 场景分解。在没有注释的多视图 RGB 图像上进行训练，uORF 学习从单个图像分解具有不同纹理背景的复杂场景。我们展示了 uORF 在无监督 3D 场景分割、新视图合成和三个数据集上的场景编辑方面表现良好。</t>
+  </si>
+  <si>
+    <t>隐式神经渲染技术已经显示出用于新视图合成的有希望的结果。然而，现有方法通常将整个场景编码为一个整体，这通常不知道对象身份，并且限制了移动或添加家具等高级编辑任务的能力。在本文中，我们提出了一种新颖的神经场景渲染系统，该系统学习对象组成的神经辐射场，并为集群和真实世界场景生成具有编辑能力的逼真渲染。具体来说，我们设计了一种新颖的双路径架构，其中场景分支对场景几何和外观进行编码，对象分支根据可学习的对象激活码对每个独立对象进行编码。为了在严重混乱的场景中进行训练，我们提出了一种场景引导的训练策略来解决遮挡区域中的 3D 空间模糊性并学习每个对象的清晰边界。大量实验表明，我们的系统不仅在静态场景新视图合成方面取得了有竞争力的性能，而且为对象级编辑产生了逼真的渲染。</t>
+  </si>
+  <si>
+    <t>语义标签与几何和辐射重建高度相关，因为具有相似形状和外观的场景实体更有可能来自相似的类别。最近的隐式神经重建技术很有吸引力，因为它们不需要事先的训练数据，但同样的完全自我监督的方法对于语义来说是不可能的，因为标签是人类定义的属性。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 是支持高质量视图合成的场景模型，针对每个场景进行了优化。在本文中，我们探索启用用户编辑类别级 NeRF - 也称为条件辐射场 - 在形状类别上训练。具体来说，我们介绍了一种将粗略的 2D 用户涂鸦传播到 3D 空间的方法，以修改局部区域的颜色或形状。首先，我们提出了一个条件辐射场，它结合了新的模块化网络组件，包括一个跨对象实例共享的形状分支。观察同一类别的多个实例，我们的模型在没有任何监督的情况下学习底层部分语义，从而允许将粗略的 2D 用户涂鸦传播到整个 3D 区域（例如，椅子座位）。接下来，我们提出了一种针对特定网络组件的混合网络更新策略，该策略平衡了效率和准确性。在用户交互过程中，我们制定了一个既满足用户约束又保留原始对象结构的优化问题。我们在三个形状数据集上展示了我们在各种编辑任务上的方法，并表明它优于以前的神经编辑方法。最后，我们编辑真实照片的外观和形状，并显示编辑传播到外推的新视图。</t>
+  </si>
+  <si>
+    <t>生成自由视点视频对于沉浸式 VR/AR 体验至关重要，但最近的神经学进展仍然缺乏编辑能力来操纵大型动态场景的视觉感知。为了填补这一空白，在本文中，我们提出了第一种仅使用稀疏的 16 个摄像头为大规模动态场景生成可编辑照片般逼真的自由视点视频的方法。我们方法的核心是一种新的分层神经表示，其中包括环境本身的每个动态实体都被制定为称为 ST-NeRF 的时空相干神经分层辐射表示。这种分层表示支持对动态场景的完全感知和真实操作，同时仍支持大范围的自由观看体验。在我们的 ST-NeRF 中，动态实体/层被表示为连续函数，以连续和自监督的方式实现动态实体的位置、变形以及外观的解耦。我们提出了一个场景解析 4D 标签映射跟踪来显式地解开空间信息，以及一个连续变形模块来隐式地解开时间运动。进一步引入了一种对象感知体绘制方案，用于重新组装所有神经层。我们采用了一种新颖的分层损失和运动感知光线采样策略，以实现对具有多个表演者的大型动态场景的有效训练，我们的框架进一步实现了各种编辑功能，即操纵规模和位置，复制或重新定时单个神经层在保持高度真实感的同时创造众多视觉效果。大量实验证明了我们的方法在为动态场景生成高质量、照片般逼真和可编辑的自由视点视频方面的有效性。</t>
+  </si>
+  <si>
+    <t>我们研究使用神经辐射场 (NeRF) 从输入图像的集合中学习高质量的 3D 对象类别模型。与以前的工作相比，我们能够做到这一点，同时将前景对象与不同的背景分开。我们通过 2 分量 NeRF 模型 FiG-NeRF 实现了这一点，该模型更喜欢将场景解释为几何恒定的背景和代表对象类别的可变形前景。我们表明，这种方法可以仅使用光度监督和随意捕获的对象图像来学习准确的 3D 对象类别模型。此外，我们的两部分分解允许模型执行准确和清晰的模态分割。我们使用合成的、实验室捕获的和野外数据，通过视图合成和图像保真度指标对我们的方法进行定量评估。我们的结果证明了令人信服的 3D 对象类别建模，其性能超过了现有方法的性能。</t>
+  </si>
+  <si>
+    <t>我们研究使用神经场来模拟不同的中尺度结构，例如毛皮、织物和草。我们建议使用由神经反射场 (NeRF-Tex) 表示的多功能体积基元，而不是使用经典的图形基元来建模结构，它联合建模材料的几何形状及其对照明的响应。 NeRF-Tex 原语可以在基础网格上实例化，以使用所需的细观和微尺度外观对其进行“纹理化”。我们根据控制外观的用户定义参数来调节反射率场。因此，单个 NeRF 纹理捕获了反射场的整个空间，而不是一个特定的结构。这增加了可以建模的外观范围，并提供了一种解决重复纹理伪影的解决方案。我们还证明了 NeRF 纹理自然地促进了连续的细节层次渲染。我们的方法将神经网络的多功能性和建模能力与虚拟场景精确建模所需的艺术控制相结合。虽然我们所有的训练数据目前都是合成的，但我们的工作提供了一个方法，可以进一步扩展以从真实图像中提取复杂、难以建模的外观。</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRF) 使用的渲染过程对每个像素单条射线进行采样，因此在训练或测试图像以不同分辨率观察场景内容时，可能会产生过度模糊或混叠的渲染。对于 NeRF 来说，通过每个像素渲染多条光线来进行超级采样的直接解决方案是不切实际的，因为渲染每条光线需要查询多层感知器数百次。我们的解决方案，我们称之为“mip-NeRF”（à la“mipmap”），扩展了 NeRF 以在连续值的尺度上表示场景。通过有效地渲染抗锯齿圆锥截头体而不是射线，mip-NeRF 减少了令人反感的锯齿伪影并显着提高了 NeRF 表示精细细节的能力，同时也比 NeRF 快 7% 和一半的大小。与 NeRF 相比，mip-NeRF 在使用 NeRF 呈现的数据集上将平均错误率降低了 17%，在我们呈现的该数据集的具有挑战性的多尺度变体上降低了 60%。 mip-NeRF 还能够在我们的多尺度数据集上匹配蛮力超采样 NeRF 的准确性，同时速度提高 22 倍。</t>
+  </si>
+  <si>
+    <t>神经隐式 3D 表示已成为从多视图图像重建表面和合成新视图的强大范例。不幸的是，DVR 或 IDR 等现有方法需要精确的每像素对象掩码作为监督。同时，神经辐射场已经彻底改变了新的视图合成。然而，NeRF 的估计体积密度不允许精确的表面重建。我们的主要见解是隐式表面模型和辐射场可以以统一的方式制定，从而使用相同的模型实现表面和体积渲染。这种统一的视角实现了新颖、更有效的采样程序，并能够在没有输入掩码的情况下重建准确的表面。我们在 DTU、BlendedMVS 和合成室内数据集上比较我们的方法。我们的实验表明，我们在重建质量方面优于 NeRF，同时在不需要掩码的情况下与 IDR 相当。</t>
+  </si>
+  <si>
+    <t>我们提出了一种新的神经表面重建方法，称为 NeuS，用于从 2D 图像输入中重建具有高保真度的对象和场景。现有的神经表面重建方法，如 DVR 和 IDR，需要前景掩码作为监督，容易陷入局部最小值，因此难以重建具有严重自遮挡或薄结构的物体。同时，最近用于新视图合成的神经方法，例如 NeRF 及其变体，使用体积渲染来生成具有优化鲁棒性的神经场景表示，即使对于高度复杂的对象也是如此。然而，从这种学习到的隐式表示中提取高质量的表面是很困难的，因为表示中没有足够的表面约束。在 NeuS 中，我们建议将表面表示为有符号距离函数 (SDF) 的零级集，并开发一种新的体绘制方法来训练神经 SDF 表示。我们观察到传统的体绘制方法会导致表面重建的固有几何误差（即偏差），因此提出了一种新的公式，该公式在一阶近似中没有偏差，从而即使没有掩模监督也能实现更准确的表面重建.在 DTU 数据集和 BlendedMVS 数据集上的实验表明，NeuS 在高质量表面重建方面优于最先进的技术，特别是对于具有复杂结构和自遮挡的物体和场景。</t>
+  </si>
+  <si>
+    <t>神经体绘制最近变得越来越流行，因为它成功地从一组稀疏的输入图像中合成了场景的新视图。到目前为止，通过神经体绘制技术学习的几何图形是使用通用密度函数建模的。此外，几何本身是使用密度函数的任意水平集提取的，这会导致嘈杂的、通常是低保真度的重建。本文的目标是改进神经体绘制中的几何表示和重建。我们通过将体积密度建模为几何形状的函数来实现这一点。这与之前将几何建模为体积密度函数的工作形成对比。更详细地说，我们将体积密度函数定义为应用于有符号距离函数 (SDF) 表示的拉普拉斯累积分布函数 (CDF)。这种简单的密度表示具有三个好处：（i）它为在神经体绘制过程中学习的几何图形提供了有用的归纳偏差； (ii) 它有助于限制不透明度近似误差，从而实现对视线的准确采样。准确的采样对于提供几何和辐射的精确耦合很重要； (iii) 它允许在体积渲染中对形状和外观进行有效的无监督解开。将这种新的密度表示应用于具有挑战性的场景多视图数据集产生了高质量的几何重建，优于相关的基线。此外，由于两者的分离，可以在场景之间切换形状和外观。</t>
+  </si>
+  <si>
+    <t>在这项工作中，我们提出了一种新的多视图深度估计方法，该方法在最近提出的神经辐射场 (NeRF) 上利用了传统的 SfM 重建和基于学习的先验。与现有的依赖于估计对应的基于神经网络的优化方法不同，我们的方法直接优化隐式体积，消除了在室内场景中匹配像素的挑战性步骤。我们方法的关键是利用基于学习的先验来指导 NeRF 的优化过程。我们的系统首先通过微调其稀疏 SfM 重建来适应目标场景上的单目深度网络。然后，我们证明了 NeRF 的形状-辐射模糊性仍然存在于室内环境中，并建议通过采用适应的深度先验来监控体绘制的采样过程来解决这个问题。最后，通过对渲染图像进行误差计算获得的每像素置信度图可用于进一步提高深度质量。实验表明，我们提出的框架在室内场景中显着优于最先进的方法，在基于对应的优化和基于 NeRF 的优化对适应深度先验的有效性方面提出了令人惊讶的发现。此外，我们表明引导优化方案不会牺牲神经辐射场的原始合成能力，提高了可见视图和新视图的渲染质量。</t>
+  </si>
+  <si>
+    <t>人类对我们周围的 3D 环境有着强烈的直觉理解。我们大脑中的物理心智模型适用于不同材料的物体，使我们能够执行远远超出当前机器人范围的广泛操作任务。在这项工作中，我们希望纯粹从 2D 视觉观察中学习动态 3D 场景的模型。我们的模型结合了神经弧度</t>
+  </si>
+  <si>
+    <t>神经辐射场 (NeRFs) 最近已成为表示自然、复杂 3D 场景的强大范例。 NeRF 表示神经网络中的连续体积密度和 RGB 值，并通过光线追踪从看不见的相机视点生成照片般逼真的图像。我们提出了一种算法，用于在表示为 NeRF 的 3D 环境中导航机器人，仅使用板载 RGB 相机进行定位。我们假设场景的 NeRF 已经离线预训练，机器人的目标是在 NeRF 中的未占用空间中导航以达到目标姿势。我们引入了一种轨迹优化算法，该算法基于离散时间版本的差分平坦度避免与 NeRF 中的高密度区域发生碰撞，该版本可以约束机器人的完整姿势和控制输入。我们还引入了一种基于优化的过滤方法来估计 NeRF 中机器人的 6DoF 姿势和速度，仅给定一个板载 RGB 相机。我们将轨迹规划器与位姿过滤器结合在一个在线重新规划循环中，以提供基于视觉的机器人导航管道。我们展示了一个四旋翼机器人仅使用 RGB 相机在丛林健身房环境、教堂内部和巨石阵中导航的模拟结果。我们还演示了一个在教堂中导航的全向地面机器人，要求它重新定向以适应狭窄的缝隙。可以在此 https 网址上找到这项工作的视频。</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2107.07905</t>
   </si>
 </sst>
 </file>
@@ -986,11 +2396,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1346,23 +2753,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:T103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="93.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5" customWidth="1"/>
     <col min="3" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="161.5" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" customWidth="1"/>
+    <col min="9" max="17" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +2792,7 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
@@ -1406,19 +2814,25 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P1" t="s">
         <v>14</v>
       </c>
       <c r="Q1" t="s">
+        <v>258</v>
+      </c>
+      <c r="R1" t="s">
+        <v>261</v>
+      </c>
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1437,14 +2851,14 @@
       <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
       <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1452,25 +2866,25 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>130</v>
+        <v>108</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1478,16 +2892,16 @@
         <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>131</v>
+      <c r="H4" t="s">
+        <v>130</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1496,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1504,28 +2918,28 @@
         <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>132</v>
+      <c r="H5" t="s">
+        <v>131</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1533,22 +2947,22 @@
         <v>27</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
+      </c>
+      <c r="H6" t="s">
+        <v>132</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1556,19 +2970,19 @@
         <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>111</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
+      </c>
+      <c r="H7" t="s">
+        <v>133</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -1577,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1585,19 +2999,19 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>134</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -1606,7 +3020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1614,20 +3028,20 @@
         <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" t="s">
         <v>152</v>
       </c>
-      <c r="E9" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="J9">
         <v>1</v>
       </c>
@@ -1635,7 +3049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1643,28 +3057,28 @@
         <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" t="s">
-        <v>113</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="R10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="H10" t="s">
+        <v>135</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1672,25 +3086,25 @@
         <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G11" t="s">
-        <v>114</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
+      </c>
+      <c r="H11" t="s">
+        <v>136</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1698,19 +3112,19 @@
         <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G12" t="s">
-        <v>115</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>138</v>
+        <v>114</v>
+      </c>
+      <c r="H12" t="s">
+        <v>137</v>
       </c>
       <c r="M12">
         <v>1</v>
@@ -1719,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1727,19 +3141,19 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G13" t="s">
-        <v>116</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
+      </c>
+      <c r="H13" t="s">
+        <v>138</v>
       </c>
       <c r="J13">
         <v>1</v>
@@ -1748,7 +3162,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1756,31 +3170,31 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G14" t="s">
-        <v>117</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
+      </c>
+      <c r="H14" t="s">
+        <v>139</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
-      <c r="R14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="T14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1788,16 +3202,16 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G15" t="s">
-        <v>118</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
+      </c>
+      <c r="H15" t="s">
+        <v>140</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1805,11 +3219,11 @@
       <c r="M15">
         <v>1</v>
       </c>
-      <c r="R15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+      <c r="T15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1817,19 +3231,19 @@
         <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G16" t="s">
-        <v>119</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
+      </c>
+      <c r="H16" t="s">
+        <v>141</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -1838,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1846,28 +3260,31 @@
         <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G17" t="s">
-        <v>120</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
+      </c>
+      <c r="H17" t="s">
+        <v>142</v>
       </c>
       <c r="R17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+      <c r="T17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1875,22 +3292,22 @@
         <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
+      </c>
+      <c r="H18" t="s">
+        <v>143</v>
       </c>
       <c r="I18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1898,22 +3315,22 @@
         <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
+      </c>
+      <c r="H19" t="s">
+        <v>144</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -1922,7 +3339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1930,19 +3347,19 @@
         <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>123</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
+      </c>
+      <c r="H20" t="s">
+        <v>145</v>
       </c>
       <c r="N20">
         <v>1</v>
@@ -1951,7 +3368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1959,22 +3376,22 @@
         <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
+      </c>
+      <c r="H21" t="s">
+        <v>146</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -1983,7 +3400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -1991,25 +3408,25 @@
         <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="R22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="68" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -2017,19 +3434,19 @@
         <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G23" t="s">
-        <v>126</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
+      </c>
+      <c r="H23" t="s">
+        <v>148</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2038,27 +3455,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>290</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
+      </c>
+      <c r="H24" t="s">
+        <v>149</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -2070,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="119" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -2078,23 +3495,2365 @@
         <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G25" t="s">
-        <v>129</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="R25">
+        <v>128</v>
+      </c>
+      <c r="H25" t="s">
+        <v>150</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>155</v>
+      </c>
+      <c r="C26" t="s">
+        <v>157</v>
+      </c>
+      <c r="D26" t="s">
+        <v>259</v>
+      </c>
+      <c r="E26" t="s">
+        <v>158</v>
+      </c>
+      <c r="F26" t="s">
+        <v>159</v>
+      </c>
+      <c r="G26" t="s">
+        <v>160</v>
+      </c>
+      <c r="H26" t="s">
+        <v>161</v>
+      </c>
+      <c r="T26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" t="s">
+        <v>163</v>
+      </c>
+      <c r="F27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>167</v>
+      </c>
+      <c r="C28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D28" t="s">
+        <v>169</v>
+      </c>
+      <c r="E28" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" t="s">
+        <v>173</v>
+      </c>
+      <c r="G28" t="s">
+        <v>171</v>
+      </c>
+      <c r="H28" t="s">
+        <v>170</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>174</v>
+      </c>
+      <c r="D29" t="s">
+        <v>175</v>
+      </c>
+      <c r="E29" t="s">
+        <v>176</v>
+      </c>
+      <c r="G29" t="s">
+        <v>474</v>
+      </c>
+      <c r="H29" t="s">
+        <v>549</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>154</v>
+      </c>
+      <c r="B30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C30" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" t="s">
+        <v>179</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+      <c r="F30" t="s">
+        <v>181</v>
+      </c>
+      <c r="G30" t="s">
+        <v>475</v>
+      </c>
+      <c r="H30" t="s">
+        <v>550</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>154</v>
+      </c>
+      <c r="B31" t="s">
+        <v>182</v>
+      </c>
+      <c r="C31" t="s">
+        <v>185</v>
+      </c>
+      <c r="D31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E31" t="s">
+        <v>184</v>
+      </c>
+      <c r="G31" t="s">
+        <v>476</v>
+      </c>
+      <c r="H31" t="s">
+        <v>551</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" t="s">
+        <v>186</v>
+      </c>
+      <c r="C32" t="s">
+        <v>185</v>
+      </c>
+      <c r="D32" t="s">
+        <v>187</v>
+      </c>
+      <c r="E32" t="s">
+        <v>188</v>
+      </c>
+      <c r="F32" t="s">
+        <v>189</v>
+      </c>
+      <c r="G32" t="s">
+        <v>477</v>
+      </c>
+      <c r="H32" t="s">
+        <v>552</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" t="s">
+        <v>190</v>
+      </c>
+      <c r="C33" t="s">
+        <v>191</v>
+      </c>
+      <c r="D33" t="s">
+        <v>192</v>
+      </c>
+      <c r="E33" t="s">
+        <v>193</v>
+      </c>
+      <c r="F33" t="s">
+        <v>194</v>
+      </c>
+      <c r="G33" t="s">
+        <v>478</v>
+      </c>
+      <c r="H33" t="s">
+        <v>553</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B34" t="s">
+        <v>195</v>
+      </c>
+      <c r="C34" t="s">
+        <v>196</v>
+      </c>
+      <c r="D34" t="s">
+        <v>197</v>
+      </c>
+      <c r="E34" t="s">
+        <v>198</v>
+      </c>
+      <c r="G34" t="s">
+        <v>479</v>
+      </c>
+      <c r="H34" t="s">
+        <v>554</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B35" t="s">
+        <v>199</v>
+      </c>
+      <c r="C35" t="s">
+        <v>358</v>
+      </c>
+      <c r="D35" t="s">
+        <v>200</v>
+      </c>
+      <c r="E35" t="s">
+        <v>201</v>
+      </c>
+      <c r="F35" t="s">
+        <v>202</v>
+      </c>
+      <c r="G35" t="s">
+        <v>480</v>
+      </c>
+      <c r="H35" t="s">
+        <v>555</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" t="s">
+        <v>203</v>
+      </c>
+      <c r="C36" t="s">
+        <v>205</v>
+      </c>
+      <c r="D36" t="s">
+        <v>206</v>
+      </c>
+      <c r="E36" t="s">
+        <v>207</v>
+      </c>
+      <c r="F36" t="s">
+        <v>204</v>
+      </c>
+      <c r="G36" t="s">
+        <v>481</v>
+      </c>
+      <c r="H36" t="s">
+        <v>556</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>154</v>
+      </c>
+      <c r="B37" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" t="s">
+        <v>209</v>
+      </c>
+      <c r="D37" t="s">
+        <v>210</v>
+      </c>
+      <c r="E37" t="s">
+        <v>211</v>
+      </c>
+      <c r="F37" t="s">
+        <v>212</v>
+      </c>
+      <c r="G37" t="s">
+        <v>482</v>
+      </c>
+      <c r="H37" t="s">
+        <v>557</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" t="s">
+        <v>213</v>
+      </c>
+      <c r="C38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E38" t="s">
+        <v>215</v>
+      </c>
+      <c r="G38" t="s">
+        <v>483</v>
+      </c>
+      <c r="H38" t="s">
+        <v>558</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>216</v>
+      </c>
+      <c r="C39" t="s">
+        <v>205</v>
+      </c>
+      <c r="D39" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" t="s">
+        <v>219</v>
+      </c>
+      <c r="G39" t="s">
+        <v>484</v>
+      </c>
+      <c r="H39" t="s">
+        <v>559</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+      <c r="T39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>220</v>
+      </c>
+      <c r="C40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" t="s">
+        <v>221</v>
+      </c>
+      <c r="E40" t="s">
+        <v>222</v>
+      </c>
+      <c r="G40" t="s">
+        <v>485</v>
+      </c>
+      <c r="H40" t="s">
+        <v>560</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+      <c r="T40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>223</v>
+      </c>
+      <c r="C41" t="s">
+        <v>168</v>
+      </c>
+      <c r="D41" t="s">
+        <v>224</v>
+      </c>
+      <c r="E41" t="s">
+        <v>225</v>
+      </c>
+      <c r="F41" t="s">
+        <v>226</v>
+      </c>
+      <c r="G41" t="s">
+        <v>486</v>
+      </c>
+      <c r="H41" t="s">
+        <v>561</v>
+      </c>
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="T41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>227</v>
+      </c>
+      <c r="C42" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" t="s">
+        <v>228</v>
+      </c>
+      <c r="E42" t="s">
+        <v>229</v>
+      </c>
+      <c r="F42" t="s">
+        <v>230</v>
+      </c>
+      <c r="G42" t="s">
+        <v>487</v>
+      </c>
+      <c r="H42" t="s">
+        <v>562</v>
+      </c>
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+      <c r="R42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
+        <v>231</v>
+      </c>
+      <c r="C43" t="s">
+        <v>185</v>
+      </c>
+      <c r="D43" t="s">
+        <v>232</v>
+      </c>
+      <c r="E43" t="s">
+        <v>233</v>
+      </c>
+      <c r="F43" t="s">
+        <v>234</v>
+      </c>
+      <c r="G43" t="s">
+        <v>488</v>
+      </c>
+      <c r="H43" t="s">
+        <v>563</v>
+      </c>
+      <c r="L43">
+        <v>1</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" t="s">
+        <v>235</v>
+      </c>
+      <c r="C44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" t="s">
+        <v>236</v>
+      </c>
+      <c r="E44" t="s">
+        <v>237</v>
+      </c>
+      <c r="G44" t="s">
+        <v>489</v>
+      </c>
+      <c r="H44" t="s">
+        <v>564</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
+        <v>238</v>
+      </c>
+      <c r="C45" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" t="s">
+        <v>239</v>
+      </c>
+      <c r="E45" t="s">
+        <v>240</v>
+      </c>
+      <c r="F45" t="s">
+        <v>241</v>
+      </c>
+      <c r="G45" t="s">
+        <v>490</v>
+      </c>
+      <c r="H45" t="s">
+        <v>565</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" t="s">
+        <v>242</v>
+      </c>
+      <c r="C46" t="s">
+        <v>243</v>
+      </c>
+      <c r="D46" t="s">
+        <v>244</v>
+      </c>
+      <c r="E46" t="s">
+        <v>245</v>
+      </c>
+      <c r="G46" t="s">
+        <v>491</v>
+      </c>
+      <c r="H46" t="s">
+        <v>566</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" t="s">
+        <v>246</v>
+      </c>
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="D47" t="s">
+        <v>247</v>
+      </c>
+      <c r="E47" t="s">
+        <v>248</v>
+      </c>
+      <c r="F47" t="s">
+        <v>249</v>
+      </c>
+      <c r="G47" t="s">
+        <v>492</v>
+      </c>
+      <c r="H47" t="s">
+        <v>567</v>
+      </c>
+      <c r="R47">
+        <v>1</v>
+      </c>
+      <c r="T47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>154</v>
+      </c>
+      <c r="B48" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" t="s">
+        <v>251</v>
+      </c>
+      <c r="D48" t="s">
+        <v>252</v>
+      </c>
+      <c r="E48" t="s">
+        <v>253</v>
+      </c>
+      <c r="F48" t="s">
+        <v>254</v>
+      </c>
+      <c r="G48" t="s">
+        <v>493</v>
+      </c>
+      <c r="H48" t="s">
+        <v>568</v>
+      </c>
+      <c r="O48">
+        <v>1</v>
+      </c>
+      <c r="R48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" t="s">
+        <v>255</v>
+      </c>
+      <c r="C49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" t="s">
+        <v>260</v>
+      </c>
+      <c r="E49" t="s">
+        <v>256</v>
+      </c>
+      <c r="F49" t="s">
+        <v>257</v>
+      </c>
+      <c r="G49" t="s">
+        <v>494</v>
+      </c>
+      <c r="H49" t="s">
+        <v>569</v>
+      </c>
+      <c r="Q49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" t="s">
+        <v>262</v>
+      </c>
+      <c r="C50" t="s">
+        <v>168</v>
+      </c>
+      <c r="D50" t="s">
+        <v>263</v>
+      </c>
+      <c r="E50" t="s">
+        <v>264</v>
+      </c>
+      <c r="F50" t="s">
+        <v>265</v>
+      </c>
+      <c r="G50" t="s">
+        <v>495</v>
+      </c>
+      <c r="H50" t="s">
+        <v>570</v>
+      </c>
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" t="s">
+        <v>209</v>
+      </c>
+      <c r="D51" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" t="s">
+        <v>268</v>
+      </c>
+      <c r="G51" t="s">
+        <v>496</v>
+      </c>
+      <c r="H51" t="s">
+        <v>571</v>
+      </c>
+      <c r="Q51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" t="s">
+        <v>269</v>
+      </c>
+      <c r="C52" t="s">
+        <v>185</v>
+      </c>
+      <c r="D52" t="s">
+        <v>270</v>
+      </c>
+      <c r="E52" t="s">
+        <v>271</v>
+      </c>
+      <c r="F52" t="s">
+        <v>272</v>
+      </c>
+      <c r="G52" t="s">
+        <v>497</v>
+      </c>
+      <c r="H52" t="s">
+        <v>572</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="Q52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" t="s">
+        <v>273</v>
+      </c>
+      <c r="C53" t="s">
+        <v>357</v>
+      </c>
+      <c r="D53" t="s">
+        <v>275</v>
+      </c>
+      <c r="E53" t="s">
+        <v>359</v>
+      </c>
+      <c r="F53" t="s">
+        <v>274</v>
+      </c>
+      <c r="G53" t="s">
+        <v>498</v>
+      </c>
+      <c r="H53" t="s">
+        <v>573</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" t="s">
+        <v>276</v>
+      </c>
+      <c r="C54" t="s">
+        <v>191</v>
+      </c>
+      <c r="D54" t="s">
+        <v>277</v>
+      </c>
+      <c r="E54" t="s">
+        <v>278</v>
+      </c>
+      <c r="F54" t="s">
+        <v>279</v>
+      </c>
+      <c r="G54" t="s">
+        <v>499</v>
+      </c>
+      <c r="H54" t="s">
+        <v>574</v>
+      </c>
+      <c r="M54">
+        <v>1</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>280</v>
+      </c>
+      <c r="C55" t="s">
+        <v>168</v>
+      </c>
+      <c r="D55" t="s">
+        <v>281</v>
+      </c>
+      <c r="E55" t="s">
+        <v>282</v>
+      </c>
+      <c r="F55" t="s">
+        <v>283</v>
+      </c>
+      <c r="G55" t="s">
+        <v>500</v>
+      </c>
+      <c r="H55" t="s">
+        <v>575</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>154</v>
+      </c>
+      <c r="B56" t="s">
+        <v>284</v>
+      </c>
+      <c r="C56" t="s">
+        <v>168</v>
+      </c>
+      <c r="D56" t="s">
+        <v>285</v>
+      </c>
+      <c r="E56" t="s">
+        <v>287</v>
+      </c>
+      <c r="F56" t="s">
+        <v>286</v>
+      </c>
+      <c r="G56" t="s">
+        <v>501</v>
+      </c>
+      <c r="H56" t="s">
+        <v>576</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>154</v>
+      </c>
+      <c r="B57" t="s">
+        <v>288</v>
+      </c>
+      <c r="C57" t="s">
+        <v>289</v>
+      </c>
+      <c r="D57" t="s">
+        <v>291</v>
+      </c>
+      <c r="E57" t="s">
+        <v>292</v>
+      </c>
+      <c r="F57" t="s">
+        <v>293</v>
+      </c>
+      <c r="G57" t="s">
+        <v>502</v>
+      </c>
+      <c r="H57" t="s">
+        <v>577</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>154</v>
+      </c>
+      <c r="B58" t="s">
+        <v>294</v>
+      </c>
+      <c r="D58" t="s">
+        <v>295</v>
+      </c>
+      <c r="E58" t="s">
+        <v>296</v>
+      </c>
+      <c r="G58" t="s">
+        <v>503</v>
+      </c>
+      <c r="H58" t="s">
+        <v>578</v>
+      </c>
+      <c r="M58">
+        <v>1</v>
+      </c>
+      <c r="R58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>297</v>
+      </c>
+      <c r="C59" t="s">
+        <v>298</v>
+      </c>
+      <c r="D59" t="s">
+        <v>299</v>
+      </c>
+      <c r="E59" t="s">
+        <v>300</v>
+      </c>
+      <c r="F59" t="s">
+        <v>301</v>
+      </c>
+      <c r="G59" t="s">
+        <v>504</v>
+      </c>
+      <c r="H59" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>154</v>
+      </c>
+      <c r="B60" t="s">
+        <v>302</v>
+      </c>
+      <c r="C60" t="s">
+        <v>168</v>
+      </c>
+      <c r="D60" t="s">
+        <v>303</v>
+      </c>
+      <c r="E60" t="s">
+        <v>304</v>
+      </c>
+      <c r="F60" t="s">
+        <v>305</v>
+      </c>
+      <c r="G60" t="s">
+        <v>505</v>
+      </c>
+      <c r="H60" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" t="s">
+        <v>306</v>
+      </c>
+      <c r="D61" t="s">
+        <v>307</v>
+      </c>
+      <c r="E61" t="s">
+        <v>308</v>
+      </c>
+      <c r="G61" t="s">
+        <v>506</v>
+      </c>
+      <c r="H61" t="s">
+        <v>581</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>154</v>
+      </c>
+      <c r="B62" t="s">
+        <v>309</v>
+      </c>
+      <c r="D62" t="s">
+        <v>310</v>
+      </c>
+      <c r="E62" t="s">
+        <v>311</v>
+      </c>
+      <c r="G62" t="s">
+        <v>507</v>
+      </c>
+      <c r="H62" t="s">
+        <v>582</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>312</v>
+      </c>
+      <c r="C63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" t="s">
+        <v>471</v>
+      </c>
+      <c r="E63" t="s">
+        <v>313</v>
+      </c>
+      <c r="F63" t="s">
+        <v>314</v>
+      </c>
+      <c r="G63" t="s">
+        <v>508</v>
+      </c>
+      <c r="H63" t="s">
+        <v>583</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
+        <v>315</v>
+      </c>
+      <c r="C64" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" t="s">
+        <v>316</v>
+      </c>
+      <c r="E64" t="s">
+        <v>317</v>
+      </c>
+      <c r="F64" t="s">
+        <v>318</v>
+      </c>
+      <c r="G64" t="s">
+        <v>509</v>
+      </c>
+      <c r="H64" t="s">
+        <v>584</v>
+      </c>
+      <c r="M64">
+        <v>1</v>
+      </c>
+      <c r="N64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" t="s">
+        <v>319</v>
+      </c>
+      <c r="C65" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" t="s">
+        <v>320</v>
+      </c>
+      <c r="E65" t="s">
+        <v>321</v>
+      </c>
+      <c r="F65" t="s">
+        <v>322</v>
+      </c>
+      <c r="G65" t="s">
+        <v>510</v>
+      </c>
+      <c r="H65" t="s">
+        <v>585</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" t="s">
+        <v>323</v>
+      </c>
+      <c r="C66" t="s">
+        <v>205</v>
+      </c>
+      <c r="D66" t="s">
+        <v>324</v>
+      </c>
+      <c r="E66" t="s">
+        <v>325</v>
+      </c>
+      <c r="F66" t="s">
+        <v>326</v>
+      </c>
+      <c r="G66" t="s">
+        <v>511</v>
+      </c>
+      <c r="H66" t="s">
+        <v>586</v>
+      </c>
+      <c r="M66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" t="s">
+        <v>327</v>
+      </c>
+      <c r="C67" t="s">
+        <v>185</v>
+      </c>
+      <c r="D67" t="s">
+        <v>472</v>
+      </c>
+      <c r="E67" t="s">
+        <v>328</v>
+      </c>
+      <c r="F67" t="s">
+        <v>329</v>
+      </c>
+      <c r="G67" t="s">
+        <v>512</v>
+      </c>
+      <c r="H67" t="s">
+        <v>587</v>
+      </c>
+      <c r="M67">
+        <v>1</v>
+      </c>
+      <c r="S67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>154</v>
+      </c>
+      <c r="B68" t="s">
+        <v>330</v>
+      </c>
+      <c r="C68" t="s">
+        <v>185</v>
+      </c>
+      <c r="D68" t="s">
+        <v>331</v>
+      </c>
+      <c r="E68" t="s">
+        <v>332</v>
+      </c>
+      <c r="F68" t="s">
+        <v>333</v>
+      </c>
+      <c r="G68" t="s">
+        <v>513</v>
+      </c>
+      <c r="H68" t="s">
+        <v>588</v>
+      </c>
+      <c r="N68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>154</v>
+      </c>
+      <c r="B69" t="s">
+        <v>334</v>
+      </c>
+      <c r="C69" t="s">
+        <v>360</v>
+      </c>
+      <c r="D69" t="s">
+        <v>335</v>
+      </c>
+      <c r="E69" t="s">
+        <v>336</v>
+      </c>
+      <c r="F69" t="s">
+        <v>337</v>
+      </c>
+      <c r="G69" t="s">
+        <v>514</v>
+      </c>
+      <c r="H69" t="s">
+        <v>589</v>
+      </c>
+      <c r="L69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" t="s">
+        <v>338</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" t="s">
+        <v>339</v>
+      </c>
+      <c r="E70" t="s">
+        <v>341</v>
+      </c>
+      <c r="F70" t="s">
+        <v>340</v>
+      </c>
+      <c r="G70" t="s">
+        <v>515</v>
+      </c>
+      <c r="H70" t="s">
+        <v>590</v>
+      </c>
+      <c r="M70">
+        <v>1</v>
+      </c>
+      <c r="P70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" t="s">
+        <v>342</v>
+      </c>
+      <c r="C71" t="s">
+        <v>343</v>
+      </c>
+      <c r="D71" t="s">
+        <v>344</v>
+      </c>
+      <c r="E71" t="s">
+        <v>345</v>
+      </c>
+      <c r="F71" t="s">
+        <v>346</v>
+      </c>
+      <c r="G71" t="s">
+        <v>516</v>
+      </c>
+      <c r="H71" t="s">
+        <v>591</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>154</v>
+      </c>
+      <c r="B72" t="s">
+        <v>347</v>
+      </c>
+      <c r="C72" t="s">
+        <v>209</v>
+      </c>
+      <c r="D72" t="s">
+        <v>348</v>
+      </c>
+      <c r="E72" t="s">
+        <v>349</v>
+      </c>
+      <c r="F72" t="s">
+        <v>350</v>
+      </c>
+      <c r="G72" t="s">
+        <v>517</v>
+      </c>
+      <c r="H72" t="s">
+        <v>592</v>
+      </c>
+      <c r="I72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>154</v>
+      </c>
+      <c r="B73" t="s">
+        <v>351</v>
+      </c>
+      <c r="C73" t="s">
+        <v>352</v>
+      </c>
+      <c r="D73" t="s">
+        <v>353</v>
+      </c>
+      <c r="E73" t="s">
+        <v>354</v>
+      </c>
+      <c r="F73" t="s">
+        <v>355</v>
+      </c>
+      <c r="G73" t="s">
+        <v>518</v>
+      </c>
+      <c r="H73" t="s">
+        <v>593</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>154</v>
+      </c>
+      <c r="B74" t="s">
+        <v>356</v>
+      </c>
+      <c r="C74" t="s">
+        <v>360</v>
+      </c>
+      <c r="D74" t="s">
+        <v>361</v>
+      </c>
+      <c r="E74" t="s">
+        <v>362</v>
+      </c>
+      <c r="F74" t="s">
+        <v>363</v>
+      </c>
+      <c r="G74" t="s">
+        <v>519</v>
+      </c>
+      <c r="H74" t="s">
+        <v>594</v>
+      </c>
+      <c r="O74">
+        <v>1</v>
+      </c>
+      <c r="R74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>154</v>
+      </c>
+      <c r="B75" t="s">
+        <v>365</v>
+      </c>
+      <c r="D75" t="s">
+        <v>473</v>
+      </c>
+      <c r="E75" t="s">
+        <v>364</v>
+      </c>
+      <c r="F75" t="s">
+        <v>366</v>
+      </c>
+      <c r="G75" t="s">
+        <v>520</v>
+      </c>
+      <c r="H75" t="s">
+        <v>595</v>
+      </c>
+      <c r="O75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>154</v>
+      </c>
+      <c r="B76" t="s">
+        <v>367</v>
+      </c>
+      <c r="C76" t="s">
+        <v>185</v>
+      </c>
+      <c r="D76" t="s">
+        <v>368</v>
+      </c>
+      <c r="E76" t="s">
+        <v>369</v>
+      </c>
+      <c r="G76" t="s">
+        <v>521</v>
+      </c>
+      <c r="H76" t="s">
+        <v>596</v>
+      </c>
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>370</v>
+      </c>
+      <c r="C77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D77" t="s">
+        <v>371</v>
+      </c>
+      <c r="E77" t="s">
+        <v>372</v>
+      </c>
+      <c r="F77" t="s">
+        <v>373</v>
+      </c>
+      <c r="G77" t="s">
+        <v>522</v>
+      </c>
+      <c r="H77" t="s">
+        <v>597</v>
+      </c>
+      <c r="O77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" t="s">
+        <v>374</v>
+      </c>
+      <c r="C78" t="s">
+        <v>191</v>
+      </c>
+      <c r="D78" t="s">
+        <v>375</v>
+      </c>
+      <c r="E78" t="s">
+        <v>376</v>
+      </c>
+      <c r="G78" t="s">
+        <v>523</v>
+      </c>
+      <c r="H78" t="s">
+        <v>598</v>
+      </c>
+      <c r="M78">
+        <v>1</v>
+      </c>
+      <c r="O78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>154</v>
+      </c>
+      <c r="B79" t="s">
+        <v>377</v>
+      </c>
+      <c r="C79" t="s">
+        <v>191</v>
+      </c>
+      <c r="D79" t="s">
+        <v>378</v>
+      </c>
+      <c r="E79" t="s">
+        <v>379</v>
+      </c>
+      <c r="F79" t="s">
+        <v>380</v>
+      </c>
+      <c r="G79" t="s">
+        <v>524</v>
+      </c>
+      <c r="H79" t="s">
+        <v>599</v>
+      </c>
+      <c r="O79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" t="s">
+        <v>381</v>
+      </c>
+      <c r="C80" t="s">
+        <v>185</v>
+      </c>
+      <c r="D80" t="s">
+        <v>382</v>
+      </c>
+      <c r="E80" t="s">
+        <v>383</v>
+      </c>
+      <c r="F80" t="s">
+        <v>384</v>
+      </c>
+      <c r="G80" t="s">
+        <v>525</v>
+      </c>
+      <c r="H80" t="s">
+        <v>600</v>
+      </c>
+      <c r="O80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>154</v>
+      </c>
+      <c r="B81" t="s">
+        <v>385</v>
+      </c>
+      <c r="C81" t="s">
+        <v>185</v>
+      </c>
+      <c r="D81" t="s">
+        <v>386</v>
+      </c>
+      <c r="E81" t="s">
+        <v>387</v>
+      </c>
+      <c r="F81" t="s">
+        <v>388</v>
+      </c>
+      <c r="G81" t="s">
+        <v>526</v>
+      </c>
+      <c r="H81" t="s">
+        <v>601</v>
+      </c>
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>154</v>
+      </c>
+      <c r="B82" t="s">
+        <v>389</v>
+      </c>
+      <c r="C82" t="s">
+        <v>168</v>
+      </c>
+      <c r="D82" t="s">
+        <v>390</v>
+      </c>
+      <c r="E82" t="s">
+        <v>391</v>
+      </c>
+      <c r="G82" t="s">
+        <v>527</v>
+      </c>
+      <c r="H82" t="s">
+        <v>602</v>
+      </c>
+      <c r="I82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>154</v>
+      </c>
+      <c r="B83" t="s">
+        <v>392</v>
+      </c>
+      <c r="C83" t="s">
+        <v>289</v>
+      </c>
+      <c r="D83" t="s">
+        <v>393</v>
+      </c>
+      <c r="E83" t="s">
+        <v>394</v>
+      </c>
+      <c r="F83" t="s">
+        <v>395</v>
+      </c>
+      <c r="G83" t="s">
+        <v>528</v>
+      </c>
+      <c r="H83" t="s">
+        <v>603</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>397</v>
+      </c>
+      <c r="C84" t="s">
+        <v>398</v>
+      </c>
+      <c r="D84" t="s">
+        <v>399</v>
+      </c>
+      <c r="E84" t="s">
+        <v>396</v>
+      </c>
+      <c r="G84" t="s">
+        <v>529</v>
+      </c>
+      <c r="H84" t="s">
+        <v>604</v>
+      </c>
+      <c r="I84">
+        <v>1</v>
+      </c>
+      <c r="J84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>154</v>
+      </c>
+      <c r="B85" t="s">
+        <v>400</v>
+      </c>
+      <c r="D85" t="s">
+        <v>401</v>
+      </c>
+      <c r="E85" t="s">
+        <v>403</v>
+      </c>
+      <c r="F85" t="s">
+        <v>402</v>
+      </c>
+      <c r="G85" t="s">
+        <v>530</v>
+      </c>
+      <c r="H85" t="s">
+        <v>605</v>
+      </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+      <c r="T85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" t="s">
+        <v>404</v>
+      </c>
+      <c r="C86" t="s">
+        <v>289</v>
+      </c>
+      <c r="D86" t="s">
+        <v>405</v>
+      </c>
+      <c r="E86" t="s">
+        <v>406</v>
+      </c>
+      <c r="F86" t="s">
+        <v>407</v>
+      </c>
+      <c r="G86" t="s">
+        <v>531</v>
+      </c>
+      <c r="H86" t="s">
+        <v>606</v>
+      </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>154</v>
+      </c>
+      <c r="B87" t="s">
+        <v>408</v>
+      </c>
+      <c r="D87" t="s">
+        <v>409</v>
+      </c>
+      <c r="E87" t="s">
+        <v>410</v>
+      </c>
+      <c r="F87" t="s">
+        <v>410</v>
+      </c>
+      <c r="G87" t="s">
+        <v>532</v>
+      </c>
+      <c r="H87" t="s">
+        <v>607</v>
+      </c>
+      <c r="J87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" t="s">
+        <v>411</v>
+      </c>
+      <c r="C88" t="s">
+        <v>289</v>
+      </c>
+      <c r="D88" t="s">
+        <v>412</v>
+      </c>
+      <c r="E88" t="s">
+        <v>413</v>
+      </c>
+      <c r="G88" t="s">
+        <v>533</v>
+      </c>
+      <c r="H88" t="s">
+        <v>608</v>
+      </c>
+      <c r="L88">
+        <v>1</v>
+      </c>
+      <c r="R88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>154</v>
+      </c>
+      <c r="B89" t="s">
+        <v>414</v>
+      </c>
+      <c r="C89" t="s">
+        <v>289</v>
+      </c>
+      <c r="D89" t="s">
+        <v>415</v>
+      </c>
+      <c r="E89" t="s">
+        <v>416</v>
+      </c>
+      <c r="F89" t="s">
+        <v>417</v>
+      </c>
+      <c r="G89" t="s">
+        <v>534</v>
+      </c>
+      <c r="H89" t="s">
+        <v>609</v>
+      </c>
+      <c r="L89">
+        <v>1</v>
+      </c>
+      <c r="O89">
+        <v>1</v>
+      </c>
+      <c r="T89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>154</v>
+      </c>
+      <c r="B90" t="s">
+        <v>418</v>
+      </c>
+      <c r="C90" t="s">
+        <v>343</v>
+      </c>
+      <c r="D90" t="s">
+        <v>419</v>
+      </c>
+      <c r="E90" t="s">
+        <v>624</v>
+      </c>
+      <c r="G90" t="s">
+        <v>535</v>
+      </c>
+      <c r="H90" t="s">
+        <v>610</v>
+      </c>
+      <c r="J90">
+        <v>1</v>
+      </c>
+      <c r="P90">
+        <v>1</v>
+      </c>
+      <c r="S90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91" t="s">
+        <v>420</v>
+      </c>
+      <c r="C91" t="s">
+        <v>185</v>
+      </c>
+      <c r="D91" t="s">
+        <v>421</v>
+      </c>
+      <c r="E91" t="s">
+        <v>422</v>
+      </c>
+      <c r="F91" t="s">
+        <v>423</v>
+      </c>
+      <c r="G91" t="s">
+        <v>536</v>
+      </c>
+      <c r="H91" t="s">
+        <v>611</v>
+      </c>
+      <c r="J91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>154</v>
+      </c>
+      <c r="B92" t="s">
+        <v>427</v>
+      </c>
+      <c r="C92" t="s">
+        <v>191</v>
+      </c>
+      <c r="D92" t="s">
+        <v>426</v>
+      </c>
+      <c r="E92" t="s">
+        <v>424</v>
+      </c>
+      <c r="F92" t="s">
+        <v>425</v>
+      </c>
+      <c r="G92" t="s">
+        <v>537</v>
+      </c>
+      <c r="H92" t="s">
+        <v>612</v>
+      </c>
+      <c r="S92">
+        <v>1</v>
+      </c>
+      <c r="T92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>154</v>
+      </c>
+      <c r="B93" t="s">
+        <v>428</v>
+      </c>
+      <c r="C93" t="s">
+        <v>185</v>
+      </c>
+      <c r="D93" t="s">
+        <v>429</v>
+      </c>
+      <c r="E93" t="s">
+        <v>430</v>
+      </c>
+      <c r="F93" t="s">
+        <v>431</v>
+      </c>
+      <c r="G93" t="s">
+        <v>538</v>
+      </c>
+      <c r="H93" t="s">
+        <v>613</v>
+      </c>
+      <c r="J93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>154</v>
+      </c>
+      <c r="B94" t="s">
+        <v>432</v>
+      </c>
+      <c r="C94" t="s">
+        <v>196</v>
+      </c>
+      <c r="D94" t="s">
+        <v>433</v>
+      </c>
+      <c r="E94" t="s">
+        <v>434</v>
+      </c>
+      <c r="F94" t="s">
+        <v>435</v>
+      </c>
+      <c r="G94" t="s">
+        <v>539</v>
+      </c>
+      <c r="H94" t="s">
+        <v>614</v>
+      </c>
+      <c r="J94">
+        <v>1</v>
+      </c>
+      <c r="Q94">
+        <v>1</v>
+      </c>
+      <c r="R94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>154</v>
+      </c>
+      <c r="B95" t="s">
+        <v>436</v>
+      </c>
+      <c r="C95" t="s">
+        <v>437</v>
+      </c>
+      <c r="D95" t="s">
+        <v>438</v>
+      </c>
+      <c r="E95" t="s">
+        <v>439</v>
+      </c>
+      <c r="G95" t="s">
+        <v>540</v>
+      </c>
+      <c r="H95" t="s">
+        <v>615</v>
+      </c>
+      <c r="I95">
+        <v>1</v>
+      </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>154</v>
+      </c>
+      <c r="B96" t="s">
+        <v>440</v>
+      </c>
+      <c r="C96" t="s">
+        <v>441</v>
+      </c>
+      <c r="D96" t="s">
+        <v>442</v>
+      </c>
+      <c r="E96" t="s">
+        <v>443</v>
+      </c>
+      <c r="F96" t="s">
+        <v>444</v>
+      </c>
+      <c r="G96" t="s">
+        <v>541</v>
+      </c>
+      <c r="H96" t="s">
+        <v>616</v>
+      </c>
+      <c r="P96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>154</v>
+      </c>
+      <c r="B97" t="s">
+        <v>445</v>
+      </c>
+      <c r="C97" t="s">
+        <v>191</v>
+      </c>
+      <c r="D97" t="s">
+        <v>446</v>
+      </c>
+      <c r="E97" t="s">
+        <v>447</v>
+      </c>
+      <c r="F97" t="s">
+        <v>448</v>
+      </c>
+      <c r="G97" t="s">
+        <v>542</v>
+      </c>
+      <c r="H97" t="s">
+        <v>617</v>
+      </c>
+      <c r="K97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>154</v>
+      </c>
+      <c r="B98" t="s">
+        <v>450</v>
+      </c>
+      <c r="C98" t="s">
+        <v>191</v>
+      </c>
+      <c r="D98" t="s">
+        <v>451</v>
+      </c>
+      <c r="E98" t="s">
+        <v>449</v>
+      </c>
+      <c r="F98" t="s">
+        <v>452</v>
+      </c>
+      <c r="G98" t="s">
+        <v>543</v>
+      </c>
+      <c r="H98" t="s">
+        <v>618</v>
+      </c>
+      <c r="N98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>154</v>
+      </c>
+      <c r="B99" t="s">
+        <v>453</v>
+      </c>
+      <c r="C99" t="s">
+        <v>360</v>
+      </c>
+      <c r="D99" t="s">
+        <v>454</v>
+      </c>
+      <c r="E99" t="s">
+        <v>455</v>
+      </c>
+      <c r="F99" t="s">
+        <v>456</v>
+      </c>
+      <c r="G99" t="s">
+        <v>544</v>
+      </c>
+      <c r="H99" t="s">
+        <v>619</v>
+      </c>
+      <c r="N99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>154</v>
+      </c>
+      <c r="B100" t="s">
+        <v>457</v>
+      </c>
+      <c r="C100" t="s">
+        <v>360</v>
+      </c>
+      <c r="D100" t="s">
+        <v>458</v>
+      </c>
+      <c r="E100" t="s">
+        <v>459</v>
+      </c>
+      <c r="G100" t="s">
+        <v>545</v>
+      </c>
+      <c r="H100" t="s">
+        <v>620</v>
+      </c>
+      <c r="N100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101" t="s">
+        <v>460</v>
+      </c>
+      <c r="C101" t="s">
+        <v>191</v>
+      </c>
+      <c r="D101" t="s">
+        <v>461</v>
+      </c>
+      <c r="E101" t="s">
+        <v>462</v>
+      </c>
+      <c r="F101" t="s">
+        <v>463</v>
+      </c>
+      <c r="G101" t="s">
+        <v>546</v>
+      </c>
+      <c r="H101" t="s">
+        <v>621</v>
+      </c>
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>154</v>
+      </c>
+      <c r="B102" t="s">
+        <v>464</v>
+      </c>
+      <c r="C102" t="s">
+        <v>465</v>
+      </c>
+      <c r="D102" t="s">
+        <v>466</v>
+      </c>
+      <c r="E102" t="s">
+        <v>467</v>
+      </c>
+      <c r="G102" t="s">
+        <v>547</v>
+      </c>
+      <c r="H102" t="s">
+        <v>622</v>
+      </c>
+      <c r="L102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>154</v>
+      </c>
+      <c r="B103" t="s">
+        <v>468</v>
+      </c>
+      <c r="D103" t="s">
+        <v>469</v>
+      </c>
+      <c r="E103" t="s">
+        <v>470</v>
+      </c>
+      <c r="G103" t="s">
+        <v>548</v>
+      </c>
+      <c r="H103" t="s">
+        <v>623</v>
+      </c>
+      <c r="L103">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B26" r:id="rId1" display="https://www.matthewtancik.com/nerf" xr:uid="{35967FB2-814A-154F-8541-7714319F096C}"/>
+    <hyperlink ref="B27" r:id="rId2" display="https://lingjie0206.github.io/papers/NSVF/" xr:uid="{F2DD4E80-7653-6B46-BE0A-8E826172F88C}"/>
+    <hyperlink ref="B28" r:id="rId3" display="http://www.computationalimaging.org/publications/automatic-integration/" xr:uid="{A28EC183-687F-8A46-9CA4-4A7708A6C750}"/>
+    <hyperlink ref="B29" r:id="rId4" display="https://arxiv.org/abs/2011.12490" xr:uid="{C5B06987-5C0D-E443-82C4-02F6431045D1}"/>
+    <hyperlink ref="B30" r:id="rId5" display="https://depthoraclenerf.github.io/" xr:uid="{3CEB0E14-63E6-574A-9FC6-2051AD0460B0}"/>
+    <hyperlink ref="B31" r:id="rId6" display="https://arxiv.org/abs/2103.10380" xr:uid="{EA18432D-CDAD-5D46-AB83-9539228413CB}"/>
+    <hyperlink ref="B32" r:id="rId7" display="https://arxiv.org/abs/2103.13744" xr:uid="{429A6E53-E8CB-BC4C-9538-A2470024449F}"/>
+    <hyperlink ref="B33" r:id="rId8" display="https://alexyu.net/plenoctrees/" xr:uid="{7DC25326-9D8E-8D47-A044-DD17F9ED0CD0}"/>
+    <hyperlink ref="B34" r:id="rId9" display="https://arxiv.org/abs/2103.01954" xr:uid="{A2FF4FE9-43D0-5F44-93A7-55BE57938D31}"/>
+    <hyperlink ref="B35" r:id="rId10" display="https://vsitzmann.github.io/lfns/" xr:uid="{F6597C48-9252-3349-B84C-D97A31F62416}"/>
+    <hyperlink ref="B36" r:id="rId11" display="https://arxiv.org/pdf/2107.02791.pdf" xr:uid="{4E32310C-E8E8-1445-9B6E-B1A0C6585A89}"/>
+    <hyperlink ref="B38" r:id="rId12" display="https://nerf-w.github.io/" xr:uid="{1C3AF7E4-0ED6-6341-ACDB-04910971A9DA}"/>
+    <hyperlink ref="B43" r:id="rId13" display="https://gvv.mpi-inf.mpg.de/projects/nonrigid_nerf/" xr:uid="{2DDCA2B8-C06B-604A-A893-ED7E083125F7}"/>
+    <hyperlink ref="B44" r:id="rId14" display="https://volumetric-avatars.github.io/" xr:uid="{B38221A4-28D3-EC48-BD13-F22F93351407}"/>
+    <hyperlink ref="B46" r:id="rId15" display="https://arxiv.org/abs/2202.00181" xr:uid="{A924BD42-5B3F-3740-81C0-0C81F8B5122D}"/>
+    <hyperlink ref="B47" r:id="rId16" display="https://zju3dv.github.io/animatable_nerf/" xr:uid="{79B54E94-A634-C04E-BBD6-E0740CB05D22}"/>
+    <hyperlink ref="B48" r:id="rId17" display="https://vcai.mpi-inf.mpg.de/projects/NeuralActor/" xr:uid="{8B2119CC-BEBB-1141-9295-5A03BB8F0926}"/>
+    <hyperlink ref="B50" r:id="rId18" display="https://zju3dv.github.io/neuralbody/" xr:uid="{B4F98C3C-2C12-3647-8B14-C77A228D92A6}"/>
+    <hyperlink ref="D51" r:id="rId19" display="https://neural-3d-video.github.io/" xr:uid="{F5C4215C-421A-2E4F-9166-06F8B5156E7B}"/>
+    <hyperlink ref="B55" r:id="rId20" display="https://arxiv.org/abs/2012.02190" xr:uid="{53D1B557-9DD9-0941-A181-C2437740945C}"/>
+    <hyperlink ref="D55" r:id="rId21" display="https://alexyu.net/pixelnerf" xr:uid="{FE08CB9D-CA82-2641-899B-1CED2638D0C9}"/>
+    <hyperlink ref="B56" r:id="rId22" display="https://arxiv.org/abs/2012.02189" xr:uid="{A3166556-FD50-524F-9D7B-7DFABC9BA22F}"/>
+    <hyperlink ref="B59" r:id="rId23" display="https://arxiv.org/pdf/2102.08860.pdf" xr:uid="{C98AD7DA-8A21-4B40-A0E6-ABB79200584D}"/>
+    <hyperlink ref="B60" r:id="rId24" display="https://ibrnet.github.io/static/paper.pdf" xr:uid="{B64854DE-6A9F-EE41-8605-5F214EE9ADE2}"/>
+    <hyperlink ref="D60" r:id="rId25" display="https://ibrnet.github.io/" xr:uid="{5B6CC4DE-F7F9-2647-9B5C-A1E194127C73}"/>
+    <hyperlink ref="B61" r:id="rId26" display="https://arxiv.org/pdf/2103.17269.pdf" xr:uid="{62D8EC5C-C4AC-DA46-9FDF-0E23E2D5C874}"/>
+    <hyperlink ref="B62" r:id="rId27" display="https://arxiv.org/pdf/2104.00587.pdf" xr:uid="{B37AC469-58DD-BF4C-8A04-F712B1A8EB94}"/>
+    <hyperlink ref="B63" r:id="rId28" display="https://apple.github.io/ml-gsn/" xr:uid="{7717E2BE-FF3E-EF48-92FF-8653D9AB6AAE}"/>
+    <hyperlink ref="B64" r:id="rId29" display="https://apchenstu.github.io/mvsnerf/" xr:uid="{D01EC804-00BD-B442-AED3-391DEE153AF0}"/>
+    <hyperlink ref="B65" r:id="rId30" display="https://virtualhumans.mpi-inf.mpg.de/srf/" xr:uid="{BBFCEAB6-1067-4A46-B94B-1149F1DB3378}"/>
+    <hyperlink ref="D65" r:id="rId31" display="https://virtualhumans.mpi-inf.mpg.de/srf/" xr:uid="{99CFE0A6-49E8-6C47-AD0F-4876EDDD5257}"/>
+    <hyperlink ref="B66" r:id="rId32" display="https://liuyuan-pal.github.io/NeuRay/" xr:uid="{B8E198D5-170F-6445-ABD6-FC745FE3BB4F}"/>
+    <hyperlink ref="D68" r:id="rId33" display="https://github.com/vincentfung13/MINE" xr:uid="{BC5BAD36-364E-6749-BCB4-A976C125DDC5}"/>
+    <hyperlink ref="B70" r:id="rId34" display="https://sites.google.com/view/wbjang/home/codenerf" xr:uid="{187E0164-3464-5F42-AACD-3D5C2BF3C820}"/>
+    <hyperlink ref="B72" r:id="rId35" display="https://bmild.github.io/rawnerf/" xr:uid="{A6B8E96F-1F53-7041-B6A4-60B9508480D4}"/>
+    <hyperlink ref="B73" r:id="rId36" display="http://yenchenlin.me/inerf/" xr:uid="{EE610F53-3CF1-1E40-8ACB-F1984A3C3C5D}"/>
+    <hyperlink ref="B74" r:id="rId37" display="https://lemonatsu.github.io/ANeRF-Surface-free-Pose-Refinement/" xr:uid="{8812967F-CC98-5B4A-995D-AC01039F534F}"/>
+    <hyperlink ref="D74" r:id="rId38" display="https://lemonatsu.github.io/anerf/" xr:uid="{9D7EFC10-490A-E447-9D5C-8E801A904206}"/>
+    <hyperlink ref="B79" r:id="rId39" display="https://chenhsuanlin.bitbucket.io/bundle-adjusting-NeRF/" xr:uid="{20F5B6EF-8807-F341-AF88-60ED41CC6280}"/>
+    <hyperlink ref="B80" r:id="rId40" display="https://postech-cvlab.github.io/SCNeRF/" xr:uid="{2F6B0D04-F664-0240-95C8-8B039E05A6FE}"/>
+    <hyperlink ref="B81" r:id="rId41" display="https://markboss.me/publication/2021-nerd/" xr:uid="{D07E6E46-FE31-B345-8F53-0E980351DB40}"/>
+    <hyperlink ref="B82" r:id="rId42" display="https://people.eecs.berkeley.edu/~pratul/nerv/" xr:uid="{8DA1DFFB-66B7-D945-A567-262763835FE0}"/>
+    <hyperlink ref="B85" r:id="rId43" display="https://arxiv.org/abs/2010.07492" xr:uid="{24173C9F-D45A-1744-981B-21CA290E8730}"/>
+    <hyperlink ref="D85" r:id="rId44" display="https://github.com/Kai-46/nerfplusplus" xr:uid="{AC3D8F12-8792-6341-9EDD-3119722F4FB3}"/>
+    <hyperlink ref="B86" r:id="rId45" display="https://arxiv.org/abs/2011.12100" xr:uid="{A6421490-778F-404C-9B50-F4DF3C3222E3}"/>
+    <hyperlink ref="B88" r:id="rId46" display="https://ziyanw1.github.io/hybrid_nerf/" xr:uid="{21255C5F-2079-BD42-A4E8-1473A711251E}"/>
+    <hyperlink ref="B95" r:id="rId47" display="https://fig-nerf.github.io/" xr:uid="{BCB08482-216E-F445-961F-79B17BAB2894}"/>
+    <hyperlink ref="B96" r:id="rId48" display="https://developer.nvidia.com/blog/nvidia-research-nerf-tex-neural-reflectance-field-textures/" xr:uid="{46F7C388-1CC4-9149-B59B-559EE7BCD36A}"/>
+    <hyperlink ref="B97" r:id="rId49" display="https://jonbarron.info/mipnerf/" xr:uid="{3CF7024E-5382-C942-836E-26A20DA4524C}"/>
+    <hyperlink ref="B99" r:id="rId50" display="https://arxiv.org/abs/2106.10689" xr:uid="{E7185A93-C91C-F24C-9829-6325E236C3EB}"/>
+    <hyperlink ref="B101" r:id="rId51" display="https://weiyithu.github.io/NerfingMVS/" xr:uid="{22220255-E2B3-4341-A8DE-DF8098C5B6B6}"/>
+    <hyperlink ref="B102" r:id="rId52" display="https://3d-representation-learning.github.io/nerf-dy/" xr:uid="{433A7789-7958-4642-A629-FBF537BFB55E}"/>
+    <hyperlink ref="D103" r:id="rId53" display="https://mikh3x4.github.io/nerf-navigation/" xr:uid="{8A666769-9523-DC43-A0CD-D271CCCC1BDC}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add waymo datasets on Mega, subject to change
</commit_message>
<xml_diff>
--- a/docs/weekly_nerf_meta_data.xlsx
+++ b/docs/weekly_nerf_meta_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zelinzhao/cache/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02467484-6133-BF41-B3EC-F6DEBE1007CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A38D8D-ED4E-4A46-9192-3EF3DE0EA80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="697">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="697">
   <si>
     <t>week</t>
   </si>
@@ -2974,7 +2974,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3528,9 +3528,6 @@
         <v>60</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
-      </c>
-      <c r="F20" t="s">
         <v>82</v>
       </c>
       <c r="G20" t="s">

</xml_diff>